<commit_message>
updated database based on 15-05-2020 data.
</commit_message>
<xml_diff>
--- a/Data/Covid2019/SA_data_archive/Province_database.xlsx
+++ b/Data/Covid2019/SA_data_archive/Province_database.xlsx
@@ -19,7 +19,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId15" roundtripDataSignature="AMtx7mh9xC5AUNtJ4TszMV5813pGcMEBSw=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId15" roundtripDataSignature="AMtx7mgMQ9WBQrIeC1ERsXOX7KtGc8ogSQ=="/>
     </ext>
   </extLst>
 </workbook>
@@ -200,12 +200,6 @@
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="15" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="15" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -222,6 +216,12 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="15" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="15" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -230,8 +230,8 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="10" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="10" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -519,11 +519,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="590528791"/>
-        <c:axId val="1499365975"/>
+        <c:axId val="1555755518"/>
+        <c:axId val="868457795"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="590528791"/>
+        <c:axId val="1555755518"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -568,10 +568,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1499365975"/>
+        <c:crossAx val="868457795"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1499365975"/>
+        <c:axId val="868457795"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -640,7 +640,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="590528791"/>
+        <c:crossAx val="1555755518"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -938,11 +938,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1938610896"/>
-        <c:axId val="979451361"/>
+        <c:axId val="988706281"/>
+        <c:axId val="1707678396"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1938610896"/>
+        <c:axId val="988706281"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -987,10 +987,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="979451361"/>
+        <c:crossAx val="1707678396"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="979451361"/>
+        <c:axId val="1707678396"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1059,7 +1059,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1938610896"/>
+        <c:crossAx val="988706281"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1140,8 +1140,8 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1405426215"/>
-        <c:axId val="1729819922"/>
+        <c:axId val="1953621288"/>
+        <c:axId val="464364076"/>
       </c:barChart>
       <c:lineChart>
         <c:ser>
@@ -1351,11 +1351,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1405426215"/>
-        <c:axId val="1729819922"/>
+        <c:axId val="1953621288"/>
+        <c:axId val="464364076"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1405426215"/>
+        <c:axId val="1953621288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1400,10 +1400,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1729819922"/>
+        <c:crossAx val="464364076"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1729819922"/>
+        <c:axId val="464364076"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1472,7 +1472,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1405426215"/>
+        <c:crossAx val="1953621288"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1553,8 +1553,8 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="343157074"/>
-        <c:axId val="263481665"/>
+        <c:axId val="835956443"/>
+        <c:axId val="63390345"/>
       </c:barChart>
       <c:lineChart>
         <c:ser>
@@ -1764,11 +1764,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="343157074"/>
-        <c:axId val="263481665"/>
+        <c:axId val="835956443"/>
+        <c:axId val="63390345"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="343157074"/>
+        <c:axId val="835956443"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1813,10 +1813,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="263481665"/>
+        <c:crossAx val="63390345"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="263481665"/>
+        <c:axId val="63390345"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1885,7 +1885,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343157074"/>
+        <c:crossAx val="835956443"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2146,11 +2146,11 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="1843274161"/>
-        <c:axId val="845933694"/>
+        <c:axId val="58217004"/>
+        <c:axId val="1204562180"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1843274161"/>
+        <c:axId val="58217004"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2195,10 +2195,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="845933694"/>
+        <c:crossAx val="1204562180"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="845933694"/>
+        <c:axId val="1204562180"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2267,7 +2267,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1843274161"/>
+        <c:crossAx val="58217004"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -2533,11 +2533,11 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="1657401390"/>
-        <c:axId val="1095867056"/>
+        <c:axId val="1962937958"/>
+        <c:axId val="622949600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1657401390"/>
+        <c:axId val="1962937958"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2582,10 +2582,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1095867056"/>
+        <c:crossAx val="622949600"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1095867056"/>
+        <c:axId val="622949600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2654,7 +2654,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1657401390"/>
+        <c:crossAx val="1962937958"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2735,8 +2735,8 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1353981976"/>
-        <c:axId val="1008784418"/>
+        <c:axId val="600019366"/>
+        <c:axId val="1488485850"/>
       </c:barChart>
       <c:lineChart>
         <c:ser>
@@ -2946,11 +2946,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1353981976"/>
-        <c:axId val="1008784418"/>
+        <c:axId val="600019366"/>
+        <c:axId val="1488485850"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1353981976"/>
+        <c:axId val="600019366"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2995,10 +2995,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1008784418"/>
+        <c:crossAx val="1488485850"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1008784418"/>
+        <c:axId val="1488485850"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3067,7 +3067,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1353981976"/>
+        <c:crossAx val="600019366"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3109,7 +3109,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1261421000" name="Chart 6" title="Chart"/>
+        <xdr:cNvPr id="1261421000" name="Chart 5" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3139,7 +3139,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1879382530" name="Chart 7" title="Chart"/>
+        <xdr:cNvPr id="1879382530" name="Chart 6" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3199,7 +3199,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="891414374" name="Chart 2" title="Chart"/>
+        <xdr:cNvPr id="891414374" name="Chart 1" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3237,7 +3237,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2142510870" name="Chart 3" title="Chart"/>
+        <xdr:cNvPr id="2142510870" name="Chart 2" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3267,7 +3267,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="263283604" name="Chart 4" title="Chart"/>
+        <xdr:cNvPr id="263283604" name="Chart 3" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3301,7 +3301,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1540763434" name="Chart 5" title="Chart"/>
+        <xdr:cNvPr id="1540763434" name="Chart 4" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -10040,1855 +10040,1855 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="22">
         <f>Confirmed!B3/Testing!B3</f>
         <v>0.008695652174</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="22">
         <f>Confirmed!C3/Testing!C3</f>
         <v>0.01937984496</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="22">
         <f>Confirmed!D3/Testing!D3</f>
         <v>0.02090592334</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="22">
         <f>Confirmed!E3/Testing!E3</f>
         <v>0.009677419355</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="22">
         <f>Confirmed!F3/Testing!F3</f>
         <v>0.01807228916</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="22">
         <f>Confirmed!G3/Testing!G3</f>
         <v>0.01955307263</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="22">
         <f>Confirmed!H3/Testing!H3</f>
         <v>0.0180878553</v>
       </c>
-      <c r="I4" s="21">
+      <c r="I4" s="22">
         <f>Confirmed!I3/Testing!I3</f>
         <v>0.0171990172</v>
       </c>
-      <c r="J4" s="21">
+      <c r="J4" s="22">
         <f>Confirmed!J3/Testing!J3</f>
         <v>0.01605504587</v>
       </c>
-      <c r="K4" s="21">
+      <c r="K4" s="22">
         <f>Confirmed!K3/Testing!K3</f>
         <v>0.0174291939</v>
       </c>
-      <c r="L4" s="21">
+      <c r="L4" s="22">
         <f>Confirmed!L3/Testing!L3</f>
         <v>0.0170575693</v>
       </c>
-      <c r="M4" s="21">
+      <c r="M4" s="22">
         <f>Confirmed!M3/Testing!M3</f>
         <v>0.0170575693</v>
       </c>
-      <c r="N4" s="21">
+      <c r="N4" s="22">
         <f>Confirmed!N3/Testing!N3</f>
         <v>0.02524271845</v>
       </c>
-      <c r="O4" s="21">
+      <c r="O4" s="22">
         <f>Confirmed!O3/Testing!O3</f>
         <v>0.02697841727</v>
       </c>
-      <c r="P4" s="21">
+      <c r="P4" s="22">
         <f>Confirmed!P3/Testing!P3</f>
         <v>0.02542372881</v>
       </c>
-      <c r="Q4" s="21">
+      <c r="Q4" s="22">
         <f>Confirmed!Q3/Testing!Q3</f>
         <v>0.02640264026</v>
       </c>
-      <c r="R4" s="21">
+      <c r="R4" s="22">
         <f>Confirmed!R3/Testing!R3</f>
         <v>0.02472952087</v>
       </c>
-      <c r="S4" s="21">
+      <c r="S4" s="22">
         <f>Confirmed!S3/Testing!S3</f>
         <v>0.02366863905</v>
       </c>
-      <c r="T4" s="21">
+      <c r="T4" s="22">
         <f>Confirmed!T3/Testing!T3</f>
         <v>0.02275960171</v>
       </c>
-      <c r="U4" s="21">
+      <c r="U4" s="22">
         <f>Confirmed!U3/Testing!U3</f>
         <v>0.0218878249</v>
       </c>
-      <c r="V4" s="21">
+      <c r="V4" s="22">
         <f>Confirmed!V3/Testing!V3</f>
         <v>0.02083333333</v>
       </c>
-      <c r="W4" s="21">
+      <c r="W4" s="22">
         <f>Confirmed!W3/Testing!W3</f>
         <v>0.01965601966</v>
       </c>
-      <c r="X4" s="21">
+      <c r="X4" s="22">
         <f>Confirmed!X3/Testing!X3</f>
         <v>0.01834862385</v>
       </c>
-      <c r="Y4" s="21">
+      <c r="Y4" s="22">
         <f>Confirmed!Y3/Testing!Y3</f>
         <v>0.01727861771</v>
       </c>
-      <c r="Z4" s="21">
+      <c r="Z4" s="22">
         <f>Confirmed!Z3/Testing!Z3</f>
         <v>0.01834862385</v>
       </c>
-      <c r="AA4" s="21">
+      <c r="AA4" s="22">
         <f>Confirmed!AA3/Testing!AA3</f>
         <v>0.0156097561</v>
       </c>
-      <c r="AB4" s="21">
+      <c r="AB4" s="22">
         <f>Confirmed!AB3/Testing!AB3</f>
         <v>0.01481481481</v>
       </c>
-      <c r="AC4" s="21">
+      <c r="AC4" s="22">
         <f>Confirmed!AC3/Testing!AC3</f>
         <v>0.01380500431</v>
       </c>
-      <c r="AD4" s="21">
+      <c r="AD4" s="22">
         <f>Confirmed!AD3/Testing!AD3</f>
         <v>0.01299756296</v>
       </c>
-      <c r="AE4" s="21">
+      <c r="AE4" s="22">
         <f>Confirmed!AE3/Testing!AE3</f>
         <v>0.01230769231</v>
       </c>
-      <c r="AF4" s="21">
+      <c r="AF4" s="22">
         <f>Confirmed!AF3/Testing!AF3</f>
         <v>0.01248164464</v>
       </c>
-      <c r="AG4" s="21">
+      <c r="AG4" s="22">
         <f>Confirmed!AG3/Testing!AG3</f>
         <v>0.01179736294</v>
       </c>
-      <c r="AH4" s="21">
+      <c r="AH4" s="22">
         <f>Confirmed!AH3/Testing!AH3</f>
         <v>0.01134846462</v>
       </c>
-      <c r="AI4" s="21">
+      <c r="AI4" s="22">
         <f>Confirmed!AI3/Testing!AI3</f>
         <v>0.01067839196</v>
       </c>
-      <c r="AJ4" s="21">
+      <c r="AJ4" s="22">
         <f>Confirmed!AJ3/Testing!AJ3</f>
         <v>0.01014319809</v>
       </c>
-      <c r="AK4" s="21">
+      <c r="AK4" s="22">
         <f>Confirmed!AK3/Testing!AK3</f>
         <v>0.01024473534</v>
       </c>
-      <c r="AL4" s="21">
+      <c r="AL4" s="22">
         <f>Confirmed!AL3/Testing!AL3</f>
         <v>0.01234567901</v>
       </c>
-      <c r="AM4" s="21">
+      <c r="AM4" s="22">
         <f>Confirmed!AM3/Testing!AM3</f>
         <v>0.01209677419</v>
       </c>
-      <c r="AN4" s="21">
+      <c r="AN4" s="22">
         <f>Confirmed!AN3/Testing!AN3</f>
         <v>0.01201923077</v>
       </c>
-      <c r="AO4" s="21">
+      <c r="AO4" s="22">
         <f>Confirmed!AO3/Testing!AO3</f>
         <v>0.01200923788</v>
       </c>
-      <c r="AP4" s="21">
+      <c r="AP4" s="22">
         <f>Confirmed!AP3/Testing!AP3</f>
         <v>0.0115248227</v>
       </c>
-      <c r="AQ4" s="21">
+      <c r="AQ4" s="22">
         <f>Confirmed!AQ3/Testing!AQ3</f>
         <v>0.01144552777</v>
       </c>
-      <c r="AR4" s="21">
+      <c r="AR4" s="22">
         <f>Confirmed!AR3/Testing!AR3</f>
         <v>0.01086519115</v>
       </c>
-      <c r="AS4" s="21">
+      <c r="AS4" s="22">
         <f>Confirmed!AS3/Testing!AS3</f>
         <v>0.01069927398</v>
       </c>
-      <c r="AT4" s="21">
+      <c r="AT4" s="22">
         <f>Confirmed!AT3/Testing!AT3</f>
         <v>0.01052249637</v>
       </c>
-      <c r="AU4" s="21">
+      <c r="AU4" s="22">
         <f>Confirmed!AU3/Testing!AU3</f>
         <v>0.01043478261</v>
       </c>
-      <c r="AV4" s="21">
+      <c r="AV4" s="22">
         <f>Confirmed!AV3/Testing!AV3</f>
         <v>0.01005025126</v>
       </c>
-      <c r="AW4" s="21">
+      <c r="AW4" s="22">
         <f>Confirmed!AW3/Testing!AW3</f>
         <v>0.009615384615</v>
       </c>
-      <c r="AX4" s="21">
+      <c r="AX4" s="22">
         <f>Confirmed!AX3/Testing!AX3</f>
         <v>0.009526736325</v>
       </c>
-      <c r="AY4" s="21">
+      <c r="AY4" s="22">
         <f>Confirmed!AY3/Testing!AY3</f>
         <v>0.009988249119</v>
       </c>
-      <c r="AZ4" s="21"/>
+      <c r="AZ4" s="22"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="22">
         <f>Confirmed!B4/Testing!B4</f>
         <v>0.01425178147</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="22">
         <f>Confirmed!C4/Testing!C4</f>
         <v>0.01271186441</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="22">
         <f>Confirmed!D4/Testing!D4</f>
         <v>0.01142857143</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="22">
         <f>Confirmed!E4/Testing!E4</f>
         <v>0.01410934744</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="22">
         <f>Confirmed!F4/Testing!F4</f>
         <v>0.01320132013</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="22">
         <f>Confirmed!G4/Testing!G4</f>
         <v>0.01376146789</v>
       </c>
-      <c r="H5" s="21">
+      <c r="H5" s="22">
         <f>Confirmed!H4/Testing!H4</f>
         <v>0.01271186441</v>
       </c>
-      <c r="I5" s="21">
+      <c r="I5" s="22">
         <f>Confirmed!I4/Testing!I4</f>
         <v>0.01211305518</v>
       </c>
-      <c r="J5" s="21">
+      <c r="J5" s="22">
         <f>Confirmed!J4/Testing!J4</f>
         <v>0.01381909548</v>
       </c>
-      <c r="K5" s="21">
+      <c r="K5" s="22">
         <f>Confirmed!K4/Testing!K4</f>
         <v>0.01311084625</v>
       </c>
-      <c r="L5" s="21">
+      <c r="L5" s="22">
         <f>Confirmed!L4/Testing!L4</f>
         <v>0.01283547258</v>
       </c>
-      <c r="M5" s="21">
+      <c r="M5" s="22">
         <f>Confirmed!M4/Testing!M4</f>
         <v>0.01283547258</v>
       </c>
-      <c r="N5" s="21">
+      <c r="N5" s="22">
         <f>Confirmed!N4/Testing!N4</f>
         <v>0.01594048884</v>
       </c>
-      <c r="O5" s="21">
+      <c r="O5" s="22">
         <f>Confirmed!O4/Testing!O4</f>
         <v>0.01476377953</v>
       </c>
-      <c r="P5" s="21">
+      <c r="P5" s="22">
         <f>Confirmed!P4/Testing!P4</f>
         <v>0.01669758813</v>
       </c>
-      <c r="Q5" s="21">
+      <c r="Q5" s="22">
         <f>Confirmed!Q4/Testing!Q4</f>
         <v>0.01714801444</v>
       </c>
-      <c r="R5" s="21">
+      <c r="R5" s="22">
         <f>Confirmed!R4/Testing!R4</f>
         <v>0.01607445008</v>
       </c>
-      <c r="S5" s="21">
+      <c r="S5" s="22">
         <f>Confirmed!S4/Testing!S4</f>
         <v>0.01781376518</v>
       </c>
-      <c r="T5" s="21">
+      <c r="T5" s="22">
         <f>Confirmed!T4/Testing!T4</f>
         <v>0.01713395639</v>
       </c>
-      <c r="U5" s="21">
+      <c r="U5" s="22">
         <f>Confirmed!U4/Testing!U4</f>
         <v>0.01721556886</v>
       </c>
-      <c r="V5" s="21">
+      <c r="V5" s="22">
         <f>Confirmed!V4/Testing!V4</f>
         <v>0.017106201</v>
       </c>
-      <c r="W5" s="21">
+      <c r="W5" s="22">
         <f>Confirmed!W4/Testing!W4</f>
         <v>0.01612903226</v>
       </c>
-      <c r="X5" s="21">
+      <c r="X5" s="22">
         <f>Confirmed!X4/Testing!X4</f>
         <v>0.01505646173</v>
       </c>
-      <c r="Y5" s="21">
+      <c r="Y5" s="22">
         <f>Confirmed!Y4/Testing!Y4</f>
         <v>0.0141760189</v>
       </c>
-      <c r="Z5" s="21">
+      <c r="Z5" s="22">
         <f>Confirmed!Z4/Testing!Z4</f>
         <v>0.0139431121</v>
       </c>
-      <c r="AA5" s="21">
+      <c r="AA5" s="22">
         <f>Confirmed!AA4/Testing!AA4</f>
         <v>0.01281366791</v>
       </c>
-      <c r="AB5" s="21">
+      <c r="AB5" s="22">
         <f>Confirmed!AB4/Testing!AB4</f>
         <v>0.01215805471</v>
       </c>
-      <c r="AC5" s="21">
+      <c r="AC5" s="22">
         <f>Confirmed!AC4/Testing!AC4</f>
         <v>0.01179801793</v>
       </c>
-      <c r="AD5" s="21">
+      <c r="AD5" s="22">
         <f>Confirmed!AD4/Testing!AD4</f>
         <v>0.01111605158</v>
       </c>
-      <c r="AE5" s="21">
+      <c r="AE5" s="22">
         <f>Confirmed!AE4/Testing!AE4</f>
         <v>0.01178451178</v>
       </c>
-      <c r="AF5" s="21">
+      <c r="AF5" s="22">
         <f>Confirmed!AF4/Testing!AF4</f>
         <v>0.01124949779</v>
       </c>
-      <c r="AG5" s="21">
+      <c r="AG5" s="22">
         <f>Confirmed!AG4/Testing!AG4</f>
         <v>0.0106302202</v>
       </c>
-      <c r="AH5" s="21">
+      <c r="AH5" s="22">
         <f>Confirmed!AH4/Testing!AH4</f>
         <v>0.01059167275</v>
       </c>
-      <c r="AI5" s="21">
+      <c r="AI5" s="22">
         <f>Confirmed!AI4/Testing!AI4</f>
         <v>0.009969061533</v>
       </c>
-      <c r="AJ5" s="21">
+      <c r="AJ5" s="22">
         <f>Confirmed!AJ4/Testing!AJ4</f>
         <v>0.0101207966</v>
       </c>
-      <c r="AK5" s="21">
+      <c r="AK5" s="22">
         <f>Confirmed!AK4/Testing!AK4</f>
         <v>0.01090342679</v>
       </c>
-      <c r="AL5" s="21">
+      <c r="AL5" s="22">
         <f>Confirmed!AL4/Testing!AL4</f>
         <v>0.01028202115</v>
       </c>
-      <c r="AM5" s="21">
+      <c r="AM5" s="22">
         <f>Confirmed!AM4/Testing!AM4</f>
         <v>0.009925558313</v>
       </c>
-      <c r="AN5" s="21">
+      <c r="AN5" s="22">
         <f>Confirmed!AN4/Testing!AN4</f>
         <v>0.009208103131</v>
       </c>
-      <c r="AO5" s="21">
+      <c r="AO5" s="22">
         <f>Confirmed!AO4/Testing!AO4</f>
         <v>0.008847320526</v>
       </c>
-      <c r="AP5" s="21">
+      <c r="AP5" s="22">
         <f>Confirmed!AP4/Testing!AP4</f>
         <v>0.008974048023</v>
       </c>
-      <c r="AQ5" s="21">
+      <c r="AQ5" s="22">
         <f>Confirmed!AQ4/Testing!AQ4</f>
         <v>0.009276437848</v>
       </c>
-      <c r="AR5" s="21">
+      <c r="AR5" s="22">
         <f>Confirmed!AR4/Testing!AR4</f>
         <v>0.009247027741</v>
       </c>
-      <c r="AS5" s="21">
+      <c r="AS5" s="22">
         <f>Confirmed!AS4/Testing!AS4</f>
         <v>0.008572025925</v>
       </c>
-      <c r="AT5" s="21">
+      <c r="AT5" s="22">
         <f>Confirmed!AT4/Testing!AT4</f>
         <v>0.00893388922</v>
       </c>
-      <c r="AU5" s="21">
+      <c r="AU5" s="22">
         <f>Confirmed!AU4/Testing!AU4</f>
         <v>0.009514747859</v>
       </c>
-      <c r="AV5" s="21">
+      <c r="AV5" s="22">
         <f>Confirmed!AV4/Testing!AV4</f>
         <v>0.009347507331</v>
       </c>
-      <c r="AW5" s="21">
+      <c r="AW5" s="22">
         <f>Confirmed!AW4/Testing!AW4</f>
         <v>0.009119607155</v>
       </c>
-      <c r="AX5" s="21">
+      <c r="AX5" s="22">
         <f>Confirmed!AX4/Testing!AX4</f>
         <v>0.009751176866</v>
       </c>
-      <c r="AY5" s="21">
+      <c r="AY5" s="22">
         <f>Confirmed!AY4/Testing!AY4</f>
         <v>0.01012698923</v>
       </c>
-      <c r="AZ5" s="21"/>
+      <c r="AZ5" s="22"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="22">
         <f>Confirmed!B5/Testing!B5</f>
         <v>0.01145038168</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="22">
         <f>Confirmed!C5/Testing!C5</f>
         <v>0.0113507378</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="22">
         <f>Confirmed!D5/Testing!D5</f>
         <v>0.01121304791</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="22">
         <f>Confirmed!E5/Testing!E5</f>
         <v>0.01039697543</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="22">
         <f>Confirmed!F5/Testing!F5</f>
         <v>0.01060070671</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="22">
         <f>Confirmed!G5/Testing!G5</f>
         <v>0.009836065574</v>
       </c>
-      <c r="H6" s="21">
+      <c r="H6" s="22">
         <f>Confirmed!H5/Testing!H5</f>
         <v>0.009841029523</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I6" s="22">
         <f>Confirmed!I5/Testing!I5</f>
         <v>0.009372746936</v>
       </c>
-      <c r="J6" s="21">
+      <c r="J6" s="22">
         <f>Confirmed!J5/Testing!J5</f>
         <v>0.01211305518</v>
       </c>
-      <c r="K6" s="21">
+      <c r="K6" s="22">
         <f>Confirmed!K5/Testing!K5</f>
         <v>0.01148691768</v>
       </c>
-      <c r="L6" s="21">
+      <c r="L6" s="22">
         <f>Confirmed!L5/Testing!L5</f>
         <v>0.01124297314</v>
       </c>
-      <c r="M6" s="21">
+      <c r="M6" s="22">
         <f>Confirmed!M5/Testing!M5</f>
         <v>0.01124297314</v>
       </c>
-      <c r="N6" s="21">
+      <c r="N6" s="22">
         <f>Confirmed!N5/Testing!N5</f>
         <v>0.01195219124</v>
       </c>
-      <c r="O6" s="21">
+      <c r="O6" s="22">
         <f>Confirmed!O5/Testing!O5</f>
         <v>0.0105374078</v>
       </c>
-      <c r="P6" s="21">
+      <c r="P6" s="22">
         <f>Confirmed!P5/Testing!P5</f>
         <v>0.009940357853</v>
       </c>
-      <c r="Q6" s="21">
+      <c r="Q6" s="22">
         <f>Confirmed!Q5/Testing!Q5</f>
         <v>0.009671179884</v>
       </c>
-      <c r="R6" s="21">
+      <c r="R6" s="22">
         <f>Confirmed!R5/Testing!R5</f>
         <v>0.009519492294</v>
       </c>
-      <c r="S6" s="21">
+      <c r="S6" s="22">
         <f>Confirmed!S5/Testing!S5</f>
         <v>0.009544468547</v>
       </c>
-      <c r="T6" s="21">
+      <c r="T6" s="22">
         <f>Confirmed!T5/Testing!T5</f>
         <v>0.009178139341</v>
       </c>
-      <c r="U6" s="21">
+      <c r="U6" s="22">
         <f>Confirmed!U5/Testing!U5</f>
         <v>0.00882117081</v>
       </c>
-      <c r="V6" s="21">
+      <c r="V6" s="22">
         <f>Confirmed!V5/Testing!V5</f>
         <v>0.00840015273</v>
       </c>
-      <c r="W6" s="21">
+      <c r="W6" s="22">
         <f>Confirmed!W5/Testing!W5</f>
         <v>0.008279337653</v>
       </c>
-      <c r="X6" s="21">
+      <c r="X6" s="22">
         <f>Confirmed!X5/Testing!X5</f>
         <v>0.008400537634</v>
       </c>
-      <c r="Y6" s="21">
+      <c r="Y6" s="22">
         <f>Confirmed!Y5/Testing!Y5</f>
         <v>0.007278481013</v>
       </c>
-      <c r="Z6" s="21">
+      <c r="Z6" s="22">
         <f>Confirmed!Z5/Testing!Z5</f>
         <v>0.006869772999</v>
       </c>
-      <c r="AA6" s="21">
+      <c r="AA6" s="22">
         <f>Confirmed!AA5/Testing!AA5</f>
         <v>0.00686302545</v>
       </c>
-      <c r="AB6" s="21">
+      <c r="AB6" s="22">
         <f>Confirmed!AB5/Testing!AB5</f>
         <v>0.00623982637</v>
       </c>
-      <c r="AC6" s="21">
+      <c r="AC6" s="22">
         <f>Confirmed!AC5/Testing!AC5</f>
         <v>0.005815423515</v>
       </c>
-      <c r="AD6" s="21">
+      <c r="AD6" s="22">
         <f>Confirmed!AD5/Testing!AD5</f>
         <v>0.005717008099</v>
       </c>
-      <c r="AE6" s="21">
+      <c r="AE6" s="22">
         <f>Confirmed!AE5/Testing!AE5</f>
         <v>0.005184851217</v>
       </c>
-      <c r="AF6" s="21">
+      <c r="AF6" s="22">
         <f>Confirmed!AF5/Testing!AF5</f>
         <v>0.00495049505</v>
       </c>
-      <c r="AG6" s="21">
+      <c r="AG6" s="22">
         <f>Confirmed!AG5/Testing!AG5</f>
         <v>0.0052877771</v>
       </c>
-      <c r="AH6" s="21">
+      <c r="AH6" s="22">
         <f>Confirmed!AH5/Testing!AH5</f>
         <v>0.004695754256</v>
       </c>
-      <c r="AI6" s="21">
+      <c r="AI6" s="22">
         <f>Confirmed!AI5/Testing!AI5</f>
         <v>0.005707972749</v>
       </c>
-      <c r="AJ6" s="21">
+      <c r="AJ6" s="22">
         <f>Confirmed!AJ5/Testing!AJ5</f>
         <v>0.00629590766</v>
       </c>
-      <c r="AK6" s="21">
+      <c r="AK6" s="22">
         <f>Confirmed!AK5/Testing!AK5</f>
         <v>0.005840146838</v>
       </c>
-      <c r="AL6" s="21">
+      <c r="AL6" s="22">
         <f>Confirmed!AL5/Testing!AL5</f>
         <v>0.006294256491</v>
       </c>
-      <c r="AM6" s="21">
+      <c r="AM6" s="22">
         <f>Confirmed!AM5/Testing!AM5</f>
         <v>0.006794682422</v>
       </c>
-      <c r="AN6" s="21">
+      <c r="AN6" s="22">
         <f>Confirmed!AN5/Testing!AN5</f>
         <v>0.007470049331</v>
       </c>
-      <c r="AO6" s="21">
+      <c r="AO6" s="22">
         <f>Confirmed!AO5/Testing!AO5</f>
         <v>0.007718348003</v>
       </c>
-      <c r="AP6" s="21">
+      <c r="AP6" s="22">
         <f>Confirmed!AP5/Testing!AP5</f>
         <v>0.007405482656</v>
       </c>
-      <c r="AQ6" s="21">
+      <c r="AQ6" s="22">
         <f>Confirmed!AQ5/Testing!AQ5</f>
         <v>0.007330103118</v>
       </c>
-      <c r="AR6" s="21">
+      <c r="AR6" s="22">
         <f>Confirmed!AR5/Testing!AR5</f>
         <v>0.007076306168</v>
       </c>
-      <c r="AS6" s="21">
+      <c r="AS6" s="22">
         <f>Confirmed!AS5/Testing!AS5</f>
         <v>0.00683167208</v>
       </c>
-      <c r="AT6" s="21">
+      <c r="AT6" s="22">
         <f>Confirmed!AT5/Testing!AT5</f>
         <v>0.006486601446</v>
       </c>
-      <c r="AU6" s="21">
+      <c r="AU6" s="22">
         <f>Confirmed!AU5/Testing!AU5</f>
         <v>0.006422018349</v>
       </c>
-      <c r="AV6" s="21">
+      <c r="AV6" s="22">
         <f>Confirmed!AV5/Testing!AV5</f>
         <v>0.00618556701</v>
       </c>
-      <c r="AW6" s="21">
+      <c r="AW6" s="22">
         <f>Confirmed!AW5/Testing!AW5</f>
         <v>0.006200676437</v>
       </c>
-      <c r="AX6" s="21">
+      <c r="AX6" s="22">
         <f>Confirmed!AX5/Testing!AX5</f>
         <v>0.006034405116</v>
       </c>
-      <c r="AY6" s="21">
+      <c r="AY6" s="22">
         <f>Confirmed!AY5/Testing!AY5</f>
         <v>0.005768899604</v>
       </c>
-      <c r="AZ6" s="21"/>
+      <c r="AZ6" s="22"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="22">
         <f>Confirmed!B6/Testing!B6</f>
         <v>0.009244992296</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="22">
         <f>Confirmed!C6/Testing!C6</f>
         <v>0.015130674</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="22">
         <f>Confirmed!D6/Testing!D6</f>
         <v>0.01483312732</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="22">
         <f>Confirmed!E6/Testing!E6</f>
         <v>0.0126002291</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="22">
         <f>Confirmed!F6/Testing!F6</f>
         <v>0.01498929336</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="22">
         <f>Confirmed!G6/Testing!G6</f>
         <v>0.01390268123</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="22">
         <f>Confirmed!H6/Testing!H6</f>
         <v>0.01466544455</v>
       </c>
-      <c r="I7" s="21">
+      <c r="I7" s="22">
         <f>Confirmed!I6/Testing!I6</f>
         <v>0.01397379913</v>
       </c>
-      <c r="J7" s="21">
+      <c r="J7" s="22">
         <f>Confirmed!J6/Testing!J6</f>
         <v>0.01466992665</v>
       </c>
-      <c r="K7" s="21">
+      <c r="K7" s="22">
         <f>Confirmed!K6/Testing!K6</f>
         <v>0.01469450889</v>
       </c>
-      <c r="L7" s="21">
+      <c r="L7" s="22">
         <f>Confirmed!L6/Testing!L6</f>
         <v>0.01438304315</v>
       </c>
-      <c r="M7" s="21">
+      <c r="M7" s="22">
         <f>Confirmed!M6/Testing!M6</f>
         <v>0.01438304315</v>
       </c>
-      <c r="N7" s="21">
+      <c r="N7" s="22">
         <f>Confirmed!N6/Testing!N6</f>
         <v>0.01448275862</v>
       </c>
-      <c r="O7" s="21">
+      <c r="O7" s="22">
         <f>Confirmed!O6/Testing!O6</f>
         <v>0.01404853129</v>
       </c>
-      <c r="P7" s="21">
+      <c r="P7" s="22">
         <f>Confirmed!P6/Testing!P6</f>
         <v>0.01444912703</v>
       </c>
-      <c r="Q7" s="21">
+      <c r="Q7" s="22">
         <f>Confirmed!Q6/Testing!Q6</f>
         <v>0.01347393087</v>
       </c>
-      <c r="R7" s="21">
+      <c r="R7" s="22">
         <f>Confirmed!R6/Testing!R6</f>
         <v>0.01263042284</v>
       </c>
-      <c r="S7" s="21">
+      <c r="S7" s="22">
         <f>Confirmed!S6/Testing!S6</f>
         <v>0.01209253417</v>
       </c>
-      <c r="T7" s="21">
+      <c r="T7" s="22">
         <f>Confirmed!T6/Testing!T6</f>
         <v>0.01212733704</v>
       </c>
-      <c r="U7" s="21">
+      <c r="U7" s="22">
         <f>Confirmed!U6/Testing!U6</f>
         <v>0.01214771623</v>
       </c>
-      <c r="V7" s="21">
+      <c r="V7" s="22">
         <f>Confirmed!V6/Testing!V6</f>
         <v>0.01202590194</v>
       </c>
-      <c r="W7" s="21">
+      <c r="W7" s="22">
         <f>Confirmed!W6/Testing!W6</f>
         <v>0.01133885739</v>
       </c>
-      <c r="X7" s="21">
+      <c r="X7" s="22">
         <f>Confirmed!X6/Testing!X6</f>
         <v>0.01058631922</v>
       </c>
-      <c r="Y7" s="21">
+      <c r="Y7" s="22">
         <f>Confirmed!Y6/Testing!Y6</f>
         <v>0.01035276074</v>
       </c>
-      <c r="Z7" s="21">
+      <c r="Z7" s="22">
         <f>Confirmed!Z6/Testing!Z6</f>
         <v>0.009771986971</v>
       </c>
-      <c r="AA7" s="21">
+      <c r="AA7" s="22">
         <f>Confirmed!AA6/Testing!AA6</f>
         <v>0.009352268791</v>
       </c>
-      <c r="AB7" s="21">
+      <c r="AB7" s="22">
         <f>Confirmed!AB6/Testing!AB6</f>
         <v>0.008875739645</v>
       </c>
-      <c r="AC7" s="21">
+      <c r="AC7" s="22">
         <f>Confirmed!AC6/Testing!AC6</f>
         <v>0.008269525268</v>
       </c>
-      <c r="AD7" s="21">
+      <c r="AD7" s="22">
         <f>Confirmed!AD6/Testing!AD6</f>
         <v>0.008369408369</v>
       </c>
-      <c r="AE7" s="21">
+      <c r="AE7" s="22">
         <f>Confirmed!AE6/Testing!AE6</f>
         <v>0.008194482382</v>
       </c>
-      <c r="AF7" s="21">
+      <c r="AF7" s="22">
         <f>Confirmed!AF6/Testing!AF6</f>
         <v>0.008083441982</v>
       </c>
-      <c r="AG7" s="21">
+      <c r="AG7" s="22">
         <f>Confirmed!AG6/Testing!AG6</f>
         <v>0.007639231148</v>
       </c>
-      <c r="AH7" s="21">
+      <c r="AH7" s="22">
         <f>Confirmed!AH6/Testing!AH6</f>
         <v>0.007349454718</v>
       </c>
-      <c r="AI7" s="21">
+      <c r="AI7" s="22">
         <f>Confirmed!AI6/Testing!AI6</f>
         <v>0.006915012269</v>
       </c>
-      <c r="AJ7" s="21">
+      <c r="AJ7" s="22">
         <f>Confirmed!AJ6/Testing!AJ6</f>
         <v>0.00678109769</v>
       </c>
-      <c r="AK7" s="21">
+      <c r="AK7" s="22">
         <f>Confirmed!AK6/Testing!AK6</f>
         <v>0.006874241812</v>
       </c>
-      <c r="AL7" s="21">
+      <c r="AL7" s="22">
         <f>Confirmed!AL6/Testing!AL6</f>
         <v>0.006862371331</v>
       </c>
-      <c r="AM7" s="21">
+      <c r="AM7" s="22">
         <f>Confirmed!AM6/Testing!AM6</f>
         <v>0.006621331424</v>
       </c>
-      <c r="AN7" s="21">
+      <c r="AN7" s="22">
         <f>Confirmed!AN6/Testing!AN6</f>
         <v>0.006659836066</v>
       </c>
-      <c r="AO7" s="21">
+      <c r="AO7" s="22">
         <f>Confirmed!AO6/Testing!AO6</f>
         <v>0.00656167979</v>
       </c>
-      <c r="AP7" s="21">
+      <c r="AP7" s="22">
         <f>Confirmed!AP6/Testing!AP6</f>
         <v>0.006296237998</v>
       </c>
-      <c r="AQ7" s="21">
+      <c r="AQ7" s="22">
         <f>Confirmed!AQ6/Testing!AQ6</f>
         <v>0.006171910281</v>
       </c>
-      <c r="AR7" s="21">
+      <c r="AR7" s="22">
         <f>Confirmed!AR6/Testing!AR6</f>
         <v>0.006144612746</v>
       </c>
-      <c r="AS7" s="21">
+      <c r="AS7" s="22">
         <f>Confirmed!AS6/Testing!AS6</f>
         <v>0.006920884788</v>
       </c>
-      <c r="AT7" s="21">
+      <c r="AT7" s="22">
         <f>Confirmed!AT6/Testing!AT6</f>
         <v>0.006956969853</v>
       </c>
-      <c r="AU7" s="21">
+      <c r="AU7" s="22">
         <f>Confirmed!AU6/Testing!AU6</f>
         <v>0.006669136717</v>
       </c>
-      <c r="AV7" s="21">
+      <c r="AV7" s="22">
         <f>Confirmed!AV6/Testing!AV6</f>
         <v>0.006423218746</v>
       </c>
-      <c r="AW7" s="21">
+      <c r="AW7" s="22">
         <f>Confirmed!AW6/Testing!AW6</f>
         <v>0.006146141589</v>
       </c>
-      <c r="AX7" s="21">
+      <c r="AX7" s="22">
         <f>Confirmed!AX6/Testing!AX6</f>
         <v>0.006001091107</v>
       </c>
-      <c r="AY7" s="21">
+      <c r="AY7" s="22">
         <f>Confirmed!AY6/Testing!AY6</f>
         <v>0.0059461715</v>
       </c>
-      <c r="AZ7" s="21"/>
+      <c r="AZ7" s="22"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="22">
         <f>Confirmed!B7/Testing!B7</f>
         <v>0.001903311762</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="22">
         <f>Confirmed!C7/Testing!C7</f>
         <v>0.003397893306</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="22">
         <f>Confirmed!D7/Testing!D7</f>
         <v>0.003661885871</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="22">
         <f>Confirmed!E7/Testing!E7</f>
         <v>0.003393665158</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="22">
         <f>Confirmed!F7/Testing!F7</f>
         <v>0.003173763555</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="22">
         <f>Confirmed!G7/Testing!G7</f>
         <v>0.003678273664</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="22">
         <f>Confirmed!H7/Testing!H7</f>
         <v>0.003849637681</v>
       </c>
-      <c r="I8" s="21">
+      <c r="I8" s="22">
         <f>Confirmed!I7/Testing!I7</f>
         <v>0.004529767041</v>
       </c>
-      <c r="J8" s="21">
+      <c r="J8" s="22">
         <f>Confirmed!J7/Testing!J7</f>
         <v>0.005034232783</v>
       </c>
-      <c r="K8" s="21">
+      <c r="K8" s="22">
         <f>Confirmed!K7/Testing!K7</f>
         <v>0.005920550038</v>
       </c>
-      <c r="L8" s="21">
+      <c r="L8" s="22">
         <f>Confirmed!L7/Testing!L7</f>
         <v>0.005982426622</v>
       </c>
-      <c r="M8" s="21">
+      <c r="M8" s="22">
         <f>Confirmed!M7/Testing!M7</f>
         <v>0.005982426622</v>
       </c>
-      <c r="N8" s="21">
+      <c r="N8" s="22">
         <f>Confirmed!N7/Testing!N7</f>
         <v>0.007664793051</v>
       </c>
-      <c r="O8" s="21">
+      <c r="O8" s="22">
         <f>Confirmed!O7/Testing!O7</f>
         <v>0.009619933764</v>
       </c>
-      <c r="P8" s="21">
+      <c r="P8" s="22">
         <f>Confirmed!P7/Testing!P7</f>
         <v>0.0101145322</v>
       </c>
-      <c r="Q8" s="21">
+      <c r="Q8" s="22">
         <f>Confirmed!Q7/Testing!Q7</f>
         <v>0.009986973513</v>
       </c>
-      <c r="R8" s="21">
+      <c r="R8" s="22">
         <f>Confirmed!R7/Testing!R7</f>
         <v>0.01193544012</v>
       </c>
-      <c r="S8" s="21">
+      <c r="S8" s="22">
         <f>Confirmed!S7/Testing!S7</f>
         <v>0.01350298624</v>
       </c>
-      <c r="T8" s="21">
+      <c r="T8" s="22">
         <f>Confirmed!T7/Testing!T7</f>
         <v>0.02172013481</v>
       </c>
-      <c r="U8" s="21">
+      <c r="U8" s="22">
         <f>Confirmed!U7/Testing!U7</f>
         <v>0.02388095524</v>
       </c>
-      <c r="V8" s="21">
+      <c r="V8" s="22">
         <f>Confirmed!V7/Testing!V7</f>
         <v>0.025139984</v>
       </c>
-      <c r="W8" s="21">
+      <c r="W8" s="22">
         <f>Confirmed!W7/Testing!W7</f>
         <v>0.02650290886</v>
       </c>
-      <c r="X8" s="21">
+      <c r="X8" s="22">
         <f>Confirmed!X7/Testing!X7</f>
         <v>0.02714932127</v>
       </c>
-      <c r="Y8" s="21">
+      <c r="Y8" s="22">
         <f>Confirmed!Y7/Testing!Y7</f>
         <v>0.02774621212</v>
       </c>
-      <c r="Z8" s="21">
+      <c r="Z8" s="22">
         <f>Confirmed!Z7/Testing!Z7</f>
         <v>0.02771321294</v>
       </c>
-      <c r="AA8" s="21">
+      <c r="AA8" s="22">
         <f>Confirmed!AA7/Testing!AA7</f>
         <v>0.02952250556</v>
       </c>
-      <c r="AB8" s="21">
+      <c r="AB8" s="22">
         <f>Confirmed!AB7/Testing!AB7</f>
         <v>0.03061307349</v>
       </c>
-      <c r="AC8" s="21">
+      <c r="AC8" s="22">
         <f>Confirmed!AC7/Testing!AC7</f>
         <v>0.03155027616</v>
       </c>
-      <c r="AD8" s="21">
+      <c r="AD8" s="22">
         <f>Confirmed!AD7/Testing!AD7</f>
         <v>0.03421484069</v>
       </c>
-      <c r="AE8" s="21">
+      <c r="AE8" s="22">
         <f>Confirmed!AE7/Testing!AE7</f>
         <v>0.03292403184</v>
       </c>
-      <c r="AF8" s="21">
+      <c r="AF8" s="22">
         <f>Confirmed!AF7/Testing!AF7</f>
         <v>0.0344605475</v>
       </c>
-      <c r="AG8" s="21">
+      <c r="AG8" s="22">
         <f>Confirmed!AG7/Testing!AG7</f>
         <v>0.03578819233</v>
       </c>
-      <c r="AH8" s="21">
+      <c r="AH8" s="22">
         <f>Confirmed!AH7/Testing!AH7</f>
         <v>0.03607190959</v>
       </c>
-      <c r="AI8" s="21">
+      <c r="AI8" s="22">
         <f>Confirmed!AI7/Testing!AI7</f>
         <v>0.0347145691</v>
       </c>
-      <c r="AJ8" s="21">
+      <c r="AJ8" s="22">
         <f>Confirmed!AJ7/Testing!AJ7</f>
         <v>0.03386548024</v>
       </c>
-      <c r="AK8" s="21">
+      <c r="AK8" s="22">
         <f>Confirmed!AK7/Testing!AK7</f>
         <v>0.03450686642</v>
       </c>
-      <c r="AL8" s="21">
+      <c r="AL8" s="22">
         <f>Confirmed!AL7/Testing!AL7</f>
         <v>0.03446814522</v>
       </c>
-      <c r="AM8" s="21">
+      <c r="AM8" s="22">
         <f>Confirmed!AM7/Testing!AM7</f>
         <v>0.03421145686</v>
       </c>
-      <c r="AN8" s="21">
+      <c r="AN8" s="22">
         <f>Confirmed!AN7/Testing!AN7</f>
         <v>0.03433150569</v>
       </c>
-      <c r="AO8" s="21">
+      <c r="AO8" s="22">
         <f>Confirmed!AO7/Testing!AO7</f>
         <v>0.03395737094</v>
       </c>
-      <c r="AP8" s="21">
+      <c r="AP8" s="22">
         <f>Confirmed!AP7/Testing!AP7</f>
         <v>0.03300933126</v>
       </c>
-      <c r="AQ8" s="21">
+      <c r="AQ8" s="22">
         <f>Confirmed!AQ7/Testing!AQ7</f>
         <v>0.03454045211</v>
       </c>
-      <c r="AR8" s="21">
+      <c r="AR8" s="22">
         <f>Confirmed!AR7/Testing!AR7</f>
         <v>0.03490752506</v>
       </c>
-      <c r="AS8" s="21">
+      <c r="AS8" s="22">
         <f>Confirmed!AS7/Testing!AS7</f>
         <v>0.03613205966</v>
       </c>
-      <c r="AT8" s="21">
+      <c r="AT8" s="22">
         <f>Confirmed!AT7/Testing!AT7</f>
         <v>0.0387601833</v>
       </c>
-      <c r="AU8" s="21">
+      <c r="AU8" s="22">
         <f>Confirmed!AU7/Testing!AU7</f>
         <v>0.041366687</v>
       </c>
-      <c r="AV8" s="21">
+      <c r="AV8" s="22">
         <f>Confirmed!AV7/Testing!AV7</f>
         <v>0.04418980461</v>
       </c>
-      <c r="AW8" s="21">
+      <c r="AW8" s="22">
         <f>Confirmed!AW7/Testing!AW7</f>
         <v>0.04312865497</v>
       </c>
-      <c r="AX8" s="21">
+      <c r="AX8" s="22">
         <f>Confirmed!AX7/Testing!AX7</f>
         <v>0.0422888254</v>
       </c>
-      <c r="AY8" s="21">
+      <c r="AY8" s="22">
         <f>Confirmed!AY7/Testing!AY7</f>
         <v>0.04282511789</v>
       </c>
-      <c r="AZ8" s="21"/>
+      <c r="AZ8" s="22"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="22">
         <f>Confirmed!B8/Testing!B8</f>
         <v>0.03363074811</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="22">
         <f>Confirmed!C8/Testing!C8</f>
         <v>0.04166666667</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="22">
         <f>Confirmed!D8/Testing!D8</f>
         <v>0.03962575674</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="22">
         <f>Confirmed!E8/Testing!E8</f>
         <v>0.03671596124</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="22">
         <f>Confirmed!F8/Testing!F8</f>
         <v>0.03528850739</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="22">
         <f>Confirmed!G8/Testing!G8</f>
         <v>0.03361344538</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="22">
         <f>Confirmed!H8/Testing!H8</f>
         <v>0.03429971417</v>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="22">
         <f>Confirmed!I8/Testing!I8</f>
         <v>0.03267211202</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J9" s="22">
         <f>Confirmed!J8/Testing!J8</f>
         <v>0.03086419753</v>
       </c>
-      <c r="K9" s="21">
+      <c r="K9" s="22">
         <f>Confirmed!K8/Testing!K8</f>
         <v>0.02995867769</v>
       </c>
-      <c r="L9" s="21">
+      <c r="L9" s="22">
         <f>Confirmed!L8/Testing!L8</f>
         <v>0.03000674309</v>
       </c>
-      <c r="M9" s="21">
+      <c r="M9" s="22">
         <f>Confirmed!M8/Testing!M8</f>
         <v>0.03000674309</v>
       </c>
-      <c r="N9" s="21">
+      <c r="N9" s="22">
         <f>Confirmed!N8/Testing!N8</f>
         <v>0.02702702703</v>
       </c>
-      <c r="O9" s="21">
+      <c r="O9" s="22">
         <f>Confirmed!O8/Testing!O8</f>
         <v>0.02645051195</v>
       </c>
-      <c r="P9" s="21">
+      <c r="P9" s="22">
         <f>Confirmed!P8/Testing!P8</f>
         <v>0.02520783052</v>
       </c>
-      <c r="Q9" s="21">
+      <c r="Q9" s="22">
         <f>Confirmed!Q8/Testing!Q8</f>
         <v>0.0245302714</v>
       </c>
-      <c r="R9" s="21">
+      <c r="R9" s="22">
         <f>Confirmed!R8/Testing!R8</f>
         <v>0.02347762289</v>
       </c>
-      <c r="S9" s="21">
+      <c r="S9" s="22">
         <f>Confirmed!S8/Testing!S8</f>
         <v>0.02247191011</v>
       </c>
-      <c r="T9" s="21">
+      <c r="T9" s="22">
         <f>Confirmed!T8/Testing!T8</f>
         <v>0.02205716858</v>
       </c>
-      <c r="U9" s="21">
+      <c r="U9" s="22">
         <f>Confirmed!U8/Testing!U8</f>
         <v>0.02099112746</v>
       </c>
-      <c r="V9" s="21">
+      <c r="V9" s="22">
         <f>Confirmed!V8/Testing!V8</f>
         <v>0.02019369462</v>
       </c>
-      <c r="W9" s="21">
+      <c r="W9" s="22">
         <f>Confirmed!W8/Testing!W8</f>
         <v>0.01942501943</v>
       </c>
-      <c r="X9" s="21">
+      <c r="X9" s="22">
         <f>Confirmed!X8/Testing!X8</f>
         <v>0.01813236627</v>
       </c>
-      <c r="Y9" s="21">
+      <c r="Y9" s="22">
         <f>Confirmed!Y8/Testing!Y8</f>
         <v>0.01707358716</v>
       </c>
-      <c r="Z9" s="21">
+      <c r="Z9" s="22">
         <f>Confirmed!Z8/Testing!Z8</f>
         <v>0.0169245648</v>
       </c>
-      <c r="AA9" s="21">
+      <c r="AA9" s="22">
         <f>Confirmed!AA8/Testing!AA8</f>
         <v>0.01635550069</v>
       </c>
-      <c r="AB9" s="21">
+      <c r="AB9" s="22">
         <f>Confirmed!AB8/Testing!AB8</f>
         <v>0.01551976574</v>
       </c>
-      <c r="AC9" s="21">
+      <c r="AC9" s="22">
         <f>Confirmed!AC8/Testing!AC8</f>
         <v>0.01446111869</v>
       </c>
-      <c r="AD9" s="21">
+      <c r="AD9" s="22">
         <f>Confirmed!AD8/Testing!AD8</f>
         <v>0.01426735219</v>
       </c>
-      <c r="AE9" s="21">
+      <c r="AE9" s="22">
         <f>Confirmed!AE8/Testing!AE8</f>
         <v>0.01350364964</v>
       </c>
-      <c r="AF9" s="21">
+      <c r="AF9" s="22">
         <f>Confirmed!AF8/Testing!AF8</f>
         <v>0.01277584204</v>
       </c>
-      <c r="AG9" s="21">
+      <c r="AG9" s="22">
         <f>Confirmed!AG8/Testing!AG8</f>
         <v>0.01218173837</v>
       </c>
-      <c r="AH9" s="21">
+      <c r="AH9" s="22">
         <f>Confirmed!AH8/Testing!AH8</f>
         <v>0.01193115827</v>
       </c>
-      <c r="AI9" s="21">
+      <c r="AI9" s="22">
         <f>Confirmed!AI8/Testing!AI8</f>
         <v>0.01122702434</v>
       </c>
-      <c r="AJ9" s="21">
+      <c r="AJ9" s="22">
         <f>Confirmed!AJ8/Testing!AJ8</f>
         <v>0.01094752737</v>
       </c>
-      <c r="AK9" s="21">
+      <c r="AK9" s="22">
         <f>Confirmed!AK8/Testing!AK8</f>
         <v>0.01062488745</v>
       </c>
-      <c r="AL9" s="21">
+      <c r="AL9" s="22">
         <f>Confirmed!AL8/Testing!AL8</f>
         <v>0.01027339107</v>
       </c>
-      <c r="AM9" s="21">
+      <c r="AM9" s="22">
         <f>Confirmed!AM8/Testing!AM8</f>
         <v>0.009723439866</v>
       </c>
-      <c r="AN9" s="21">
+      <c r="AN9" s="22">
         <f>Confirmed!AN8/Testing!AN8</f>
         <v>0.009506426344</v>
       </c>
-      <c r="AO9" s="21">
+      <c r="AO9" s="22">
         <f>Confirmed!AO8/Testing!AO8</f>
         <v>0.009352623119</v>
       </c>
-      <c r="AP9" s="21">
+      <c r="AP9" s="22">
         <f>Confirmed!AP8/Testing!AP8</f>
         <v>0.009113853057</v>
       </c>
-      <c r="AQ9" s="21">
+      <c r="AQ9" s="22">
         <f>Confirmed!AQ8/Testing!AQ8</f>
         <v>0.008983641727</v>
       </c>
-      <c r="AR9" s="21">
+      <c r="AR9" s="22">
         <f>Confirmed!AR8/Testing!AR8</f>
         <v>0.0084643289</v>
       </c>
-      <c r="AS9" s="21">
+      <c r="AS9" s="22">
         <f>Confirmed!AS8/Testing!AS8</f>
         <v>0.008098634111</v>
       </c>
-      <c r="AT9" s="21">
+      <c r="AT9" s="22">
         <f>Confirmed!AT8/Testing!AT8</f>
         <v>0.007746600103</v>
       </c>
-      <c r="AU9" s="21">
+      <c r="AU9" s="22">
         <f>Confirmed!AU8/Testing!AU8</f>
         <v>0.007426151053</v>
       </c>
-      <c r="AV9" s="21">
+      <c r="AV9" s="22">
         <f>Confirmed!AV8/Testing!AV8</f>
         <v>0.007152317881</v>
       </c>
-      <c r="AW9" s="21">
+      <c r="AW9" s="22">
         <f>Confirmed!AW8/Testing!AW8</f>
         <v>0.00699584305</v>
       </c>
-      <c r="AX9" s="21">
+      <c r="AX9" s="22">
         <f>Confirmed!AX8/Testing!AX8</f>
         <v>0.007046702629</v>
       </c>
-      <c r="AY9" s="21">
+      <c r="AY9" s="22">
         <f>Confirmed!AY8/Testing!AY8</f>
         <v>0.007015750592</v>
       </c>
-      <c r="AZ9" s="21"/>
+      <c r="AZ9" s="22"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="22">
         <f>Confirmed!B9/Testing!B9</f>
         <v>0.0257296467</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="22">
         <f>Confirmed!C9/Testing!C9</f>
         <v>0.02674438539</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="22">
         <f>Confirmed!D9/Testing!D9</f>
         <v>0.02570812808</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="22">
         <f>Confirmed!E9/Testing!E9</f>
         <v>0.02439372325</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="22">
         <f>Confirmed!F9/Testing!F9</f>
         <v>0.02387940235</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="22">
         <f>Confirmed!G9/Testing!G9</f>
         <v>0.02300841168</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="22">
         <f>Confirmed!H9/Testing!H9</f>
         <v>0.02353209961</v>
       </c>
-      <c r="I10" s="21">
+      <c r="I10" s="22">
         <f>Confirmed!I9/Testing!I9</f>
         <v>0.02339244914</v>
       </c>
-      <c r="J10" s="21">
+      <c r="J10" s="22">
         <f>Confirmed!J9/Testing!J9</f>
         <v>0.02356765542</v>
       </c>
-      <c r="K10" s="21">
+      <c r="K10" s="22">
         <f>Confirmed!K9/Testing!K9</f>
         <v>0.02369942197</v>
       </c>
-      <c r="L10" s="21">
+      <c r="L10" s="22">
         <f>Confirmed!L9/Testing!L9</f>
         <v>0.02423842309</v>
       </c>
-      <c r="M10" s="21">
+      <c r="M10" s="22">
         <f>Confirmed!M9/Testing!M9</f>
         <v>0.02423842309</v>
       </c>
-      <c r="N10" s="21">
+      <c r="N10" s="22">
         <f>Confirmed!N9/Testing!N9</f>
         <v>0.03041498411</v>
       </c>
-      <c r="O10" s="21">
+      <c r="O10" s="22">
         <f>Confirmed!O9/Testing!O9</f>
         <v>0.0307875895</v>
       </c>
-      <c r="P10" s="21">
+      <c r="P10" s="22">
         <f>Confirmed!P9/Testing!P9</f>
         <v>0.03091236495</v>
       </c>
-      <c r="Q10" s="21">
+      <c r="Q10" s="22">
         <f>Confirmed!Q9/Testing!Q9</f>
         <v>0.03051540371</v>
       </c>
-      <c r="R10" s="21">
+      <c r="R10" s="22">
         <f>Confirmed!R9/Testing!R9</f>
         <v>0.03030925014</v>
       </c>
-      <c r="S10" s="21">
+      <c r="S10" s="22">
         <f>Confirmed!S9/Testing!S9</f>
         <v>0.03045386076</v>
       </c>
-      <c r="T10" s="21">
+      <c r="T10" s="22">
         <f>Confirmed!T9/Testing!T9</f>
         <v>0.0307895731</v>
       </c>
-      <c r="U10" s="21">
+      <c r="U10" s="22">
         <f>Confirmed!U9/Testing!U9</f>
         <v>0.03141836673</v>
       </c>
-      <c r="V10" s="21">
+      <c r="V10" s="22">
         <f>Confirmed!V9/Testing!V9</f>
         <v>0.03106807309</v>
       </c>
-      <c r="W10" s="21">
+      <c r="W10" s="22">
         <f>Confirmed!W9/Testing!W9</f>
         <v>0.03211781968</v>
       </c>
-      <c r="X10" s="21">
+      <c r="X10" s="22">
         <f>Confirmed!X9/Testing!X9</f>
         <v>0.03063812519</v>
       </c>
-      <c r="Y10" s="21">
+      <c r="Y10" s="22">
         <f>Confirmed!Y9/Testing!Y9</f>
         <v>0.02947217578</v>
       </c>
-      <c r="Z10" s="21">
+      <c r="Z10" s="22">
         <f>Confirmed!Z9/Testing!Z9</f>
         <v>0.02881493506</v>
       </c>
-      <c r="AA10" s="21">
+      <c r="AA10" s="22">
         <f>Confirmed!AA9/Testing!AA9</f>
         <v>0.02896361203</v>
       </c>
-      <c r="AB10" s="21">
+      <c r="AB10" s="22">
         <f>Confirmed!AB9/Testing!AB9</f>
         <v>0.03104775948</v>
       </c>
-      <c r="AC10" s="21">
+      <c r="AC10" s="22">
         <f>Confirmed!AC9/Testing!AC9</f>
         <v>0.03079917564</v>
       </c>
-      <c r="AD10" s="21">
+      <c r="AD10" s="22">
         <f>Confirmed!AD9/Testing!AD9</f>
         <v>0.03023874587</v>
       </c>
-      <c r="AE10" s="21">
+      <c r="AE10" s="22">
         <f>Confirmed!AE9/Testing!AE9</f>
         <v>0.028825211</v>
       </c>
-      <c r="AF10" s="21">
+      <c r="AF10" s="22">
         <f>Confirmed!AF9/Testing!AF9</f>
         <v>0.02803950874</v>
       </c>
-      <c r="AG10" s="21">
+      <c r="AG10" s="22">
         <f>Confirmed!AG9/Testing!AG9</f>
         <v>0.02769249662</v>
       </c>
-      <c r="AH10" s="21">
+      <c r="AH10" s="22">
         <f>Confirmed!AH9/Testing!AH9</f>
         <v>0.0271459798</v>
       </c>
-      <c r="AI10" s="21">
+      <c r="AI10" s="22">
         <f>Confirmed!AI9/Testing!AI9</f>
         <v>0.02657253245</v>
       </c>
-      <c r="AJ10" s="21">
+      <c r="AJ10" s="22">
         <f>Confirmed!AJ9/Testing!AJ9</f>
         <v>0.02587458746</v>
       </c>
-      <c r="AK10" s="21">
+      <c r="AK10" s="22">
         <f>Confirmed!AK9/Testing!AK9</f>
         <v>0.02534068868</v>
       </c>
-      <c r="AL10" s="21">
+      <c r="AL10" s="22">
         <f>Confirmed!AL9/Testing!AL9</f>
         <v>0.02496377758</v>
       </c>
-      <c r="AM10" s="21">
+      <c r="AM10" s="22">
         <f>Confirmed!AM9/Testing!AM9</f>
         <v>0.02399108138</v>
       </c>
-      <c r="AN10" s="21">
+      <c r="AN10" s="22">
         <f>Confirmed!AN9/Testing!AN9</f>
         <v>0.02353091358</v>
       </c>
-      <c r="AO10" s="21">
+      <c r="AO10" s="22">
         <f>Confirmed!AO9/Testing!AO9</f>
         <v>0.023342804</v>
       </c>
-      <c r="AP10" s="21">
+      <c r="AP10" s="22">
         <f>Confirmed!AP9/Testing!AP9</f>
         <v>0.02331921236</v>
       </c>
-      <c r="AQ10" s="21">
+      <c r="AQ10" s="22">
         <f>Confirmed!AQ9/Testing!AQ9</f>
         <v>0.02258106866</v>
       </c>
-      <c r="AR10" s="21">
+      <c r="AR10" s="22">
         <f>Confirmed!AR9/Testing!AR9</f>
         <v>0.02230887013</v>
       </c>
-      <c r="AS10" s="21">
+      <c r="AS10" s="22">
         <f>Confirmed!AS9/Testing!AS9</f>
         <v>0.02211476685</v>
       </c>
-      <c r="AT10" s="21">
+      <c r="AT10" s="22">
         <f>Confirmed!AT9/Testing!AT9</f>
         <v>0.0217192391</v>
       </c>
-      <c r="AU10" s="21">
+      <c r="AU10" s="22">
         <f>Confirmed!AU9/Testing!AU9</f>
         <v>0.02111288933</v>
       </c>
-      <c r="AV10" s="21">
+      <c r="AV10" s="22">
         <f>Confirmed!AV9/Testing!AV9</f>
         <v>0.02066072831</v>
       </c>
-      <c r="AW10" s="21">
+      <c r="AW10" s="22">
         <f>Confirmed!AW9/Testing!AW9</f>
         <v>0.02003942647</v>
       </c>
-      <c r="AX10" s="21">
+      <c r="AX10" s="22">
         <f>Confirmed!AX9/Testing!AX9</f>
         <v>0.01963210202</v>
       </c>
-      <c r="AY10" s="21">
+      <c r="AY10" s="22">
         <f>Confirmed!AY9/Testing!AY9</f>
         <v>0.01926276386</v>
       </c>
-      <c r="AZ10" s="21"/>
+      <c r="AZ10" s="22"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="22">
         <f>Confirmed!B10/Testing!B10</f>
         <v>0.03934031953</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="22">
         <f>Confirmed!C10/Testing!C10</f>
         <v>0.04156441718</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="22">
         <f>Confirmed!D10/Testing!D10</f>
         <v>0.04269972452</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="22">
         <f>Confirmed!E10/Testing!E10</f>
         <v>0.04135818228</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="22">
         <f>Confirmed!F10/Testing!F10</f>
         <v>0.03879207448</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="22">
         <f>Confirmed!G10/Testing!G10</f>
         <v>0.03608589772</v>
       </c>
-      <c r="H11" s="21">
+      <c r="H11" s="22">
         <f>Confirmed!H10/Testing!H10</f>
         <v>0.03607931316</v>
       </c>
-      <c r="I11" s="21">
+      <c r="I11" s="22">
         <f>Confirmed!I10/Testing!I10</f>
         <v>0.03640965732</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="22">
         <f>Confirmed!J10/Testing!J10</f>
         <v>0.03935648064</v>
       </c>
-      <c r="K11" s="21">
+      <c r="K11" s="22">
         <f>Confirmed!K10/Testing!K10</f>
         <v>0.03913455737</v>
       </c>
-      <c r="L11" s="21">
+      <c r="L11" s="22">
         <f>Confirmed!L10/Testing!L10</f>
         <v>0.03898734177</v>
       </c>
-      <c r="M11" s="21">
+      <c r="M11" s="22">
         <f>Confirmed!M10/Testing!M10</f>
         <v>0.03898734177</v>
       </c>
-      <c r="N11" s="21">
+      <c r="N11" s="22">
         <f>Confirmed!N10/Testing!N10</f>
         <v>0.03805058037</v>
       </c>
-      <c r="O11" s="21">
+      <c r="O11" s="22">
         <f>Confirmed!O10/Testing!O10</f>
         <v>0.03666002278</v>
       </c>
-      <c r="P11" s="21">
+      <c r="P11" s="22">
         <f>Confirmed!P10/Testing!P10</f>
         <v>0.03631847476</v>
       </c>
-      <c r="Q11" s="21">
+      <c r="Q11" s="22">
         <f>Confirmed!Q10/Testing!Q10</f>
         <v>0.03566529492</v>
       </c>
-      <c r="R11" s="21">
+      <c r="R11" s="22">
         <f>Confirmed!R10/Testing!R10</f>
         <v>0.03593510866</v>
       </c>
-      <c r="S11" s="21">
+      <c r="S11" s="22">
         <f>Confirmed!S10/Testing!S10</f>
         <v>0.0361558746</v>
       </c>
-      <c r="T11" s="21">
+      <c r="T11" s="22">
         <f>Confirmed!T10/Testing!T10</f>
         <v>0.03622535211</v>
       </c>
-      <c r="U11" s="21">
+      <c r="U11" s="22">
         <f>Confirmed!U10/Testing!U10</f>
         <v>0.03558468288</v>
       </c>
-      <c r="V11" s="21">
+      <c r="V11" s="22">
         <f>Confirmed!V10/Testing!V10</f>
         <v>0.03481175864</v>
       </c>
-      <c r="W11" s="21">
+      <c r="W11" s="22">
         <f>Confirmed!W10/Testing!W10</f>
         <v>0.03486336672</v>
       </c>
-      <c r="X11" s="21">
+      <c r="X11" s="22">
         <f>Confirmed!X10/Testing!X10</f>
         <v>0.03794308537</v>
       </c>
-      <c r="Y11" s="21">
+      <c r="Y11" s="22">
         <f>Confirmed!Y10/Testing!Y10</f>
         <v>0.03709718779</v>
       </c>
-      <c r="Z11" s="21">
+      <c r="Z11" s="22">
         <f>Confirmed!Z10/Testing!Z10</f>
         <v>0.03792616502</v>
       </c>
-      <c r="AA11" s="21">
+      <c r="AA11" s="22">
         <f>Confirmed!AA10/Testing!AA10</f>
         <v>0.03900818786</v>
       </c>
-      <c r="AB11" s="21">
+      <c r="AB11" s="22">
         <f>Confirmed!AB10/Testing!AB10</f>
         <v>0.03954408854</v>
       </c>
-      <c r="AC11" s="21">
+      <c r="AC11" s="22">
         <f>Confirmed!AC10/Testing!AC10</f>
         <v>0.04367423596</v>
       </c>
-      <c r="AD11" s="21">
+      <c r="AD11" s="22">
         <f>Confirmed!AD10/Testing!AD10</f>
         <v>0.04545747008</v>
       </c>
-      <c r="AE11" s="21">
+      <c r="AE11" s="22">
         <f>Confirmed!AE10/Testing!AE10</f>
         <v>0.04610091045</v>
       </c>
-      <c r="AF11" s="21">
+      <c r="AF11" s="22">
         <f>Confirmed!AF10/Testing!AF10</f>
         <v>0.04674554493</v>
       </c>
-      <c r="AG11" s="21">
+      <c r="AG11" s="22">
         <f>Confirmed!AG10/Testing!AG10</f>
         <v>0.04771584759</v>
       </c>
-      <c r="AH11" s="21">
+      <c r="AH11" s="22">
         <f>Confirmed!AH10/Testing!AH10</f>
         <v>0.04942252293</v>
       </c>
-      <c r="AI11" s="21">
+      <c r="AI11" s="22">
         <f>Confirmed!AI10/Testing!AI10</f>
         <v>0.05309756522</v>
       </c>
-      <c r="AJ11" s="21">
+      <c r="AJ11" s="22">
         <f>Confirmed!AJ10/Testing!AJ10</f>
         <v>0.0553258841</v>
       </c>
-      <c r="AK11" s="21">
+      <c r="AK11" s="22">
         <f>Confirmed!AK10/Testing!AK10</f>
         <v>0.05650341455</v>
       </c>
-      <c r="AL11" s="21">
+      <c r="AL11" s="22">
         <f>Confirmed!AL10/Testing!AL10</f>
         <v>0.05738088154</v>
       </c>
-      <c r="AM11" s="21">
+      <c r="AM11" s="22">
         <f>Confirmed!AM10/Testing!AM10</f>
         <v>0.06072696804</v>
       </c>
-      <c r="AN11" s="21">
+      <c r="AN11" s="22">
         <f>Confirmed!AN10/Testing!AN10</f>
         <v>0.06399908627</v>
       </c>
-      <c r="AO11" s="21">
+      <c r="AO11" s="22">
         <f>Confirmed!AO10/Testing!AO10</f>
         <v>0.0660046088</v>
       </c>
-      <c r="AP11" s="21">
+      <c r="AP11" s="22">
         <f>Confirmed!AP10/Testing!AP10</f>
         <v>0.06598111817</v>
       </c>
-      <c r="AQ11" s="21">
+      <c r="AQ11" s="22">
         <f>Confirmed!AQ10/Testing!AQ10</f>
         <v>0.06702241912</v>
       </c>
-      <c r="AR11" s="21">
+      <c r="AR11" s="22">
         <f>Confirmed!AR10/Testing!AR10</f>
         <v>0.0716390805</v>
       </c>
-      <c r="AS11" s="21">
+      <c r="AS11" s="22">
         <f>Confirmed!AS10/Testing!AS10</f>
         <v>0.07274900157</v>
       </c>
-      <c r="AT11" s="21">
+      <c r="AT11" s="22">
         <f>Confirmed!AT10/Testing!AT10</f>
         <v>0.07422727795</v>
       </c>
-      <c r="AU11" s="21">
+      <c r="AU11" s="22">
         <f>Confirmed!AU10/Testing!AU10</f>
         <v>0.07739439335</v>
       </c>
-      <c r="AV11" s="21">
+      <c r="AV11" s="22">
         <f>Confirmed!AV10/Testing!AV10</f>
         <v>0.08095850628</v>
       </c>
-      <c r="AW11" s="21">
+      <c r="AW11" s="22">
         <f>Confirmed!AW10/Testing!AW10</f>
         <v>0.08518386925</v>
       </c>
-      <c r="AX11" s="21">
+      <c r="AX11" s="22">
         <f>Confirmed!AX10/Testing!AX10</f>
         <v>0.08801167812</v>
       </c>
-      <c r="AY11" s="21">
+      <c r="AY11" s="22">
         <f>Confirmed!AY10/Testing!AY10</f>
         <v>0.09068918196</v>
       </c>
-      <c r="AZ11" s="21"/>
+      <c r="AZ11" s="22"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="22">
         <f>Confirmed!B11/Testing!B11</f>
         <v>0.04339522546</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="22">
         <f>Confirmed!C11/Testing!C11</f>
         <v>0.05048782798</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="22">
         <f>Confirmed!D11/Testing!D11</f>
         <v>0.04968098681</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="22">
         <f>Confirmed!E11/Testing!E11</f>
         <v>0.04871511903</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="22">
         <f>Confirmed!F11/Testing!F11</f>
         <v>0.04666420936</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="22">
         <f>Confirmed!G11/Testing!G11</f>
         <v>0.04409050516</v>
       </c>
-      <c r="H12" s="21">
+      <c r="H12" s="22">
         <f>Confirmed!H11/Testing!H11</f>
         <v>0.04185077642</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="22">
         <f>Confirmed!I11/Testing!I11</f>
         <v>0.04040161125</v>
       </c>
-      <c r="J12" s="21">
+      <c r="J12" s="22">
         <f>Confirmed!J11/Testing!J11</f>
         <v>0.0389019872</v>
       </c>
-      <c r="K12" s="21">
+      <c r="K12" s="22">
         <f>Confirmed!K11/Testing!K11</f>
         <v>0.03747870528</v>
       </c>
-      <c r="L12" s="21">
+      <c r="L12" s="22">
         <f>Confirmed!L11/Testing!L11</f>
         <v>0.03715864082</v>
       </c>
-      <c r="M12" s="21">
+      <c r="M12" s="22">
         <f>Confirmed!M11/Testing!M11</f>
         <v>0.03715864082</v>
       </c>
-      <c r="N12" s="21">
+      <c r="N12" s="22">
         <f>Confirmed!N11/Testing!N11</f>
         <v>0.03712495253</v>
       </c>
-      <c r="O12" s="21">
+      <c r="O12" s="22">
         <f>Confirmed!O11/Testing!O11</f>
         <v>0.03494966369</v>
       </c>
-      <c r="P12" s="21">
+      <c r="P12" s="22">
         <f>Confirmed!P11/Testing!P11</f>
         <v>0.0332103321</v>
       </c>
-      <c r="Q12" s="21">
+      <c r="Q12" s="22">
         <f>Confirmed!Q11/Testing!Q11</f>
         <v>0.03279812813</v>
       </c>
-      <c r="R12" s="21">
+      <c r="R12" s="22">
         <f>Confirmed!R11/Testing!R11</f>
         <v>0.03270321361</v>
       </c>
-      <c r="S12" s="21">
+      <c r="S12" s="22">
         <f>Confirmed!S11/Testing!S11</f>
         <v>0.03220903301</v>
       </c>
-      <c r="T12" s="21">
+      <c r="T12" s="22">
         <f>Confirmed!T11/Testing!T11</f>
         <v>0.03162729202</v>
       </c>
-      <c r="U12" s="21">
+      <c r="U12" s="22">
         <f>Confirmed!U11/Testing!U11</f>
         <v>0.03110888108</v>
       </c>
-      <c r="V12" s="21">
+      <c r="V12" s="22">
         <f>Confirmed!V11/Testing!V11</f>
         <v>0.03086380431</v>
       </c>
-      <c r="W12" s="21">
+      <c r="W12" s="22">
         <f>Confirmed!W11/Testing!W11</f>
         <v>0.03056965256</v>
       </c>
-      <c r="X12" s="21">
+      <c r="X12" s="22">
         <f>Confirmed!X11/Testing!X11</f>
         <v>0.03086021807</v>
       </c>
-      <c r="Y12" s="21">
+      <c r="Y12" s="22">
         <f>Confirmed!Y11/Testing!Y11</f>
         <v>0.03030143061</v>
       </c>
-      <c r="Z12" s="21">
+      <c r="Z12" s="22">
         <f>Confirmed!Z11/Testing!Z11</f>
         <v>0.02915379248</v>
       </c>
-      <c r="AA12" s="21">
+      <c r="AA12" s="22">
         <f>Confirmed!AA11/Testing!AA11</f>
         <v>0.02859937029</v>
       </c>
-      <c r="AB12" s="21">
+      <c r="AB12" s="22">
         <f>Confirmed!AB11/Testing!AB11</f>
         <v>0.0277035897</v>
       </c>
-      <c r="AC12" s="21">
+      <c r="AC12" s="22">
         <f>Confirmed!AC11/Testing!AC11</f>
         <v>0.02640347547</v>
       </c>
-      <c r="AD12" s="21">
+      <c r="AD12" s="22">
         <f>Confirmed!AD11/Testing!AD11</f>
         <v>0.025451511</v>
       </c>
-      <c r="AE12" s="21">
+      <c r="AE12" s="22">
         <f>Confirmed!AE11/Testing!AE11</f>
         <v>0.02452234091</v>
       </c>
-      <c r="AF12" s="21">
+      <c r="AF12" s="22">
         <f>Confirmed!AF11/Testing!AF11</f>
         <v>0.02389629975</v>
       </c>
-      <c r="AG12" s="21">
+      <c r="AG12" s="22">
         <f>Confirmed!AG11/Testing!AG11</f>
         <v>0.02295399023</v>
       </c>
-      <c r="AH12" s="21">
+      <c r="AH12" s="22">
         <f>Confirmed!AH11/Testing!AH11</f>
         <v>0.0224761283</v>
       </c>
-      <c r="AI12" s="21">
+      <c r="AI12" s="22">
         <f>Confirmed!AI11/Testing!AI11</f>
         <v>0.021626271</v>
       </c>
-      <c r="AJ12" s="21">
+      <c r="AJ12" s="22">
         <f>Confirmed!AJ11/Testing!AJ11</f>
         <v>0.02109655394</v>
       </c>
-      <c r="AK12" s="21">
+      <c r="AK12" s="22">
         <f>Confirmed!AK11/Testing!AK11</f>
         <v>0.02097658751</v>
       </c>
-      <c r="AL12" s="21">
+      <c r="AL12" s="22">
         <f>Confirmed!AL11/Testing!AL11</f>
         <v>0.02097388109</v>
       </c>
-      <c r="AM12" s="21">
+      <c r="AM12" s="22">
         <f>Confirmed!AM11/Testing!AM11</f>
         <v>0.02000887093</v>
       </c>
-      <c r="AN12" s="21">
+      <c r="AN12" s="22">
         <f>Confirmed!AN11/Testing!AN11</f>
         <v>0.019527622</v>
       </c>
-      <c r="AO12" s="21">
+      <c r="AO12" s="22">
         <f>Confirmed!AO11/Testing!AO11</f>
         <v>0.01916756085</v>
       </c>
-      <c r="AP12" s="21">
+      <c r="AP12" s="22">
         <f>Confirmed!AP11/Testing!AP11</f>
         <v>0.01864054101</v>
       </c>
-      <c r="AQ12" s="21">
+      <c r="AQ12" s="22">
         <f>Confirmed!AQ11/Testing!AQ11</f>
         <v>0.01869604419</v>
       </c>
-      <c r="AR12" s="21">
+      <c r="AR12" s="22">
         <f>Confirmed!AR11/Testing!AR11</f>
         <v>0.01821079661</v>
       </c>
-      <c r="AS12" s="21">
+      <c r="AS12" s="22">
         <f>Confirmed!AS11/Testing!AS11</f>
         <v>0.01784463026</v>
       </c>
-      <c r="AT12" s="21">
+      <c r="AT12" s="22">
         <f>Confirmed!AT11/Testing!AT11</f>
         <v>0.01731494212</v>
       </c>
-      <c r="AU12" s="21">
+      <c r="AU12" s="22">
         <f>Confirmed!AU11/Testing!AU11</f>
         <v>0.01676020408</v>
       </c>
-      <c r="AV12" s="21">
+      <c r="AV12" s="22">
         <f>Confirmed!AV11/Testing!AV11</f>
         <v>0.01649440632</v>
       </c>
-      <c r="AW12" s="21">
+      <c r="AW12" s="22">
         <f>Confirmed!AW11/Testing!AW11</f>
         <v>0.01625353636</v>
       </c>
-      <c r="AX12" s="21">
+      <c r="AX12" s="22">
         <f>Confirmed!AX11/Testing!AX11</f>
         <v>0.01603972744</v>
       </c>
-      <c r="AY12" s="21">
+      <c r="AY12" s="22">
         <f>Confirmed!AY11/Testing!AY11</f>
         <v>0.01587312988</v>
       </c>
-      <c r="AZ12" s="21"/>
+      <c r="AZ12" s="22"/>
     </row>
     <row r="13" ht="14.25" customHeight="1"/>
     <row r="14" ht="14.25" customHeight="1"/>
@@ -11897,7 +11897,7 @@
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="7">
         <v>1263875.0</v>
       </c>
       <c r="M16" s="19"/>
@@ -11906,7 +11906,7 @@
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="7">
         <v>4027160.0</v>
       </c>
     </row>
@@ -11914,7 +11914,7 @@
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="7">
         <v>4592187.0</v>
       </c>
     </row>
@@ -11922,7 +11922,7 @@
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="7">
         <v>5982584.0</v>
       </c>
     </row>
@@ -11930,7 +11930,7 @@
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="7">
         <v>6712276.0</v>
       </c>
     </row>
@@ -11938,7 +11938,7 @@
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="7">
         <v>2887465.0</v>
       </c>
     </row>
@@ -11946,7 +11946,7 @@
       <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="7">
         <v>1.1289086E7</v>
       </c>
     </row>
@@ -11954,7 +11954,7 @@
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="7">
         <v>6844272.0</v>
       </c>
     </row>
@@ -11962,7 +11962,7 @@
       <c r="A24" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="7">
         <v>1.5176115E7</v>
       </c>
     </row>
@@ -15182,365 +15182,365 @@
       <c r="AZ11" s="1"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="7">
         <v>28537.0</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="7">
         <v>31963.0</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="7">
         <v>35593.0</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="7">
         <v>38409.0</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="7">
         <v>41072.0</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="7">
         <v>44292.0</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="7">
         <v>47965.0</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="7">
         <v>50361.0</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="7">
         <v>53937.0</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="7">
         <v>56873.0</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12" s="8">
         <v>58098.0</v>
       </c>
-      <c r="M12" s="10">
+      <c r="M12" s="8">
         <v>58098.0</v>
       </c>
-      <c r="N12" s="9">
+      <c r="N12" s="7">
         <v>63776.0</v>
       </c>
-      <c r="O12" s="9">
+      <c r="O12" s="7">
         <v>68874.0</v>
       </c>
-      <c r="P12" s="9">
+      <c r="P12" s="7">
         <v>73028.0</v>
       </c>
-      <c r="Q12" s="9">
+      <c r="Q12" s="7">
         <v>75053.0</v>
       </c>
-      <c r="R12" s="9">
+      <c r="R12" s="7">
         <v>80085.0</v>
       </c>
-      <c r="S12" s="9">
+      <c r="S12" s="7">
         <v>83663.0</v>
       </c>
-      <c r="T12" s="9">
+      <c r="T12" s="7">
         <v>87022.0</v>
       </c>
-      <c r="U12" s="9">
+      <c r="U12" s="7">
         <v>90515.0</v>
       </c>
-      <c r="V12" s="9">
+      <c r="V12" s="7">
         <v>95060.0</v>
       </c>
-      <c r="W12" s="9">
+      <c r="W12" s="7">
         <v>100827.0</v>
       </c>
-      <c r="X12" s="9">
+      <c r="X12" s="7">
         <v>108021.0</v>
       </c>
-      <c r="Y12" s="9">
+      <c r="Y12" s="7">
         <v>114711.0</v>
       </c>
-      <c r="Z12" s="9">
+      <c r="Z12" s="7">
         <v>121510.0</v>
       </c>
-      <c r="AA12" s="9">
+      <c r="AA12" s="7">
         <v>126937.0</v>
       </c>
-      <c r="AB12" s="9">
+      <c r="AB12" s="7">
         <v>133774.0</v>
       </c>
-      <c r="AC12" s="9">
+      <c r="AC12" s="7">
         <v>143570.0</v>
       </c>
-      <c r="AD12" s="9">
+      <c r="AD12" s="7">
         <v>152390.0</v>
       </c>
-      <c r="AE12" s="9">
+      <c r="AE12" s="7">
         <v>161004.0</v>
       </c>
-      <c r="AF12" s="9">
+      <c r="AF12" s="7">
         <v>168643.0</v>
       </c>
-      <c r="AG12" s="9">
+      <c r="AG12" s="7">
         <v>178470.0</v>
       </c>
-      <c r="AH12" s="9">
+      <c r="AH12" s="7">
         <v>185497.0</v>
       </c>
-      <c r="AI12" s="9">
+      <c r="AI12" s="7">
         <v>197127.0</v>
       </c>
-      <c r="AJ12" s="9">
+      <c r="AJ12" s="7">
         <v>207530.0</v>
       </c>
-      <c r="AK12" s="9">
+      <c r="AK12" s="7">
         <v>217522.0</v>
       </c>
-      <c r="AL12" s="9">
+      <c r="AL12" s="7">
         <v>230686.0</v>
       </c>
-      <c r="AM12" s="9">
+      <c r="AM12" s="7">
         <v>245747.0</v>
       </c>
-      <c r="AN12" s="9">
+      <c r="AN12" s="7">
         <v>257541.0</v>
       </c>
-      <c r="AO12" s="9">
+      <c r="AO12" s="7">
         <v>268064.0</v>
       </c>
-      <c r="AP12" s="11">
+      <c r="AP12" s="9">
         <v>279379.0</v>
       </c>
-      <c r="AQ12" s="9">
+      <c r="AQ12" s="7">
         <v>292153.0</v>
       </c>
-      <c r="AR12" s="9">
+      <c r="AR12" s="7">
         <v>307752.0</v>
       </c>
-      <c r="AS12" s="9">
+      <c r="AS12" s="7">
         <v>324079.0</v>
       </c>
-      <c r="AT12" s="9">
+      <c r="AT12" s="7">
         <v>341336.0</v>
       </c>
-      <c r="AU12" s="9">
+      <c r="AU12" s="7">
         <v>356067.0</v>
       </c>
-      <c r="AV12" s="9">
+      <c r="AV12" s="7">
         <v>369697.0</v>
       </c>
-      <c r="AW12" s="12">
+      <c r="AW12" s="10">
         <v>386352.0</v>
       </c>
-      <c r="AX12" s="9">
+      <c r="AX12" s="7">
         <v>403018.0</v>
       </c>
-      <c r="AY12" s="12">
+      <c r="AY12" s="10">
         <v>421555.0</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="12">
         <f t="shared" ref="B13:AZ13" si="21">sum(B2:B11)</f>
         <v>28536</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="12">
         <f t="shared" si="21"/>
         <v>31965</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="12">
         <f t="shared" si="21"/>
         <v>35592</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="12">
         <f t="shared" si="21"/>
         <v>38409</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="12">
         <f t="shared" si="21"/>
         <v>41073</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="12">
         <f t="shared" si="21"/>
         <v>44293</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="12">
         <f t="shared" si="21"/>
         <v>47966</v>
       </c>
-      <c r="I13" s="14">
+      <c r="I13" s="12">
         <f t="shared" si="21"/>
         <v>50359</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="12">
         <f t="shared" si="21"/>
         <v>53939</v>
       </c>
-      <c r="K13" s="14">
+      <c r="K13" s="12">
         <f t="shared" si="21"/>
         <v>56874</v>
       </c>
-      <c r="L13" s="14">
+      <c r="L13" s="12">
         <f t="shared" si="21"/>
         <v>58097</v>
       </c>
-      <c r="M13" s="14">
+      <c r="M13" s="12">
         <f t="shared" si="21"/>
         <v>58097</v>
       </c>
-      <c r="N13" s="14">
+      <c r="N13" s="12">
         <f t="shared" si="21"/>
         <v>63775</v>
       </c>
-      <c r="O13" s="14">
+      <c r="O13" s="12">
         <f t="shared" si="21"/>
         <v>68873</v>
       </c>
-      <c r="P13" s="14">
+      <c r="P13" s="12">
         <f t="shared" si="21"/>
         <v>73029</v>
       </c>
-      <c r="Q13" s="14">
+      <c r="Q13" s="12">
         <f t="shared" si="21"/>
         <v>75054</v>
       </c>
-      <c r="R13" s="14">
+      <c r="R13" s="12">
         <f t="shared" si="21"/>
         <v>80085</v>
       </c>
-      <c r="S13" s="14">
+      <c r="S13" s="12">
         <f t="shared" si="21"/>
         <v>83664</v>
       </c>
-      <c r="T13" s="14">
+      <c r="T13" s="12">
         <f t="shared" si="21"/>
         <v>87021</v>
       </c>
-      <c r="U13" s="14">
+      <c r="U13" s="12">
         <f t="shared" si="21"/>
         <v>90515</v>
       </c>
-      <c r="V13" s="14">
+      <c r="V13" s="12">
         <f t="shared" si="21"/>
         <v>95061</v>
       </c>
-      <c r="W13" s="14">
+      <c r="W13" s="12">
         <f t="shared" si="21"/>
         <v>100827</v>
       </c>
-      <c r="X13" s="14">
+      <c r="X13" s="12">
         <f t="shared" si="21"/>
         <v>108020</v>
       </c>
-      <c r="Y13" s="14">
+      <c r="Y13" s="12">
         <f t="shared" si="21"/>
         <v>114709</v>
       </c>
-      <c r="Z13" s="14">
+      <c r="Z13" s="12">
         <f t="shared" si="21"/>
         <v>121510</v>
       </c>
-      <c r="AA13" s="14">
+      <c r="AA13" s="12">
         <f t="shared" si="21"/>
         <v>126938</v>
       </c>
-      <c r="AB13" s="14">
+      <c r="AB13" s="12">
         <f t="shared" si="21"/>
         <v>133773</v>
       </c>
-      <c r="AC13" s="14">
+      <c r="AC13" s="12">
         <f t="shared" si="21"/>
         <v>143570</v>
       </c>
-      <c r="AD13" s="14">
+      <c r="AD13" s="12">
         <f t="shared" si="21"/>
         <v>152390</v>
       </c>
-      <c r="AE13" s="14">
+      <c r="AE13" s="12">
         <f t="shared" si="21"/>
         <v>161004</v>
       </c>
-      <c r="AF13" s="14">
+      <c r="AF13" s="12">
         <f t="shared" si="21"/>
         <v>168643</v>
       </c>
-      <c r="AG13" s="14">
+      <c r="AG13" s="12">
         <f t="shared" si="21"/>
         <v>178470</v>
       </c>
-      <c r="AH13" s="14">
+      <c r="AH13" s="12">
         <f t="shared" si="21"/>
         <v>185498</v>
       </c>
-      <c r="AI13" s="14">
+      <c r="AI13" s="12">
         <f t="shared" si="21"/>
         <v>197129</v>
       </c>
-      <c r="AJ13" s="14">
+      <c r="AJ13" s="12">
         <f t="shared" si="21"/>
         <v>207531</v>
       </c>
-      <c r="AK13" s="14">
+      <c r="AK13" s="12">
         <f t="shared" si="21"/>
         <v>217522</v>
       </c>
-      <c r="AL13" s="14">
+      <c r="AL13" s="12">
         <f t="shared" si="21"/>
         <v>230685</v>
       </c>
-      <c r="AM13" s="14">
+      <c r="AM13" s="12">
         <f t="shared" si="21"/>
         <v>245746</v>
       </c>
-      <c r="AN13" s="14">
+      <c r="AN13" s="12">
         <f t="shared" si="21"/>
         <v>257541</v>
       </c>
-      <c r="AO13" s="14">
+      <c r="AO13" s="12">
         <f t="shared" si="21"/>
         <v>268064</v>
       </c>
-      <c r="AP13" s="14">
+      <c r="AP13" s="12">
         <f t="shared" si="21"/>
         <v>279379</v>
       </c>
-      <c r="AQ13" s="14">
+      <c r="AQ13" s="12">
         <f t="shared" si="21"/>
         <v>292153</v>
       </c>
-      <c r="AR13" s="14">
+      <c r="AR13" s="12">
         <f t="shared" si="21"/>
         <v>307752</v>
       </c>
-      <c r="AS13" s="14">
+      <c r="AS13" s="12">
         <f t="shared" si="21"/>
         <v>324079</v>
       </c>
-      <c r="AT13" s="14">
+      <c r="AT13" s="12">
         <f t="shared" si="21"/>
         <v>341335</v>
       </c>
-      <c r="AU13" s="14">
+      <c r="AU13" s="12">
         <f t="shared" si="21"/>
         <v>356067</v>
       </c>
-      <c r="AV13" s="14">
+      <c r="AV13" s="12">
         <f t="shared" si="21"/>
         <v>369697</v>
       </c>
-      <c r="AW13" s="14">
+      <c r="AW13" s="12">
         <f t="shared" si="21"/>
         <v>386354</v>
       </c>
-      <c r="AX13" s="14">
+      <c r="AX13" s="12">
         <f t="shared" si="21"/>
         <v>403019</v>
       </c>
-      <c r="AY13" s="14">
+      <c r="AY13" s="12">
         <f t="shared" si="21"/>
         <v>421555</v>
       </c>
-      <c r="AZ13" s="14">
+      <c r="AZ13" s="12">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -18803,354 +18803,354 @@
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="7">
         <v>28537.0</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="7">
         <v>31963.0</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="7">
         <v>35593.0</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="7">
         <v>38409.0</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="7">
         <v>41072.0</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="7">
         <v>44292.0</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="7">
         <v>47965.0</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="7">
         <v>50361.0</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="7">
         <v>53937.0</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="7">
         <v>56873.0</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12" s="8">
         <v>58098.0</v>
       </c>
-      <c r="M12" s="10">
+      <c r="M12" s="8">
         <v>58098.0</v>
       </c>
-      <c r="N12" s="9">
+      <c r="N12" s="7">
         <v>63776.0</v>
       </c>
-      <c r="O12" s="9">
+      <c r="O12" s="7">
         <v>68874.0</v>
       </c>
-      <c r="P12" s="9">
+      <c r="P12" s="7">
         <v>73028.0</v>
       </c>
-      <c r="Q12" s="9">
+      <c r="Q12" s="7">
         <v>75053.0</v>
       </c>
-      <c r="R12" s="9">
+      <c r="R12" s="7">
         <v>80085.0</v>
       </c>
-      <c r="S12" s="9">
+      <c r="S12" s="7">
         <v>83663.0</v>
       </c>
-      <c r="T12" s="9">
+      <c r="T12" s="7">
         <v>87022.0</v>
       </c>
-      <c r="U12" s="9">
+      <c r="U12" s="7">
         <v>90515.0</v>
       </c>
-      <c r="V12" s="9">
+      <c r="V12" s="7">
         <v>95060.0</v>
       </c>
-      <c r="W12" s="9">
+      <c r="W12" s="7">
         <v>100827.0</v>
       </c>
-      <c r="X12" s="9">
+      <c r="X12" s="7">
         <v>108021.0</v>
       </c>
-      <c r="Y12" s="9">
+      <c r="Y12" s="7">
         <v>114711.0</v>
       </c>
-      <c r="Z12" s="9">
+      <c r="Z12" s="7">
         <v>121510.0</v>
       </c>
-      <c r="AA12" s="9">
+      <c r="AA12" s="7">
         <v>126937.0</v>
       </c>
-      <c r="AB12" s="9">
+      <c r="AB12" s="7">
         <v>133774.0</v>
       </c>
-      <c r="AC12" s="9">
+      <c r="AC12" s="7">
         <v>143570.0</v>
       </c>
-      <c r="AD12" s="9">
+      <c r="AD12" s="7">
         <v>152390.0</v>
       </c>
-      <c r="AE12" s="9">
+      <c r="AE12" s="7">
         <v>161004.0</v>
       </c>
-      <c r="AF12" s="9">
+      <c r="AF12" s="7">
         <v>168643.0</v>
       </c>
-      <c r="AG12" s="9">
+      <c r="AG12" s="7">
         <v>178470.0</v>
       </c>
-      <c r="AH12" s="9">
+      <c r="AH12" s="7">
         <v>185497.0</v>
       </c>
-      <c r="AI12" s="9">
+      <c r="AI12" s="7">
         <v>197127.0</v>
       </c>
-      <c r="AJ12" s="9">
+      <c r="AJ12" s="7">
         <v>207530.0</v>
       </c>
-      <c r="AK12" s="9">
+      <c r="AK12" s="7">
         <v>217522.0</v>
       </c>
-      <c r="AL12" s="9">
+      <c r="AL12" s="7">
         <v>230686.0</v>
       </c>
-      <c r="AM12" s="9">
+      <c r="AM12" s="7">
         <v>245747.0</v>
       </c>
-      <c r="AN12" s="9">
+      <c r="AN12" s="7">
         <v>257541.0</v>
       </c>
-      <c r="AO12" s="9">
+      <c r="AO12" s="7">
         <v>268064.0</v>
       </c>
-      <c r="AP12" s="11">
+      <c r="AP12" s="9">
         <v>279379.0</v>
       </c>
-      <c r="AQ12" s="9">
+      <c r="AQ12" s="7">
         <v>292153.0</v>
       </c>
-      <c r="AR12" s="9">
+      <c r="AR12" s="7">
         <v>307752.0</v>
       </c>
-      <c r="AS12" s="9">
+      <c r="AS12" s="7">
         <v>324079.0</v>
       </c>
-      <c r="AT12" s="9">
+      <c r="AT12" s="7">
         <v>341336.0</v>
       </c>
-      <c r="AU12" s="9">
+      <c r="AU12" s="7">
         <v>356067.0</v>
       </c>
-      <c r="AV12" s="9">
+      <c r="AV12" s="7">
         <v>369697.0</v>
       </c>
-      <c r="AW12" s="9">
+      <c r="AW12" s="7">
         <v>386352.0</v>
       </c>
-      <c r="AX12" s="9">
+      <c r="AX12" s="7">
         <v>403018.0</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="12">
         <f t="shared" ref="B13:AV13" si="21">sum(B2:B11)</f>
         <v>1916</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="12">
         <f t="shared" si="21"/>
         <v>2146</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="12">
         <f t="shared" si="21"/>
         <v>2390</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="12">
         <f t="shared" si="21"/>
         <v>2579</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="12">
         <f t="shared" si="21"/>
         <v>2757</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="12">
         <f t="shared" si="21"/>
         <v>2973</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="12">
         <f t="shared" si="21"/>
         <v>3219</v>
       </c>
-      <c r="I13" s="14">
+      <c r="I13" s="12">
         <f t="shared" si="21"/>
         <v>3379</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="12">
         <f t="shared" si="21"/>
         <v>3620</v>
       </c>
-      <c r="K13" s="14">
+      <c r="K13" s="12">
         <f t="shared" si="21"/>
         <v>3817</v>
       </c>
-      <c r="L13" s="14">
+      <c r="L13" s="12">
         <f t="shared" si="21"/>
         <v>3899</v>
       </c>
-      <c r="M13" s="14">
+      <c r="M13" s="12">
         <f t="shared" si="21"/>
         <v>3899</v>
       </c>
-      <c r="N13" s="14">
+      <c r="N13" s="12">
         <f t="shared" si="21"/>
         <v>4279</v>
       </c>
-      <c r="O13" s="14">
+      <c r="O13" s="12">
         <f t="shared" si="21"/>
         <v>4621</v>
       </c>
-      <c r="P13" s="14">
+      <c r="P13" s="12">
         <f t="shared" si="21"/>
         <v>4902</v>
       </c>
-      <c r="Q13" s="14">
+      <c r="Q13" s="12">
         <f t="shared" si="21"/>
         <v>5038</v>
       </c>
-      <c r="R13" s="14">
+      <c r="R13" s="12">
         <f t="shared" si="21"/>
         <v>5375</v>
       </c>
-      <c r="S13" s="14">
+      <c r="S13" s="12">
         <f t="shared" si="21"/>
         <v>5615</v>
       </c>
-      <c r="T13" s="14">
+      <c r="T13" s="12">
         <f t="shared" si="21"/>
         <v>5842</v>
       </c>
-      <c r="U13" s="14">
+      <c r="U13" s="12">
         <f t="shared" si="21"/>
         <v>6077</v>
       </c>
-      <c r="V13" s="14">
+      <c r="V13" s="12">
         <f t="shared" si="21"/>
         <v>6382</v>
       </c>
-      <c r="W13" s="14">
+      <c r="W13" s="12">
         <f t="shared" si="21"/>
         <v>6768</v>
       </c>
-      <c r="X13" s="14">
+      <c r="X13" s="12">
         <f t="shared" si="21"/>
         <v>7251</v>
       </c>
-      <c r="Y13" s="14">
+      <c r="Y13" s="12">
         <f t="shared" si="21"/>
         <v>7699</v>
       </c>
-      <c r="Z13" s="14">
+      <c r="Z13" s="12">
         <f t="shared" si="21"/>
         <v>8156</v>
       </c>
-      <c r="AA13" s="14">
+      <c r="AA13" s="12">
         <f t="shared" si="21"/>
         <v>8521</v>
       </c>
-      <c r="AB13" s="14">
+      <c r="AB13" s="12">
         <f t="shared" si="21"/>
         <v>8979</v>
       </c>
-      <c r="AC13" s="14">
+      <c r="AC13" s="12">
         <f t="shared" si="21"/>
         <v>9639</v>
       </c>
-      <c r="AD13" s="14">
+      <c r="AD13" s="12">
         <f t="shared" si="21"/>
         <v>10230</v>
       </c>
-      <c r="AE13" s="14">
+      <c r="AE13" s="12">
         <f t="shared" si="21"/>
         <v>10808</v>
       </c>
-      <c r="AF13" s="14">
+      <c r="AF13" s="12">
         <f t="shared" si="21"/>
         <v>11321</v>
       </c>
-      <c r="AG13" s="14">
+      <c r="AG13" s="12">
         <f t="shared" si="21"/>
         <v>11981</v>
       </c>
-      <c r="AH13" s="14">
+      <c r="AH13" s="12">
         <f t="shared" si="21"/>
         <v>12451</v>
       </c>
-      <c r="AI13" s="14">
+      <c r="AI13" s="12">
         <f t="shared" si="21"/>
         <v>13234</v>
       </c>
-      <c r="AJ13" s="14">
+      <c r="AJ13" s="12">
         <f t="shared" si="21"/>
         <v>13931</v>
       </c>
-      <c r="AK13" s="14">
+      <c r="AK13" s="12">
         <f t="shared" si="21"/>
         <v>14603</v>
       </c>
-      <c r="AL13" s="14">
+      <c r="AL13" s="12">
         <f t="shared" si="21"/>
         <v>15486</v>
       </c>
-      <c r="AM13" s="14">
+      <c r="AM13" s="12">
         <f t="shared" si="21"/>
         <v>16496</v>
       </c>
-      <c r="AN13" s="14">
+      <c r="AN13" s="12">
         <f t="shared" si="21"/>
         <v>17290</v>
       </c>
-      <c r="AO13" s="14">
+      <c r="AO13" s="12">
         <f t="shared" si="21"/>
         <v>17996</v>
       </c>
-      <c r="AP13" s="14">
+      <c r="AP13" s="12">
         <f t="shared" si="21"/>
         <v>18754</v>
       </c>
-      <c r="AQ13" s="14">
+      <c r="AQ13" s="12">
         <f t="shared" si="21"/>
         <v>19610</v>
       </c>
-      <c r="AR13" s="14">
+      <c r="AR13" s="12">
         <f t="shared" si="21"/>
         <v>20659</v>
       </c>
-      <c r="AS13" s="14">
+      <c r="AS13" s="12">
         <f t="shared" si="21"/>
         <v>21754</v>
       </c>
-      <c r="AT13" s="14">
+      <c r="AT13" s="12">
         <f t="shared" si="21"/>
         <v>22911</v>
       </c>
-      <c r="AU13" s="14">
+      <c r="AU13" s="12">
         <f t="shared" si="21"/>
         <v>23902</v>
       </c>
-      <c r="AV13" s="14">
+      <c r="AV13" s="12">
         <f t="shared" si="21"/>
         <v>24818</v>
       </c>
-      <c r="AW13" s="14">
+      <c r="AW13" s="12">
         <f>sum(AW2:AW12)</f>
         <v>412287</v>
       </c>
-      <c r="AX13" s="14">
+      <c r="AX13" s="12">
         <f>sum(AX2:AX11)</f>
         <v>27054</v>
       </c>
@@ -19239,7 +19239,7 @@
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="7">
         <v>1263875.0</v>
       </c>
     </row>
@@ -19247,7 +19247,7 @@
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="7">
         <v>4027160.0</v>
       </c>
     </row>
@@ -19255,7 +19255,7 @@
       <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="7">
         <v>4592187.0</v>
       </c>
     </row>
@@ -19263,7 +19263,7 @@
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="7">
         <v>5982584.0</v>
       </c>
     </row>
@@ -19271,7 +19271,7 @@
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="7">
         <v>6712276.0</v>
       </c>
     </row>
@@ -19279,7 +19279,7 @@
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="7">
         <v>2887465.0</v>
       </c>
     </row>
@@ -19287,7 +19287,7 @@
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="7">
         <v>1.1289086E7</v>
       </c>
     </row>
@@ -19295,7 +19295,7 @@
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="7">
         <v>6844272.0</v>
       </c>
     </row>
@@ -19303,7 +19303,7 @@
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="7">
         <v>1.5176115E7</v>
       </c>
     </row>
@@ -23184,19 +23184,19 @@
       <c r="AT1" s="2">
         <v>43961.0</v>
       </c>
-      <c r="AU1" s="7">
+      <c r="AU1" s="13">
         <v>43962.0</v>
       </c>
       <c r="AV1" s="2">
         <v>43963.0</v>
       </c>
-      <c r="AW1" s="7">
+      <c r="AW1" s="13">
         <v>43964.0</v>
       </c>
       <c r="AX1" s="2">
         <v>43965.0</v>
       </c>
-      <c r="AY1" s="8">
+      <c r="AY1" s="14">
         <v>43966.0</v>
       </c>
       <c r="AZ1" s="2">
@@ -29220,7 +29220,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7">
+      <c r="B1" s="13">
         <v>43965.0</v>
       </c>
       <c r="C1" s="2">
@@ -38777,7 +38777,7 @@
     <row r="12" ht="14.25" customHeight="1"/>
     <row r="13" ht="14.25" customHeight="1"/>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="M14" s="22" t="s">
+      <c r="M14" s="21" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated data from 25-05-2020
</commit_message>
<xml_diff>
--- a/Data/Covid2019/SA_data_archive/Province_database.xlsx
+++ b/Data/Covid2019/SA_data_archive/Province_database.xlsx
@@ -21,7 +21,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId17" roundtripDataSignature="AMtx7miAe47NojVyglIUs3l8cFtAl+2APQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId17" roundtripDataSignature="AMtx7mifJAaelrZ+SHOXETEz1qYyaLp4hw=="/>
     </ext>
   </extLst>
 </workbook>
@@ -497,14 +497,14 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="15" xfId="0" applyFill="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="15" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="15" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="15" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -591,12 +591,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Testing!$B$1:$BI$1</c:f>
+              <c:f>Testing!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Testing!$B$2:$BI$2</c:f>
+              <c:f>Testing!$B$2:$BJ$2</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -615,12 +615,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Testing!$B$1:$BI$1</c:f>
+              <c:f>Testing!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Testing!$B$3:$BI$3</c:f>
+              <c:f>Testing!$B$3:$BJ$3</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -639,12 +639,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Testing!$B$1:$BI$1</c:f>
+              <c:f>Testing!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Testing!$B$4:$BI$4</c:f>
+              <c:f>Testing!$B$4:$BJ$4</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -663,12 +663,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Testing!$B$1:$BI$1</c:f>
+              <c:f>Testing!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Testing!$B$5:$BI$5</c:f>
+              <c:f>Testing!$B$5:$BJ$5</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -687,12 +687,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Testing!$B$1:$BI$1</c:f>
+              <c:f>Testing!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Testing!$B$6:$BI$6</c:f>
+              <c:f>Testing!$B$6:$BJ$6</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -711,12 +711,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Testing!$B$1:$BI$1</c:f>
+              <c:f>Testing!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Testing!$B$7:$BI$7</c:f>
+              <c:f>Testing!$B$7:$BJ$7</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -737,12 +737,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Testing!$B$1:$BI$1</c:f>
+              <c:f>Testing!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Testing!$B$8:$BI$8</c:f>
+              <c:f>Testing!$B$8:$BJ$8</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -763,12 +763,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Testing!$B$1:$BI$1</c:f>
+              <c:f>Testing!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Testing!$B$9:$BI$9</c:f>
+              <c:f>Testing!$B$9:$BJ$9</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -789,12 +789,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Testing!$B$1:$BI$1</c:f>
+              <c:f>Testing!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Testing!$B$10:$BI$10</c:f>
+              <c:f>Testing!$B$10:$BJ$10</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -815,21 +815,21 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Testing!$B$1:$BI$1</c:f>
+              <c:f>Testing!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Testing!$B$11:$BI$11</c:f>
+              <c:f>Testing!$B$11:$BJ$11</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1254259320"/>
-        <c:axId val="74764956"/>
+        <c:axId val="2011706118"/>
+        <c:axId val="1808207017"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1254259320"/>
+        <c:axId val="2011706118"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -874,10 +874,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74764956"/>
+        <c:crossAx val="1808207017"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74764956"/>
+        <c:axId val="1808207017"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -946,7 +946,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1254259320"/>
+        <c:crossAx val="2011706118"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1013,12 +1013,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Death Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Death Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Death Rate'!$B$2:$BI$2</c:f>
+              <c:f>'Death Rate'!$B$2:$BJ$2</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
@@ -1036,12 +1036,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Death Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Death Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Death Rate'!$B$3:$BI$3</c:f>
+              <c:f>'Death Rate'!$B$3:$BJ$3</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
@@ -1059,12 +1059,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Death Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Death Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Death Rate'!$B$4:$BI$4</c:f>
+              <c:f>'Death Rate'!$B$4:$BJ$4</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
@@ -1082,12 +1082,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Death Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Death Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Death Rate'!$B$5:$BI$5</c:f>
+              <c:f>'Death Rate'!$B$5:$BJ$5</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
@@ -1105,12 +1105,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Death Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Death Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Death Rate'!$B$6:$BI$6</c:f>
+              <c:f>'Death Rate'!$B$6:$BJ$6</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
@@ -1128,12 +1128,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Death Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Death Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Death Rate'!$B$7:$BI$7</c:f>
+              <c:f>'Death Rate'!$B$7:$BJ$7</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
@@ -1151,12 +1151,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Death Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Death Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Death Rate'!$B$8:$BI$8</c:f>
+              <c:f>'Death Rate'!$B$8:$BJ$8</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
@@ -1174,12 +1174,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Death Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Death Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Death Rate'!$B$9:$BI$9</c:f>
+              <c:f>'Death Rate'!$B$9:$BJ$9</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
@@ -1197,21 +1197,21 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Death Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Death Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Death Rate'!$B$10:$BI$10</c:f>
+              <c:f>'Death Rate'!$B$10:$BJ$10</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="451768174"/>
-        <c:axId val="1940662701"/>
+        <c:axId val="159783326"/>
+        <c:axId val="399986363"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="451768174"/>
+        <c:axId val="159783326"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1256,10 +1256,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1940662701"/>
+        <c:crossAx val="399986363"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1940662701"/>
+        <c:axId val="399986363"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1328,7 +1328,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="451768174"/>
+        <c:crossAx val="159783326"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1399,18 +1399,18 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>'Infection Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Infection Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Infection Rate'!$B$2:$BI$2</c:f>
+              <c:f>'Infection Rate'!$B$2:$BJ$2</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="772357998"/>
-        <c:axId val="1126848013"/>
+        <c:axId val="739430901"/>
+        <c:axId val="347329133"/>
       </c:barChart>
       <c:lineChart>
         <c:ser>
@@ -1426,12 +1426,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Infection Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Infection Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Infection Rate'!$B$3:$BI$3</c:f>
+              <c:f>'Infection Rate'!$B$3:$BJ$3</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1449,12 +1449,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Infection Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Infection Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Infection Rate'!$B$4:$BI$4</c:f>
+              <c:f>'Infection Rate'!$B$4:$BJ$4</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1472,12 +1472,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Infection Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Infection Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Infection Rate'!$B$5:$BI$5</c:f>
+              <c:f>'Infection Rate'!$B$5:$BJ$5</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1495,12 +1495,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Infection Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Infection Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Infection Rate'!$B$6:$BI$6</c:f>
+              <c:f>'Infection Rate'!$B$6:$BJ$6</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1518,12 +1518,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Infection Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Infection Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Infection Rate'!$B$7:$BI$7</c:f>
+              <c:f>'Infection Rate'!$B$7:$BJ$7</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1541,12 +1541,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Infection Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Infection Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Infection Rate'!$B$8:$BI$8</c:f>
+              <c:f>'Infection Rate'!$B$8:$BJ$8</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1564,12 +1564,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Infection Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Infection Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Infection Rate'!$B$9:$BI$9</c:f>
+              <c:f>'Infection Rate'!$B$9:$BJ$9</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1587,12 +1587,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Infection Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Infection Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Infection Rate'!$B$10:$BI$10</c:f>
+              <c:f>'Infection Rate'!$B$10:$BJ$10</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1610,21 +1610,21 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Infection Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Infection Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Infection Rate'!$B$11:$BI$11</c:f>
+              <c:f>'Infection Rate'!$B$11:$BJ$11</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="772357998"/>
-        <c:axId val="1126848013"/>
+        <c:axId val="739430901"/>
+        <c:axId val="347329133"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="772357998"/>
+        <c:axId val="739430901"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1669,10 +1669,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1126848013"/>
+        <c:crossAx val="347329133"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1126848013"/>
+        <c:axId val="347329133"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1741,7 +1741,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="772357998"/>
+        <c:crossAx val="739430901"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1812,12 +1812,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>'Testing per Capita'!$B$1:$BI$1</c:f>
+              <c:f>'Testing per Capita'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Testing per Capita'!$B$2:$BI$2</c:f>
+              <c:f>'Testing per Capita'!$B$2:$BJ$2</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -1836,12 +1836,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>'Testing per Capita'!$B$1:$BI$1</c:f>
+              <c:f>'Testing per Capita'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Testing per Capita'!$B$3:$BI$3</c:f>
+              <c:f>'Testing per Capita'!$B$3:$BJ$3</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -1860,12 +1860,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>'Testing per Capita'!$B$1:$BI$1</c:f>
+              <c:f>'Testing per Capita'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Testing per Capita'!$B$4:$BI$4</c:f>
+              <c:f>'Testing per Capita'!$B$4:$BJ$4</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -1884,12 +1884,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>'Testing per Capita'!$B$1:$BI$1</c:f>
+              <c:f>'Testing per Capita'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Testing per Capita'!$B$5:$BI$5</c:f>
+              <c:f>'Testing per Capita'!$B$5:$BJ$5</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -1908,12 +1908,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>'Testing per Capita'!$B$1:$BI$1</c:f>
+              <c:f>'Testing per Capita'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Testing per Capita'!$B$6:$BI$6</c:f>
+              <c:f>'Testing per Capita'!$B$6:$BJ$6</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -1932,12 +1932,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>'Testing per Capita'!$B$1:$BI$1</c:f>
+              <c:f>'Testing per Capita'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Testing per Capita'!$B$7:$BI$7</c:f>
+              <c:f>'Testing per Capita'!$B$7:$BJ$7</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -1958,12 +1958,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>'Testing per Capita'!$B$1:$BI$1</c:f>
+              <c:f>'Testing per Capita'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Testing per Capita'!$B$8:$BI$8</c:f>
+              <c:f>'Testing per Capita'!$B$8:$BJ$8</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -1984,12 +1984,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>'Testing per Capita'!$B$1:$BI$1</c:f>
+              <c:f>'Testing per Capita'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Testing per Capita'!$B$9:$BI$9</c:f>
+              <c:f>'Testing per Capita'!$B$9:$BJ$9</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -2010,12 +2010,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>'Testing per Capita'!$B$1:$BI$1</c:f>
+              <c:f>'Testing per Capita'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Testing per Capita'!$B$10:$BI$10</c:f>
+              <c:f>'Testing per Capita'!$B$10:$BJ$10</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -2029,21 +2029,21 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'Testing per Capita'!$B$1:$BI$1</c:f>
+              <c:f>'Testing per Capita'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Testing per Capita'!$B$11:$BI$11</c:f>
+              <c:f>'Testing per Capita'!$B$11:$BJ$11</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="633444515"/>
-        <c:axId val="253850682"/>
+        <c:axId val="172858052"/>
+        <c:axId val="1755159097"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="633444515"/>
+        <c:axId val="172858052"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2088,10 +2088,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="253850682"/>
+        <c:crossAx val="1755159097"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="253850682"/>
+        <c:axId val="1755159097"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2160,7 +2160,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="633444515"/>
+        <c:crossAx val="172858052"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2204,7 +2204,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t>Daily tracking of closed cases (Recoveries + deaths) </a:t>
+              <a:t>Daily tracking of closed cases (Recoveries minus deaths) </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2231,12 +2231,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>'Daily tracking'!$B$1:$BI$1</c:f>
+              <c:f>'Daily tracking'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Daily tracking'!$B$2:$BI$2</c:f>
+              <c:f>'Daily tracking'!$B$2:$BJ$2</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -2255,12 +2255,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>'Daily tracking'!$B$1:$BI$1</c:f>
+              <c:f>'Daily tracking'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Daily tracking'!$B$3:$BI$3</c:f>
+              <c:f>'Daily tracking'!$B$3:$BJ$3</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -2279,12 +2279,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>'Daily tracking'!$B$1:$BI$1</c:f>
+              <c:f>'Daily tracking'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Daily tracking'!$B$4:$BI$4</c:f>
+              <c:f>'Daily tracking'!$B$4:$BJ$4</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -2303,12 +2303,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>'Daily tracking'!$B$1:$BI$1</c:f>
+              <c:f>'Daily tracking'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Daily tracking'!$B$5:$BI$5</c:f>
+              <c:f>'Daily tracking'!$B$5:$BJ$5</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -2327,12 +2327,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>'Daily tracking'!$B$1:$BI$1</c:f>
+              <c:f>'Daily tracking'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Daily tracking'!$B$6:$BI$6</c:f>
+              <c:f>'Daily tracking'!$B$6:$BJ$6</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -2351,12 +2351,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>'Daily tracking'!$B$1:$BI$1</c:f>
+              <c:f>'Daily tracking'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Daily tracking'!$B$7:$BI$7</c:f>
+              <c:f>'Daily tracking'!$B$7:$BJ$7</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -2377,12 +2377,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>'Daily tracking'!$B$1:$BI$1</c:f>
+              <c:f>'Daily tracking'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Daily tracking'!$B$8:$BI$8</c:f>
+              <c:f>'Daily tracking'!$B$8:$BJ$8</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -2403,12 +2403,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>'Daily tracking'!$B$1:$BI$1</c:f>
+              <c:f>'Daily tracking'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Daily tracking'!$B$9:$BI$9</c:f>
+              <c:f>'Daily tracking'!$B$9:$BJ$9</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -2429,12 +2429,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>'Daily tracking'!$B$1:$BI$1</c:f>
+              <c:f>'Daily tracking'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Daily tracking'!$B$10:$BI$10</c:f>
+              <c:f>'Daily tracking'!$B$10:$BJ$10</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -2448,12 +2448,12 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'Daily tracking'!$B$1:$BI$1</c:f>
+              <c:f>'Daily tracking'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Daily tracking'!$B$11:$BI$11</c:f>
+              <c:f>'Daily tracking'!$B$11:$BJ$11</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -2467,21 +2467,21 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'Daily tracking'!$B$1:$BI$1</c:f>
+              <c:f>'Daily tracking'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Daily tracking'!$B$12:$BI$12</c:f>
+              <c:f>'Daily tracking'!$B$12:$BJ$12</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="110996375"/>
-        <c:axId val="1465199055"/>
+        <c:axId val="794624464"/>
+        <c:axId val="1583439267"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="110996375"/>
+        <c:axId val="794624464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2526,10 +2526,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1465199055"/>
+        <c:crossAx val="1583439267"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1465199055"/>
+        <c:axId val="1583439267"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2598,7 +2598,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110996375"/>
+        <c:crossAx val="794624464"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2669,18 +2669,18 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Active!$B$1:$BI$1</c:f>
+              <c:f>Active!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Active!$B$2:$BI$2</c:f>
+              <c:f>Active!$B$2:$BJ$2</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1497802011"/>
-        <c:axId val="1109247780"/>
+        <c:axId val="1693947647"/>
+        <c:axId val="236895073"/>
       </c:barChart>
       <c:lineChart>
         <c:ser>
@@ -2696,12 +2696,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Active!$B$1:$BI$1</c:f>
+              <c:f>Active!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Active!$B$3:$BI$3</c:f>
+              <c:f>Active!$B$3:$BJ$3</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -2719,12 +2719,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Active!$B$1:$BI$1</c:f>
+              <c:f>Active!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Active!$B$4:$BI$4</c:f>
+              <c:f>Active!$B$4:$BJ$4</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -2742,12 +2742,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Active!$B$1:$BI$1</c:f>
+              <c:f>Active!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Active!$B$5:$BI$5</c:f>
+              <c:f>Active!$B$5:$BJ$5</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -2765,12 +2765,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Active!$B$1:$BI$1</c:f>
+              <c:f>Active!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Active!$B$6:$BI$6</c:f>
+              <c:f>Active!$B$6:$BJ$6</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -2788,12 +2788,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Active!$B$1:$BI$1</c:f>
+              <c:f>Active!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Active!$B$7:$BI$7</c:f>
+              <c:f>Active!$B$7:$BJ$7</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -2811,12 +2811,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Active!$B$1:$BI$1</c:f>
+              <c:f>Active!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Active!$B$8:$BI$8</c:f>
+              <c:f>Active!$B$8:$BJ$8</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -2834,12 +2834,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Active!$B$1:$BI$1</c:f>
+              <c:f>Active!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Active!$B$9:$BI$9</c:f>
+              <c:f>Active!$B$9:$BJ$9</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -2857,12 +2857,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Active!$B$1:$BI$1</c:f>
+              <c:f>Active!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Active!$B$10:$BI$10</c:f>
+              <c:f>Active!$B$10:$BJ$10</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -2880,21 +2880,21 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Active!$B$1:$BI$1</c:f>
+              <c:f>Active!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Active!$B$11:$BI$11</c:f>
+              <c:f>Active!$B$11:$BJ$11</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1497802011"/>
-        <c:axId val="1109247780"/>
+        <c:axId val="1693947647"/>
+        <c:axId val="236895073"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1497802011"/>
+        <c:axId val="1693947647"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2939,10 +2939,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1109247780"/>
+        <c:crossAx val="236895073"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1109247780"/>
+        <c:axId val="236895073"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3011,7 +3011,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1497802011"/>
+        <c:crossAx val="1693947647"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3092,8 +3092,8 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1575992394"/>
-        <c:axId val="911282368"/>
+        <c:axId val="343129489"/>
+        <c:axId val="663930795"/>
       </c:barChart>
       <c:lineChart>
         <c:ser>
@@ -3303,11 +3303,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1575992394"/>
-        <c:axId val="911282368"/>
+        <c:axId val="343129489"/>
+        <c:axId val="663930795"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1575992394"/>
+        <c:axId val="343129489"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3352,10 +3352,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="911282368"/>
+        <c:crossAx val="663930795"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="911282368"/>
+        <c:axId val="663930795"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3424,7 +3424,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1575992394"/>
+        <c:crossAx val="343129489"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3513,8 +3513,8 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="769001575"/>
-        <c:axId val="712512542"/>
+        <c:axId val="2009669802"/>
+        <c:axId val="825726223"/>
       </c:barChart>
       <c:lineChart>
         <c:ser>
@@ -3724,11 +3724,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="769001575"/>
-        <c:axId val="712512542"/>
+        <c:axId val="2009669802"/>
+        <c:axId val="825726223"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="769001575"/>
+        <c:axId val="2009669802"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3773,10 +3773,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="712512542"/>
+        <c:crossAx val="825726223"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="712512542"/>
+        <c:axId val="825726223"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3845,7 +3845,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="769001575"/>
+        <c:crossAx val="2009669802"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3995,11 +3995,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1274589665"/>
-        <c:axId val="152356155"/>
+        <c:axId val="1426060239"/>
+        <c:axId val="1487127247"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1274589665"/>
+        <c:axId val="1426060239"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4044,10 +4044,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152356155"/>
+        <c:crossAx val="1487127247"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152356155"/>
+        <c:axId val="1487127247"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4116,7 +4116,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1274589665"/>
+        <c:crossAx val="1426060239"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4335,11 +4335,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2130024587"/>
-        <c:axId val="575674271"/>
+        <c:axId val="1427831958"/>
+        <c:axId val="185130882"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2130024587"/>
+        <c:axId val="1427831958"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4384,10 +4384,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="575674271"/>
+        <c:crossAx val="185130882"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="575674271"/>
+        <c:axId val="185130882"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4456,7 +4456,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2130024587"/>
+        <c:crossAx val="1427831958"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4523,12 +4523,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Recovery Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Recovery Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Recovery Rate'!$B$3:$BI$3</c:f>
+              <c:f>'Recovery Rate'!$B$3:$BJ$3</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
@@ -4546,12 +4546,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Recovery Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Recovery Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Recovery Rate'!$B$4:$BI$4</c:f>
+              <c:f>'Recovery Rate'!$B$4:$BJ$4</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
@@ -4569,12 +4569,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Recovery Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Recovery Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Recovery Rate'!$B$5:$BI$5</c:f>
+              <c:f>'Recovery Rate'!$B$5:$BJ$5</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
@@ -4592,12 +4592,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Recovery Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Recovery Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Recovery Rate'!$B$6:$BI$6</c:f>
+              <c:f>'Recovery Rate'!$B$6:$BJ$6</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
@@ -4615,12 +4615,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Recovery Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Recovery Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Recovery Rate'!$B$7:$BI$7</c:f>
+              <c:f>'Recovery Rate'!$B$7:$BJ$7</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
@@ -4638,12 +4638,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Recovery Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Recovery Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Recovery Rate'!$B$8:$BI$8</c:f>
+              <c:f>'Recovery Rate'!$B$8:$BJ$8</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
@@ -4661,12 +4661,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Recovery Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Recovery Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Recovery Rate'!$B$9:$BI$9</c:f>
+              <c:f>'Recovery Rate'!$B$9:$BJ$9</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
@@ -4684,12 +4684,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Recovery Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Recovery Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Recovery Rate'!$B$10:$BI$10</c:f>
+              <c:f>'Recovery Rate'!$B$10:$BJ$10</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
@@ -4707,21 +4707,21 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Recovery Rate'!$B$1:$BI$1</c:f>
+              <c:f>'Recovery Rate'!$B$1:$BJ$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Recovery Rate'!$B$11:$BI$11</c:f>
+              <c:f>'Recovery Rate'!$B$11:$BJ$11</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="583474064"/>
-        <c:axId val="1395861590"/>
+        <c:axId val="467419886"/>
+        <c:axId val="1503816058"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="583474064"/>
+        <c:axId val="467419886"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4766,10 +4766,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1395861590"/>
+        <c:crossAx val="1503816058"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1395861590"/>
+        <c:axId val="1503816058"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4838,7 +4838,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="583474064"/>
+        <c:crossAx val="467419886"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -4979,7 +4979,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="613342381" name="Chart 1" title="Chart"/>
+        <xdr:cNvPr id="613342381" name="Chart 2" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5009,7 +5009,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="123848420" name="Chart 2" title="Chart"/>
+        <xdr:cNvPr id="123848420" name="Chart 1" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5417,7 +5417,7 @@
     <col customWidth="1" min="7" max="15" width="7.13"/>
     <col customWidth="1" min="16" max="36" width="8.0"/>
     <col customWidth="1" min="37" max="43" width="7.63"/>
-    <col customWidth="1" min="44" max="61" width="9.88"/>
+    <col customWidth="1" min="44" max="62" width="9.88"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -5595,15 +5595,18 @@
       <c r="BF1" s="2">
         <v>43973.0</v>
       </c>
-      <c r="BG1" s="3">
+      <c r="BG1" s="2">
         <v>43974.0</v>
       </c>
-      <c r="BH1" s="3">
+      <c r="BH1" s="2">
         <v>43975.0</v>
       </c>
-      <c r="BI1" s="2">
+      <c r="BI1" s="3">
+        <v>43976.0</v>
+      </c>
+      <c r="BJ1" s="2">
         <f>today()</f>
-        <v>43976</v>
+        <v>43977</v>
       </c>
     </row>
     <row r="2" ht="14.25" hidden="1" customHeight="1">
@@ -5764,6 +5767,7 @@
       <c r="BG2" s="4"/>
       <c r="BH2" s="4"/>
       <c r="BI2" s="4"/>
+      <c r="BJ2" s="4"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="1" t="s">
@@ -5946,7 +5950,10 @@
       <c r="BH3" s="4">
         <v>40.0</v>
       </c>
-      <c r="BI3" s="4"/>
+      <c r="BI3" s="4">
+        <v>45.0</v>
+      </c>
+      <c r="BJ3" s="4"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="1" t="s">
@@ -6129,7 +6136,10 @@
       <c r="BH4" s="4">
         <v>94.0</v>
       </c>
-      <c r="BI4" s="4"/>
+      <c r="BI4" s="4">
+        <v>109.0</v>
+      </c>
+      <c r="BJ4" s="4"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="1" t="s">
@@ -6312,7 +6322,10 @@
       <c r="BH5" s="4">
         <v>101.0</v>
       </c>
-      <c r="BI5" s="4"/>
+      <c r="BI5" s="4">
+        <v>102.0</v>
+      </c>
+      <c r="BJ5" s="4"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="1" t="s">
@@ -6495,7 +6508,10 @@
       <c r="BH6" s="4">
         <v>128.0</v>
       </c>
-      <c r="BI6" s="4"/>
+      <c r="BI6" s="4">
+        <v>132.0</v>
+      </c>
+      <c r="BJ6" s="4"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="1" t="s">
@@ -6678,7 +6694,10 @@
       <c r="BH7" s="4">
         <v>2690.0</v>
       </c>
-      <c r="BI7" s="4"/>
+      <c r="BI7" s="4">
+        <v>2748.0</v>
+      </c>
+      <c r="BJ7" s="4"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="1" t="s">
@@ -6861,7 +6880,10 @@
       <c r="BH8" s="4">
         <v>202.0</v>
       </c>
-      <c r="BI8" s="4"/>
+      <c r="BI8" s="4">
+        <v>208.0</v>
+      </c>
+      <c r="BJ8" s="4"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="1" t="s">
@@ -7044,7 +7066,10 @@
       <c r="BH9" s="4">
         <v>1815.0</v>
       </c>
-      <c r="BI9" s="4"/>
+      <c r="BI9" s="4">
+        <v>1882.0</v>
+      </c>
+      <c r="BJ9" s="4"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="1" t="s">
@@ -7227,7 +7252,10 @@
       <c r="BH10" s="4">
         <v>14740.0</v>
       </c>
-      <c r="BI10" s="4"/>
+      <c r="BI10" s="4">
+        <v>15396.0</v>
+      </c>
+      <c r="BJ10" s="4"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="1" t="s">
@@ -7410,7 +7438,10 @@
       <c r="BH11" s="4">
         <v>2773.0</v>
       </c>
-      <c r="BI11" s="4"/>
+      <c r="BI11" s="4">
+        <v>2993.0</v>
+      </c>
+      <c r="BJ11" s="4"/>
     </row>
     <row r="12" ht="14.25" customHeight="1"/>
     <row r="13" ht="14.25" customHeight="1"/>
@@ -8424,7 +8455,7 @@
     <col customWidth="1" min="7" max="15" width="7.13"/>
     <col customWidth="1" min="16" max="36" width="8.0"/>
     <col customWidth="1" min="37" max="45" width="7.63"/>
-    <col customWidth="1" min="46" max="61" width="8.88"/>
+    <col customWidth="1" min="46" max="62" width="8.88"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -8605,12 +8636,15 @@
       <c r="BG1" s="2">
         <v>43974.0</v>
       </c>
-      <c r="BH1" s="3">
+      <c r="BH1" s="2">
         <v>43975.0</v>
       </c>
       <c r="BI1" s="2">
+        <v>43976.0</v>
+      </c>
+      <c r="BJ1" s="2">
         <f>today()</f>
-        <v>43976</v>
+        <v>43977</v>
       </c>
     </row>
     <row r="2" ht="14.25" hidden="1" customHeight="1">
@@ -8814,8 +8848,9 @@
       <c r="BF2" s="1"/>
       <c r="BG2" s="1"/>
       <c r="BH2" s="1"/>
-      <c r="BI2" s="1">
-        <f>Confirmed!BI2-Active!BI2</f>
+      <c r="BI2" s="1"/>
+      <c r="BJ2" s="1">
+        <f>Confirmed!BJ2-Active!BJ2</f>
         <v>0</v>
       </c>
     </row>
@@ -9059,7 +9094,11 @@
         <f>Confirmed!BH3-Active!BH4</f>
         <v>29</v>
       </c>
-      <c r="BI3" s="1"/>
+      <c r="BI3" s="1">
+        <f>Confirmed!BI3-Active!BI4</f>
+        <v>29</v>
+      </c>
+      <c r="BJ3" s="1"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="1" t="s">
@@ -9301,7 +9340,11 @@
         <f>Confirmed!BH4-Active!BH5</f>
         <v>30</v>
       </c>
-      <c r="BI4" s="1"/>
+      <c r="BI4" s="1">
+        <f>Confirmed!BI4-Active!BI5</f>
+        <v>30</v>
+      </c>
+      <c r="BJ4" s="1"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="1" t="s">
@@ -9543,7 +9586,11 @@
         <f>Confirmed!BH5-Active!BH6</f>
         <v>58</v>
       </c>
-      <c r="BI5" s="1"/>
+      <c r="BI5" s="1">
+        <f>Confirmed!BI5-Active!BI6</f>
+        <v>61</v>
+      </c>
+      <c r="BJ5" s="1"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="1" t="s">
@@ -9785,7 +9832,11 @@
         <f>Confirmed!BH6-Active!BH7</f>
         <v>56</v>
       </c>
-      <c r="BI6" s="1"/>
+      <c r="BI6" s="1">
+        <f>Confirmed!BI6-Active!BI7</f>
+        <v>58</v>
+      </c>
+      <c r="BJ6" s="1"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="1" t="s">
@@ -10027,7 +10078,11 @@
         <f>Confirmed!BH7-Active!BH8</f>
         <v>1394</v>
       </c>
-      <c r="BI7" s="1"/>
+      <c r="BI7" s="1">
+        <f>Confirmed!BI7-Active!BI8</f>
+        <v>1396</v>
+      </c>
+      <c r="BJ7" s="1"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="1" t="s">
@@ -10269,7 +10324,11 @@
         <f>Confirmed!BH8-Active!BH9</f>
         <v>127</v>
       </c>
-      <c r="BI8" s="1"/>
+      <c r="BI8" s="1">
+        <f>Confirmed!BI8-Active!BI9</f>
+        <v>127</v>
+      </c>
+      <c r="BJ8" s="1"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="1" t="s">
@@ -10511,7 +10570,11 @@
         <f>Confirmed!BH9-Active!BH10</f>
         <v>1160</v>
       </c>
-      <c r="BI9" s="1"/>
+      <c r="BI9" s="1">
+        <f>Confirmed!BI9-Active!BI10</f>
+        <v>1217</v>
+      </c>
+      <c r="BJ9" s="1"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="1" t="s">
@@ -10753,7 +10816,11 @@
         <f>Confirmed!BH10-Active!BH11</f>
         <v>6806</v>
       </c>
-      <c r="BI10" s="1"/>
+      <c r="BI10" s="1">
+        <f>Confirmed!BI10-Active!BI11</f>
+        <v>7551</v>
+      </c>
+      <c r="BJ10" s="1"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="1" t="s">
@@ -10995,7 +11062,11 @@
         <f>Confirmed!BH11-Active!BH12</f>
         <v>1869</v>
       </c>
-      <c r="BI11" s="1"/>
+      <c r="BI11" s="1">
+        <f>Confirmed!BI11-Active!BI12</f>
+        <v>1929</v>
+      </c>
+      <c r="BJ11" s="1"/>
     </row>
     <row r="12" ht="14.25" customHeight="1"/>
     <row r="13" ht="14.25" customHeight="1"/>
@@ -12011,7 +12082,7 @@
     <col customWidth="1" min="2" max="6" width="8.38"/>
     <col customWidth="1" min="7" max="15" width="7.13"/>
     <col customWidth="1" min="16" max="36" width="8.0"/>
-    <col customWidth="1" min="37" max="61" width="7.63"/>
+    <col customWidth="1" min="37" max="62" width="7.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -12192,12 +12263,15 @@
       <c r="BG1" s="2">
         <v>43974.0</v>
       </c>
-      <c r="BH1" s="3">
+      <c r="BH1" s="2">
         <v>43975.0</v>
       </c>
       <c r="BI1" s="2">
+        <v>43976.0</v>
+      </c>
+      <c r="BJ1" s="2">
         <f>today()</f>
-        <v>43976</v>
+        <v>43977</v>
       </c>
     </row>
     <row r="2" ht="14.25" hidden="1" customHeight="1">
@@ -12393,6 +12467,7 @@
       <c r="BG2" s="1"/>
       <c r="BH2" s="1"/>
       <c r="BI2" s="1"/>
+      <c r="BJ2" s="1"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
@@ -12634,7 +12709,11 @@
         <f>IF(Closed!BH3&gt;0,100*Recoveries!BH3/Closed!BH3,100)</f>
         <v>96.55172414</v>
       </c>
-      <c r="BI3" s="1"/>
+      <c r="BI3" s="1">
+        <f>IF(Closed!BI3&gt;0,100*Recoveries!BI3/Closed!BI3,100)</f>
+        <v>96.55172414</v>
+      </c>
+      <c r="BJ3" s="1"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
@@ -12876,7 +12955,11 @@
         <f>IF(Closed!BH4&gt;0,100*Recoveries!BH4/Closed!BH4,100)</f>
         <v>96.66666667</v>
       </c>
-      <c r="BI4" s="1"/>
+      <c r="BI4" s="1">
+        <f>IF(Closed!BI4&gt;0,100*Recoveries!BI4/Closed!BI4,100)</f>
+        <v>96.66666667</v>
+      </c>
+      <c r="BJ4" s="1"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="20" t="s">
@@ -13118,7 +13201,11 @@
         <f>IF(Closed!BH5&gt;0,100*Recoveries!BH5/Closed!BH5,100)</f>
         <v>100</v>
       </c>
-      <c r="BI5" s="1"/>
+      <c r="BI5" s="1">
+        <f>IF(Closed!BI5&gt;0,100*Recoveries!BI5/Closed!BI5,100)</f>
+        <v>100</v>
+      </c>
+      <c r="BJ5" s="1"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="20" t="s">
@@ -13360,7 +13447,11 @@
         <f>IF(Closed!BH6&gt;0,100*Recoveries!BH6/Closed!BH6,100)</f>
         <v>94.64285714</v>
       </c>
-      <c r="BI6" s="1"/>
+      <c r="BI6" s="1">
+        <f>IF(Closed!BI6&gt;0,100*Recoveries!BI6/Closed!BI6,100)</f>
+        <v>94.82758621</v>
+      </c>
+      <c r="BJ6" s="1"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="20" t="s">
@@ -13602,7 +13693,11 @@
         <f>IF(Closed!BH7&gt;0,100*Recoveries!BH7/Closed!BH7,100)</f>
         <v>95.76757532</v>
       </c>
-      <c r="BI7" s="1"/>
+      <c r="BI7" s="1">
+        <f>IF(Closed!BI7&gt;0,100*Recoveries!BI7/Closed!BI7,100)</f>
+        <v>95.63037249</v>
+      </c>
+      <c r="BJ7" s="1"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="20" t="s">
@@ -13844,7 +13939,11 @@
         <f>IF(Closed!BH8&gt;0,100*Recoveries!BH8/Closed!BH8,100)</f>
         <v>95.27559055</v>
       </c>
-      <c r="BI8" s="1"/>
+      <c r="BI8" s="1">
+        <f>IF(Closed!BI8&gt;0,100*Recoveries!BI8/Closed!BI8,100)</f>
+        <v>95.27559055</v>
+      </c>
+      <c r="BJ8" s="1"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="20" t="s">
@@ -14086,7 +14185,11 @@
         <f>IF(Closed!BH9&gt;0,100*Recoveries!BH9/Closed!BH9,100)</f>
         <v>95.77586207</v>
       </c>
-      <c r="BI9" s="1"/>
+      <c r="BI9" s="1">
+        <f>IF(Closed!BI9&gt;0,100*Recoveries!BI9/Closed!BI9,100)</f>
+        <v>95.97370583</v>
+      </c>
+      <c r="BJ9" s="1"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="20" t="s">
@@ -14328,7 +14431,11 @@
         <f>IF(Closed!BH10&gt;0,100*Recoveries!BH10/Closed!BH10,100)</f>
         <v>95.87129004</v>
       </c>
-      <c r="BI10" s="1"/>
+      <c r="BI10" s="1">
+        <f>IF(Closed!BI10&gt;0,100*Recoveries!BI10/Closed!BI10,100)</f>
+        <v>95.62971792</v>
+      </c>
+      <c r="BJ10" s="1"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="20" t="s">
@@ -14570,7 +14677,11 @@
         <f>IF(Closed!BH11&gt;0,100*Recoveries!BH11/Closed!BH11,100)</f>
         <v>98.44836811</v>
       </c>
-      <c r="BI11" s="1"/>
+      <c r="BI11" s="1">
+        <f>IF(Closed!BI11&gt;0,100*Recoveries!BI11/Closed!BI11,100)</f>
+        <v>98.44479005</v>
+      </c>
+      <c r="BJ11" s="1"/>
     </row>
     <row r="12" ht="14.25" customHeight="1"/>
     <row r="13" ht="14.25" customHeight="1"/>
@@ -15594,7 +15705,7 @@
     <col customWidth="1" min="7" max="15" width="7.38"/>
     <col customWidth="1" min="16" max="28" width="10.5"/>
     <col customWidth="1" min="29" max="34" width="11.38"/>
-    <col customWidth="1" min="35" max="61" width="10.5"/>
+    <col customWidth="1" min="35" max="62" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -15775,12 +15886,15 @@
       <c r="BG1" s="2">
         <v>43974.0</v>
       </c>
-      <c r="BH1" s="3">
+      <c r="BH1" s="2">
         <v>43975.0</v>
       </c>
       <c r="BI1" s="2">
+        <v>43976.0</v>
+      </c>
+      <c r="BJ1" s="2">
         <f>today()</f>
-        <v>43976</v>
+        <v>43977</v>
       </c>
     </row>
     <row r="2" ht="14.25" hidden="1" customHeight="1">
@@ -15976,6 +16090,7 @@
       <c r="BG2" s="1"/>
       <c r="BH2" s="1"/>
       <c r="BI2" s="1"/>
+      <c r="BJ2" s="1"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="1" t="s">
@@ -16217,7 +16332,11 @@
         <f>IF(Closed!BH3&gt;0,100*Deaths!BH3/Closed!BH3,0)</f>
         <v>3.448275862</v>
       </c>
-      <c r="BI3" s="1"/>
+      <c r="BI3" s="1">
+        <f>IF(Closed!BI3&gt;0,100*Deaths!BI3/Closed!BI3,0)</f>
+        <v>3.448275862</v>
+      </c>
+      <c r="BJ3" s="1"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="1" t="s">
@@ -16459,7 +16578,11 @@
         <f>IF(Closed!BH4&gt;0,100*Deaths!BH4/Closed!BH4,0)</f>
         <v>3.333333333</v>
       </c>
-      <c r="BI4" s="1"/>
+      <c r="BI4" s="1">
+        <f>IF(Closed!BI4&gt;0,100*Deaths!BI4/Closed!BI4,0)</f>
+        <v>3.333333333</v>
+      </c>
+      <c r="BJ4" s="1"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="1" t="s">
@@ -16701,7 +16824,11 @@
         <f>IF(Closed!BH5&gt;0,100*Deaths!BH5/Closed!BH5,0)</f>
         <v>0</v>
       </c>
-      <c r="BI5" s="1"/>
+      <c r="BI5" s="1">
+        <f>IF(Closed!BI5&gt;0,100*Deaths!BI5/Closed!BI5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BJ5" s="1"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="1" t="s">
@@ -16943,7 +17070,11 @@
         <f>IF(Closed!BH6&gt;0,100*Deaths!BH6/Closed!BH6,0)</f>
         <v>5.357142857</v>
       </c>
-      <c r="BI6" s="1"/>
+      <c r="BI6" s="1">
+        <f>IF(Closed!BI6&gt;0,100*Deaths!BI6/Closed!BI6,0)</f>
+        <v>5.172413793</v>
+      </c>
+      <c r="BJ6" s="1"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="1" t="s">
@@ -17185,7 +17316,11 @@
         <f>IF(Closed!BH7&gt;0,100*Deaths!BH7/Closed!BH7,0)</f>
         <v>4.232424677</v>
       </c>
-      <c r="BI7" s="1"/>
+      <c r="BI7" s="1">
+        <f>IF(Closed!BI7&gt;0,100*Deaths!BI7/Closed!BI7,0)</f>
+        <v>4.369627507</v>
+      </c>
+      <c r="BJ7" s="1"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="1" t="s">
@@ -17427,7 +17562,11 @@
         <f>IF(Closed!BH8&gt;0,100*Deaths!BH8/Closed!BH8,0)</f>
         <v>4.724409449</v>
       </c>
-      <c r="BI8" s="1"/>
+      <c r="BI8" s="1">
+        <f>IF(Closed!BI8&gt;0,100*Deaths!BI8/Closed!BI8,0)</f>
+        <v>4.724409449</v>
+      </c>
+      <c r="BJ8" s="1"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="1" t="s">
@@ -17669,7 +17808,11 @@
         <f>IF(Closed!BH9&gt;0,100*Deaths!BH9/Closed!BH9,0)</f>
         <v>4.224137931</v>
       </c>
-      <c r="BI9" s="1"/>
+      <c r="BI9" s="1">
+        <f>IF(Closed!BI9&gt;0,100*Deaths!BI9/Closed!BI9,0)</f>
+        <v>4.026294166</v>
+      </c>
+      <c r="BJ9" s="1"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="1" t="s">
@@ -17911,7 +18054,11 @@
         <f>IF(Closed!BH10&gt;0,100*Deaths!BH10/Closed!BH10,0)</f>
         <v>4.128709962</v>
       </c>
-      <c r="BI10" s="1"/>
+      <c r="BI10" s="1">
+        <f>IF(Closed!BI10&gt;0,100*Deaths!BI10/Closed!BI10,0)</f>
+        <v>4.370282082</v>
+      </c>
+      <c r="BJ10" s="1"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="1" t="s">
@@ -18153,7 +18300,11 @@
         <f>IF(Closed!BH11&gt;0,100*Deaths!BH11/Closed!BH11,0)</f>
         <v>1.551631889</v>
       </c>
-      <c r="BI11" s="1"/>
+      <c r="BI11" s="1">
+        <f>IF(Closed!BI11&gt;0,100*Deaths!BI11/Closed!BI11,0)</f>
+        <v>1.555209953</v>
+      </c>
+      <c r="BJ11" s="1"/>
     </row>
     <row r="12" ht="14.25" customHeight="1"/>
     <row r="13" ht="14.25" customHeight="1"/>
@@ -19172,7 +19323,7 @@
     <col customWidth="1" min="7" max="15" width="7.38"/>
     <col customWidth="1" min="16" max="28" width="10.5"/>
     <col customWidth="1" min="29" max="34" width="11.38"/>
-    <col customWidth="1" min="35" max="61" width="10.5"/>
+    <col customWidth="1" min="35" max="62" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -19353,12 +19504,15 @@
       <c r="BG1" s="2">
         <v>43974.0</v>
       </c>
-      <c r="BH1" s="3">
+      <c r="BH1" s="2">
         <v>43975.0</v>
       </c>
       <c r="BI1" s="2">
+        <v>43976.0</v>
+      </c>
+      <c r="BJ1" s="2">
         <f>today()</f>
-        <v>43976</v>
+        <v>43977</v>
       </c>
     </row>
     <row r="2" ht="14.25" hidden="1" customHeight="1">
@@ -19554,13 +19708,14 @@
       <c r="BG2" s="1"/>
       <c r="BH2" s="1"/>
       <c r="BI2" s="1"/>
+      <c r="BJ2" s="1"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="14" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="21">
-        <f t="shared" ref="B3:BI3" si="1">(B4*$B$16+B5*$B$17+B6*$B$18+B7*$B$19+B8*$B$20+B9*$B$21+B10*$B$22+B11*$B$23+B12*$B$24)/sum($B$16:$B$24)</f>
+        <f t="shared" ref="B3:BJ3" si="1">(B4*$B$16+B5*$B$17+B6*$B$18+B7*$B$19+B8*$B$20+B9*$B$21+B10*$B$22+B11*$B$23+B12*$B$24)/sum($B$16:$B$24)</f>
         <v>0.02559675512</v>
       </c>
       <c r="C3" s="21">
@@ -19796,6 +19951,10 @@
         <v>0.02827787805</v>
       </c>
       <c r="BI3" s="21">
+        <f t="shared" si="1"/>
+        <v>0.02893183701</v>
+      </c>
+      <c r="BJ3" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -20040,7 +20199,11 @@
         <f>Confirmed!BH3/Testing!BH3</f>
         <v>0.007271405199</v>
       </c>
-      <c r="BI4" s="22"/>
+      <c r="BI4" s="22">
+        <f>Confirmed!BI3/Testing!BI3</f>
+        <v>0.008002845456</v>
+      </c>
+      <c r="BJ4" s="22"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="1" t="s">
@@ -20282,7 +20445,11 @@
         <f>Confirmed!BH4/Testing!BH4</f>
         <v>0.009241962442</v>
       </c>
-      <c r="BI5" s="22"/>
+      <c r="BI5" s="22">
+        <f>Confirmed!BI4/Testing!BI4</f>
+        <v>0.01048480185</v>
+      </c>
+      <c r="BJ5" s="22"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="1" t="s">
@@ -20524,7 +20691,11 @@
         <f>Confirmed!BH5/Testing!BH5</f>
         <v>0.00585948831</v>
       </c>
-      <c r="BI6" s="22"/>
+      <c r="BI6" s="22">
+        <f>Confirmed!BI5/Testing!BI5</f>
+        <v>0.005789204836</v>
+      </c>
+      <c r="BJ6" s="22"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="1" t="s">
@@ -20766,7 +20937,11 @@
         <f>Confirmed!BH6/Testing!BH6</f>
         <v>0.01050385688</v>
       </c>
-      <c r="BI7" s="22"/>
+      <c r="BI7" s="22">
+        <f>Confirmed!BI6/Testing!BI6</f>
+        <v>0.0105973025</v>
+      </c>
+      <c r="BJ7" s="22"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="1" t="s">
@@ -21008,7 +21183,11 @@
         <f>Confirmed!BH7/Testing!BH7</f>
         <v>0.04500585578</v>
       </c>
-      <c r="BI8" s="22"/>
+      <c r="BI8" s="22">
+        <f>Confirmed!BI7/Testing!BI7</f>
+        <v>0.04498060334</v>
+      </c>
+      <c r="BJ8" s="22"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="1" t="s">
@@ -21250,7 +21429,11 @@
         <f>Confirmed!BH8/Testing!BH8</f>
         <v>0.007182477599</v>
       </c>
-      <c r="BI9" s="22"/>
+      <c r="BI9" s="22">
+        <f>Confirmed!BI8/Testing!BI8</f>
+        <v>0.007235789327</v>
+      </c>
+      <c r="BJ9" s="22"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="1" t="s">
@@ -21492,7 +21675,11 @@
         <f>Confirmed!BH9/Testing!BH9</f>
         <v>0.01822655152</v>
       </c>
-      <c r="BI10" s="22"/>
+      <c r="BI10" s="22">
+        <f>Confirmed!BI9/Testing!BI9</f>
+        <v>0.01849013597</v>
+      </c>
+      <c r="BJ10" s="22"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="1" t="s">
@@ -21734,7 +21921,11 @@
         <f>Confirmed!BH10/Testing!BH10</f>
         <v>0.1136311075</v>
       </c>
-      <c r="BI11" s="22"/>
+      <c r="BI11" s="22">
+        <f>Confirmed!BI10/Testing!BI10</f>
+        <v>0.11611823</v>
+      </c>
+      <c r="BJ11" s="22"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="1" t="s">
@@ -21976,7 +22167,11 @@
         <f>Confirmed!BH11/Testing!BH11</f>
         <v>0.01446757448</v>
       </c>
-      <c r="BI12" s="22"/>
+      <c r="BI12" s="22">
+        <f>Confirmed!BI11/Testing!BI11</f>
+        <v>0.01527726734</v>
+      </c>
+      <c r="BJ12" s="22"/>
     </row>
     <row r="13" ht="14.25" customHeight="1"/>
     <row r="14" ht="14.25" customHeight="1"/>
@@ -23057,7 +23252,7 @@
     <col customWidth="1" min="7" max="15" width="7.13"/>
     <col customWidth="1" min="16" max="36" width="8.0"/>
     <col customWidth="1" min="37" max="43" width="7.63"/>
-    <col customWidth="1" min="44" max="61" width="9.88"/>
+    <col customWidth="1" min="44" max="62" width="9.88"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -23184,7 +23379,7 @@
       <c r="AO1" s="2">
         <v>43956.0</v>
       </c>
-      <c r="AP1" s="5">
+      <c r="AP1" s="6">
         <v>43957.0</v>
       </c>
       <c r="AQ1" s="2">
@@ -23205,7 +23400,7 @@
       <c r="AV1" s="2">
         <v>43963.0</v>
       </c>
-      <c r="AW1" s="5">
+      <c r="AW1" s="6">
         <v>43964.0</v>
       </c>
       <c r="AX1" s="2">
@@ -23226,24 +23421,27 @@
       <c r="BC1" s="2">
         <v>43970.0</v>
       </c>
-      <c r="BD1" s="5">
+      <c r="BD1" s="6">
         <v>43971.0</v>
       </c>
       <c r="BE1" s="2">
         <v>43972.0</v>
       </c>
-      <c r="BF1" s="6">
+      <c r="BF1" s="7">
         <v>43973.0</v>
       </c>
-      <c r="BG1" s="3">
+      <c r="BG1" s="2">
         <v>43974.0</v>
       </c>
       <c r="BH1" s="7">
         <v>43975.0</v>
       </c>
-      <c r="BI1" s="2">
+      <c r="BI1" s="3">
+        <v>43976.0</v>
+      </c>
+      <c r="BJ1" s="2">
         <f>today()</f>
-        <v>43976</v>
+        <v>43977</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
@@ -23410,7 +23608,7 @@
         <f t="shared" si="1"/>
         <v>17962</v>
       </c>
-      <c r="AP2" s="8">
+      <c r="AP2" s="5">
         <v>18720.0</v>
       </c>
       <c r="AQ2" s="1">
@@ -23437,7 +23635,7 @@
         <f t="shared" si="2"/>
         <v>21118</v>
       </c>
-      <c r="AW2" s="8">
+      <c r="AW2" s="5">
         <v>22069.0</v>
       </c>
       <c r="AX2" s="1">
@@ -23464,11 +23662,11 @@
         <f t="shared" si="3"/>
         <v>25020</v>
       </c>
-      <c r="BD2" s="8">
+      <c r="BD2" s="5">
         <v>25955.0</v>
       </c>
       <c r="BE2" s="1">
-        <f t="shared" ref="BE2:BH2" si="4">ROUND($BD2/$BD$12*BE$12,0)</f>
+        <f t="shared" ref="BE2:BI2" si="4">ROUND($BD2/$BD$12*BE$12,0)</f>
         <v>26906</v>
       </c>
       <c r="BF2" s="1">
@@ -23483,7 +23681,11 @@
         <f t="shared" si="4"/>
         <v>29898</v>
       </c>
-      <c r="BI2" s="1"/>
+      <c r="BI2" s="1">
+        <f t="shared" si="4"/>
+        <v>30559</v>
+      </c>
+      <c r="BJ2" s="1"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="1" t="s">
@@ -23649,7 +23851,7 @@
         <f t="shared" si="5"/>
         <v>2165</v>
       </c>
-      <c r="AP3" s="8">
+      <c r="AP3" s="5">
         <v>2256.0</v>
       </c>
       <c r="AQ3" s="1">
@@ -23676,7 +23878,7 @@
         <f t="shared" si="6"/>
         <v>3524</v>
       </c>
-      <c r="AW3" s="8">
+      <c r="AW3" s="5">
         <v>3683.0</v>
       </c>
       <c r="AX3" s="1">
@@ -23703,11 +23905,11 @@
         <f t="shared" si="7"/>
         <v>4604</v>
       </c>
-      <c r="BD3" s="8">
+      <c r="BD3" s="5">
         <v>4776.0</v>
       </c>
       <c r="BE3" s="1">
-        <f t="shared" ref="BE3:BH3" si="8">ROUND($BD3/$BD$12*BE$12,0)</f>
+        <f t="shared" ref="BE3:BI3" si="8">ROUND($BD3/$BD$12*BE$12,0)</f>
         <v>4951</v>
       </c>
       <c r="BF3" s="1">
@@ -23722,7 +23924,11 @@
         <f t="shared" si="8"/>
         <v>5501</v>
       </c>
-      <c r="BI3" s="1"/>
+      <c r="BI3" s="1">
+        <f t="shared" si="8"/>
+        <v>5623</v>
+      </c>
+      <c r="BJ3" s="1"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="1" t="s">
@@ -23888,7 +24094,7 @@
         <f t="shared" si="9"/>
         <v>3956</v>
       </c>
-      <c r="AP4" s="8">
+      <c r="AP4" s="5">
         <v>4123.0</v>
       </c>
       <c r="AQ4" s="1">
@@ -23915,7 +24121,7 @@
         <f t="shared" si="10"/>
         <v>5561</v>
       </c>
-      <c r="AW4" s="8">
+      <c r="AW4" s="5">
         <v>5812.0</v>
       </c>
       <c r="AX4" s="1">
@@ -23942,11 +24148,11 @@
         <f t="shared" si="11"/>
         <v>8512</v>
       </c>
-      <c r="BD4" s="8">
+      <c r="BD4" s="5">
         <v>8830.0</v>
       </c>
       <c r="BE4" s="1">
-        <f t="shared" ref="BE4:BH4" si="12">ROUND($BD4/$BD$12*BE$12,0)</f>
+        <f t="shared" ref="BE4:BI4" si="12">ROUND($BD4/$BD$12*BE$12,0)</f>
         <v>9154</v>
       </c>
       <c r="BF4" s="1">
@@ -23961,7 +24167,11 @@
         <f t="shared" si="12"/>
         <v>10171</v>
       </c>
-      <c r="BI4" s="1"/>
+      <c r="BI4" s="1">
+        <f t="shared" si="12"/>
+        <v>10396</v>
+      </c>
+      <c r="BJ4" s="1"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="1" t="s">
@@ -24127,7 +24337,7 @@
         <f t="shared" si="13"/>
         <v>7385</v>
       </c>
-      <c r="AP5" s="8">
+      <c r="AP5" s="5">
         <v>7697.0</v>
       </c>
       <c r="AQ5" s="1">
@@ -24154,7 +24364,7 @@
         <f t="shared" si="14"/>
         <v>10922</v>
       </c>
-      <c r="AW5" s="8">
+      <c r="AW5" s="5">
         <v>11414.0</v>
       </c>
       <c r="AX5" s="1">
@@ -24181,11 +24391,11 @@
         <f t="shared" si="15"/>
         <v>14425</v>
       </c>
-      <c r="BD5" s="8">
+      <c r="BD5" s="5">
         <v>14964.0</v>
       </c>
       <c r="BE5" s="1">
-        <f t="shared" ref="BE5:BH5" si="16">ROUND($BD5/$BD$12*BE$12,0)</f>
+        <f t="shared" ref="BE5:BI5" si="16">ROUND($BD5/$BD$12*BE$12,0)</f>
         <v>15512</v>
       </c>
       <c r="BF5" s="1">
@@ -24200,7 +24410,11 @@
         <f t="shared" si="16"/>
         <v>17237</v>
       </c>
-      <c r="BI5" s="1"/>
+      <c r="BI5" s="1">
+        <f t="shared" si="16"/>
+        <v>17619</v>
+      </c>
+      <c r="BJ5" s="1"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="1" t="s">
@@ -24366,7 +24580,7 @@
         <f t="shared" si="17"/>
         <v>6096</v>
       </c>
-      <c r="AP6" s="8">
+      <c r="AP6" s="5">
         <v>6353.0</v>
       </c>
       <c r="AQ6" s="1">
@@ -24393,7 +24607,7 @@
         <f t="shared" si="18"/>
         <v>7884</v>
       </c>
-      <c r="AW6" s="8">
+      <c r="AW6" s="5">
         <v>8239.0</v>
       </c>
       <c r="AX6" s="1">
@@ -24420,11 +24634,11 @@
         <f t="shared" si="19"/>
         <v>10198</v>
       </c>
-      <c r="BD6" s="8">
+      <c r="BD6" s="5">
         <v>10579.0</v>
       </c>
       <c r="BE6" s="1">
-        <f t="shared" ref="BE6:BH6" si="20">ROUND($BD6/$BD$12*BE$12,0)</f>
+        <f t="shared" ref="BE6:BI6" si="20">ROUND($BD6/$BD$12*BE$12,0)</f>
         <v>10967</v>
       </c>
       <c r="BF6" s="1">
@@ -24439,7 +24653,11 @@
         <f t="shared" si="20"/>
         <v>12186</v>
       </c>
-      <c r="BI6" s="1"/>
+      <c r="BI6" s="1">
+        <f t="shared" si="20"/>
+        <v>12456</v>
+      </c>
+      <c r="BJ6" s="1"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="1" t="s">
@@ -24605,7 +24823,7 @@
         <f t="shared" si="21"/>
         <v>24678</v>
       </c>
-      <c r="AP7" s="8">
+      <c r="AP7" s="5">
         <v>25720.0</v>
       </c>
       <c r="AQ7" s="1">
@@ -24632,7 +24850,7 @@
         <f t="shared" si="22"/>
         <v>36479</v>
       </c>
-      <c r="AW7" s="8">
+      <c r="AW7" s="5">
         <v>38122.0</v>
       </c>
       <c r="AX7" s="1">
@@ -24659,11 +24877,11 @@
         <f t="shared" si="23"/>
         <v>50020</v>
       </c>
-      <c r="BD7" s="8">
+      <c r="BD7" s="5">
         <v>51888.0</v>
       </c>
       <c r="BE7" s="1">
-        <f t="shared" ref="BE7:BH7" si="24">ROUND($BD7/$BD$12*BE$12,0)</f>
+        <f t="shared" ref="BE7:BI7" si="24">ROUND($BD7/$BD$12*BE$12,0)</f>
         <v>53789</v>
       </c>
       <c r="BF7" s="1">
@@ -24678,7 +24896,11 @@
         <f t="shared" si="24"/>
         <v>59770</v>
       </c>
-      <c r="BI7" s="1"/>
+      <c r="BI7" s="1">
+        <f t="shared" si="24"/>
+        <v>61093</v>
+      </c>
+      <c r="BJ7" s="1"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="1" t="s">
@@ -24844,7 +25066,7 @@
         <f t="shared" si="25"/>
         <v>13686</v>
       </c>
-      <c r="AP8" s="8">
+      <c r="AP8" s="5">
         <v>14264.0</v>
       </c>
       <c r="AQ8" s="1">
@@ -24871,7 +25093,7 @@
         <f t="shared" si="26"/>
         <v>18435</v>
       </c>
-      <c r="AW8" s="8">
+      <c r="AW8" s="5">
         <v>19265.0</v>
       </c>
       <c r="AX8" s="1">
@@ -24898,11 +25120,11 @@
         <f t="shared" si="27"/>
         <v>23536</v>
       </c>
-      <c r="BD8" s="8">
+      <c r="BD8" s="5">
         <v>24415.0</v>
       </c>
       <c r="BE8" s="1">
-        <f t="shared" ref="BE8:BH8" si="28">ROUND($BD8/$BD$12*BE$12,0)</f>
+        <f t="shared" ref="BE8:BI8" si="28">ROUND($BD8/$BD$12*BE$12,0)</f>
         <v>25310</v>
       </c>
       <c r="BF8" s="1">
@@ -24917,7 +25139,11 @@
         <f t="shared" si="28"/>
         <v>28124</v>
       </c>
-      <c r="BI8" s="1"/>
+      <c r="BI8" s="1">
+        <f t="shared" si="28"/>
+        <v>28746</v>
+      </c>
+      <c r="BJ8" s="1"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="1" t="s">
@@ -25083,7 +25309,7 @@
         <f t="shared" si="29"/>
         <v>48923</v>
       </c>
-      <c r="AP9" s="8">
+      <c r="AP9" s="5">
         <v>50988.0</v>
       </c>
       <c r="AQ9" s="1">
@@ -25110,7 +25336,7 @@
         <f t="shared" si="30"/>
         <v>64928</v>
       </c>
-      <c r="AW9" s="8">
+      <c r="AW9" s="5">
         <v>67853.0</v>
       </c>
       <c r="AX9" s="1">
@@ -25137,11 +25363,11 @@
         <f t="shared" si="31"/>
         <v>83335</v>
       </c>
-      <c r="BD9" s="8">
+      <c r="BD9" s="5">
         <v>86448.0</v>
       </c>
       <c r="BE9" s="1">
-        <f t="shared" ref="BE9:BH9" si="32">ROUND($BD9/$BD$12*BE$12,0)</f>
+        <f t="shared" ref="BE9:BI9" si="32">ROUND($BD9/$BD$12*BE$12,0)</f>
         <v>89616</v>
       </c>
       <c r="BF9" s="1">
@@ -25156,7 +25382,11 @@
         <f t="shared" si="32"/>
         <v>99580</v>
       </c>
-      <c r="BI9" s="1"/>
+      <c r="BI9" s="1">
+        <f t="shared" si="32"/>
+        <v>101784</v>
+      </c>
+      <c r="BJ9" s="1"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="1" t="s">
@@ -25322,7 +25552,7 @@
         <f t="shared" si="33"/>
         <v>54678</v>
       </c>
-      <c r="AP10" s="8">
+      <c r="AP10" s="5">
         <v>56986.0</v>
       </c>
       <c r="AQ10" s="1">
@@ -25349,7 +25579,7 @@
         <f t="shared" si="34"/>
         <v>79293</v>
       </c>
-      <c r="AW10" s="8">
+      <c r="AW10" s="5">
         <v>82865.0</v>
       </c>
       <c r="AX10" s="1">
@@ -25376,11 +25606,11 @@
         <f t="shared" si="35"/>
         <v>108557</v>
       </c>
-      <c r="BD10" s="8">
+      <c r="BD10" s="5">
         <v>112612.0</v>
       </c>
       <c r="BE10" s="1">
-        <f t="shared" ref="BE10:BH10" si="36">ROUND($BD10/$BD$12*BE$12,0)</f>
+        <f t="shared" ref="BE10:BI10" si="36">ROUND($BD10/$BD$12*BE$12,0)</f>
         <v>116738</v>
       </c>
       <c r="BF10" s="1">
@@ -25395,7 +25625,11 @@
         <f t="shared" si="36"/>
         <v>129718</v>
       </c>
-      <c r="BI10" s="1"/>
+      <c r="BI10" s="1">
+        <f t="shared" si="36"/>
+        <v>132589</v>
+      </c>
+      <c r="BJ10" s="1"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="1" t="s">
@@ -25561,7 +25795,7 @@
         <f t="shared" si="37"/>
         <v>88535</v>
       </c>
-      <c r="AP11" s="8">
+      <c r="AP11" s="5">
         <v>92272.0</v>
       </c>
       <c r="AQ11" s="1">
@@ -25588,7 +25822,7 @@
         <f t="shared" si="38"/>
         <v>121554</v>
       </c>
-      <c r="AW11" s="8">
+      <c r="AW11" s="5">
         <v>127030.0</v>
       </c>
       <c r="AX11" s="1">
@@ -25615,11 +25849,11 @@
         <f t="shared" si="39"/>
         <v>160402</v>
       </c>
-      <c r="BD11" s="8">
+      <c r="BD11" s="5">
         <v>166394.0</v>
       </c>
       <c r="BE11" s="1">
-        <f t="shared" ref="BE11:BH11" si="40">ROUND($BD11/$BD$12*BE$12,0)</f>
+        <f t="shared" ref="BE11:BI11" si="40">ROUND($BD11/$BD$12*BE$12,0)</f>
         <v>172491</v>
       </c>
       <c r="BF11" s="1">
@@ -25634,7 +25868,11 @@
         <f t="shared" si="40"/>
         <v>191670</v>
       </c>
-      <c r="BI11" s="1"/>
+      <c r="BI11" s="1">
+        <f t="shared" si="40"/>
+        <v>195912</v>
+      </c>
+      <c r="BJ11" s="1"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="9" t="s">
@@ -25817,13 +26055,16 @@
       <c r="BH12" s="9">
         <v>583855.0</v>
       </c>
+      <c r="BI12" s="9">
+        <v>596777.0</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="13">
-        <f t="shared" ref="B13:BI13" si="41">sum(B2:B11)</f>
+        <f t="shared" ref="B13:BJ13" si="41">sum(B2:B11)</f>
         <v>28536</v>
       </c>
       <c r="C13" s="13">
@@ -26059,6 +26300,10 @@
         <v>583855</v>
       </c>
       <c r="BI13" s="13">
+        <f t="shared" si="41"/>
+        <v>596777</v>
+      </c>
+      <c r="BJ13" s="13">
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
@@ -26152,6 +26397,7 @@
       <c r="BG15" s="4"/>
       <c r="BH15" s="4"/>
       <c r="BI15" s="4"/>
+      <c r="BJ15" s="4"/>
     </row>
     <row r="16" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
@@ -27165,7 +27411,7 @@
     <col customWidth="1" min="7" max="15" width="7.13"/>
     <col customWidth="1" min="16" max="36" width="8.0"/>
     <col customWidth="1" min="37" max="43" width="7.63"/>
-    <col customWidth="1" min="44" max="61" width="9.88"/>
+    <col customWidth="1" min="44" max="62" width="9.88"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -27350,8 +27596,11 @@
         <v>43975.0</v>
       </c>
       <c r="BI1" s="2">
+        <v>43976.0</v>
+      </c>
+      <c r="BJ1" s="2">
         <f>TODAY()</f>
-        <v>43976</v>
+        <v>43977</v>
       </c>
     </row>
     <row r="2" ht="14.25" hidden="1" customHeight="1">
@@ -27518,7 +27767,7 @@
         <f t="shared" si="1"/>
         <v>#REF!</v>
       </c>
-      <c r="AP2" s="8">
+      <c r="AP2" s="5">
         <v>18720.0</v>
       </c>
       <c r="AQ2" s="1" t="str">
@@ -27560,7 +27809,8 @@
       <c r="BF2" s="1"/>
       <c r="BG2" s="1"/>
       <c r="BH2" s="1"/>
-      <c r="BI2" s="1" t="str">
+      <c r="BI2" s="1"/>
+      <c r="BJ2" s="1" t="str">
         <f>ROUND($AP2/#REF!*#REF!,0)</f>
         <v>#REF!</v>
       </c>
@@ -27805,7 +28055,11 @@
         <f>round(100000*Testing!BH3/$B13,0)</f>
         <v>435</v>
       </c>
-      <c r="BI3" s="1"/>
+      <c r="BI3" s="1">
+        <f>round(100000*Testing!BI3/$B13,0)</f>
+        <v>445</v>
+      </c>
+      <c r="BJ3" s="1"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="1" t="s">
@@ -28047,7 +28301,11 @@
         <f>round(100000*Testing!BH4/$B14,0)</f>
         <v>253</v>
       </c>
-      <c r="BI4" s="1"/>
+      <c r="BI4" s="1">
+        <f>round(100000*Testing!BI4/$B14,0)</f>
+        <v>258</v>
+      </c>
+      <c r="BJ4" s="1"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="1" t="s">
@@ -28289,7 +28547,11 @@
         <f>round(100000*Testing!BH5/$B15,0)</f>
         <v>375</v>
       </c>
-      <c r="BI5" s="1"/>
+      <c r="BI5" s="1">
+        <f>round(100000*Testing!BI5/$B15,0)</f>
+        <v>384</v>
+      </c>
+      <c r="BJ5" s="1"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="1" t="s">
@@ -28531,7 +28793,11 @@
         <f>round(100000*Testing!BH6/$B16,0)</f>
         <v>204</v>
       </c>
-      <c r="BI6" s="1"/>
+      <c r="BI6" s="1">
+        <f>round(100000*Testing!BI6/$B16,0)</f>
+        <v>208</v>
+      </c>
+      <c r="BJ6" s="1"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="1" t="s">
@@ -28773,7 +29039,11 @@
         <f>round(100000*Testing!BH7/$B17,0)</f>
         <v>890</v>
       </c>
-      <c r="BI7" s="1"/>
+      <c r="BI7" s="1">
+        <f>round(100000*Testing!BI7/$B17,0)</f>
+        <v>910</v>
+      </c>
+      <c r="BJ7" s="1"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="1" t="s">
@@ -29015,7 +29285,11 @@
         <f>round(100000*Testing!BH8/$B18,0)</f>
         <v>974</v>
       </c>
-      <c r="BI8" s="1"/>
+      <c r="BI8" s="1">
+        <f>round(100000*Testing!BI8/$B18,0)</f>
+        <v>996</v>
+      </c>
+      <c r="BJ8" s="1"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="1" t="s">
@@ -29257,7 +29531,11 @@
         <f>round(100000*Testing!BH9/$B19,0)</f>
         <v>882</v>
       </c>
-      <c r="BI9" s="1"/>
+      <c r="BI9" s="1">
+        <f>round(100000*Testing!BI9/$B19,0)</f>
+        <v>902</v>
+      </c>
+      <c r="BJ9" s="1"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="1" t="s">
@@ -29499,7 +29777,11 @@
         <f>round(100000*Testing!BH10/$B20,0)</f>
         <v>1895</v>
       </c>
-      <c r="BI10" s="1"/>
+      <c r="BI10" s="1">
+        <f>round(100000*Testing!BI10/$B20,0)</f>
+        <v>1937</v>
+      </c>
+      <c r="BJ10" s="1"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="1" t="s">
@@ -29741,7 +30023,11 @@
         <f>round(100000*Testing!BH11/$B21,0)</f>
         <v>1263</v>
       </c>
-      <c r="BI11" s="1"/>
+      <c r="BI11" s="1">
+        <f>round(100000*Testing!BI11/$B21,0)</f>
+        <v>1291</v>
+      </c>
+      <c r="BJ11" s="1"/>
     </row>
     <row r="12" ht="14.25" customHeight="1"/>
     <row r="13" ht="14.25" customHeight="1">
@@ -30817,7 +31103,7 @@
     <col customWidth="1" min="7" max="15" width="7.13"/>
     <col customWidth="1" min="16" max="36" width="8.0"/>
     <col customWidth="1" min="37" max="45" width="7.63"/>
-    <col customWidth="1" min="46" max="61" width="8.88"/>
+    <col customWidth="1" min="46" max="62" width="8.88"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -30995,15 +31281,18 @@
       <c r="BF1" s="2">
         <v>43973.0</v>
       </c>
-      <c r="BG1" s="3">
+      <c r="BG1" s="2">
         <v>43974.0</v>
       </c>
-      <c r="BH1" s="3">
+      <c r="BH1" s="2">
         <v>43975.0</v>
       </c>
-      <c r="BI1" s="2">
+      <c r="BI1" s="3">
+        <v>43976.0</v>
+      </c>
+      <c r="BJ1" s="2">
         <f>today()</f>
-        <v>43976</v>
+        <v>43977</v>
       </c>
     </row>
     <row r="2" ht="14.25" hidden="1" customHeight="1">
@@ -31166,6 +31455,7 @@
       <c r="BG2" s="4"/>
       <c r="BH2" s="4"/>
       <c r="BI2" s="4"/>
+      <c r="BJ2" s="4"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="1" t="s">
@@ -31348,7 +31638,10 @@
       <c r="BH3" s="4">
         <v>1.0</v>
       </c>
-      <c r="BI3" s="4"/>
+      <c r="BI3" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="BJ3" s="4"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="1" t="s">
@@ -31531,7 +31824,10 @@
       <c r="BH4" s="4">
         <v>1.0</v>
       </c>
-      <c r="BI4" s="4"/>
+      <c r="BI4" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="BJ4" s="4"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="1" t="s">
@@ -31714,7 +32010,10 @@
       <c r="BH5" s="4">
         <v>0.0</v>
       </c>
-      <c r="BI5" s="4"/>
+      <c r="BI5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="BJ5" s="4"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="1" t="s">
@@ -31897,7 +32196,10 @@
       <c r="BH6" s="4">
         <v>3.0</v>
       </c>
-      <c r="BI6" s="4"/>
+      <c r="BI6" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="BJ6" s="4"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="1" t="s">
@@ -32080,7 +32382,10 @@
       <c r="BH7" s="4">
         <v>59.0</v>
       </c>
-      <c r="BI7" s="4"/>
+      <c r="BI7" s="4">
+        <v>61.0</v>
+      </c>
+      <c r="BJ7" s="4"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="1" t="s">
@@ -32263,7 +32568,10 @@
       <c r="BH8" s="4">
         <v>6.0</v>
       </c>
-      <c r="BI8" s="4"/>
+      <c r="BI8" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="BJ8" s="4"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="1" t="s">
@@ -32446,7 +32754,10 @@
       <c r="BH9" s="4">
         <v>49.0</v>
       </c>
-      <c r="BI9" s="4"/>
+      <c r="BI9" s="4">
+        <v>49.0</v>
+      </c>
+      <c r="BJ9" s="4"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="1" t="s">
@@ -32629,7 +32940,10 @@
       <c r="BH10" s="4">
         <v>281.0</v>
       </c>
-      <c r="BI10" s="4"/>
+      <c r="BI10" s="4">
+        <v>330.0</v>
+      </c>
+      <c r="BJ10" s="4"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="1" t="s">
@@ -32812,7 +33126,10 @@
       <c r="BH11" s="4">
         <v>29.0</v>
       </c>
-      <c r="BI11" s="4"/>
+      <c r="BI11" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="BJ11" s="4"/>
     </row>
     <row r="12" ht="14.25" customHeight="1"/>
     <row r="13" ht="14.25" customHeight="1"/>
@@ -33829,7 +34146,7 @@
     <col customWidth="1" min="7" max="15" width="7.13"/>
     <col customWidth="1" min="16" max="36" width="8.0"/>
     <col customWidth="1" min="37" max="45" width="7.63"/>
-    <col customWidth="1" min="46" max="61" width="8.88"/>
+    <col customWidth="1" min="46" max="62" width="8.88"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -33971,37 +34288,37 @@
       <c r="AT1" s="2">
         <v>43961.0</v>
       </c>
-      <c r="AU1" s="6">
+      <c r="AU1" s="7">
         <v>43962.0</v>
       </c>
       <c r="AV1" s="2">
         <v>43963.0</v>
       </c>
-      <c r="AW1" s="6">
+      <c r="AW1" s="7">
         <v>43964.0</v>
       </c>
       <c r="AX1" s="2">
         <v>43965.0</v>
       </c>
-      <c r="AY1" s="6">
+      <c r="AY1" s="7">
         <v>43966.0</v>
       </c>
       <c r="AZ1" s="2">
         <v>43967.0</v>
       </c>
-      <c r="BA1" s="6">
+      <c r="BA1" s="7">
         <v>43968.0</v>
       </c>
       <c r="BB1" s="2">
         <v>43969.0</v>
       </c>
-      <c r="BC1" s="6">
+      <c r="BC1" s="7">
         <v>43970.0</v>
       </c>
       <c r="BD1" s="2">
         <v>43971.0</v>
       </c>
-      <c r="BE1" s="6">
+      <c r="BE1" s="7">
         <v>43972.0</v>
       </c>
       <c r="BF1" s="2">
@@ -34010,12 +34327,15 @@
       <c r="BG1" s="7">
         <v>43974.0</v>
       </c>
-      <c r="BH1" s="3">
+      <c r="BH1" s="2">
         <v>43975.0</v>
       </c>
-      <c r="BI1" s="2">
+      <c r="BI1" s="8">
+        <v>43976.0</v>
+      </c>
+      <c r="BJ1" s="2">
         <f>today()</f>
-        <v>43976</v>
+        <v>43977</v>
       </c>
     </row>
     <row r="2" ht="14.25" hidden="1" customHeight="1">
@@ -34178,6 +34498,7 @@
       <c r="BG2" s="4"/>
       <c r="BH2" s="4"/>
       <c r="BI2" s="4"/>
+      <c r="BJ2" s="4"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="1" t="s">
@@ -34360,7 +34681,10 @@
       <c r="BH3" s="4">
         <v>28.0</v>
       </c>
-      <c r="BI3" s="4"/>
+      <c r="BI3" s="4">
+        <v>28.0</v>
+      </c>
+      <c r="BJ3" s="4"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="1" t="s">
@@ -34543,7 +34867,10 @@
       <c r="BH4" s="4">
         <v>29.0</v>
       </c>
-      <c r="BI4" s="4"/>
+      <c r="BI4" s="4">
+        <v>29.0</v>
+      </c>
+      <c r="BJ4" s="4"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="1" t="s">
@@ -34726,7 +35053,10 @@
       <c r="BH5" s="4">
         <v>58.0</v>
       </c>
-      <c r="BI5" s="4"/>
+      <c r="BI5" s="4">
+        <v>61.0</v>
+      </c>
+      <c r="BJ5" s="4"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="1" t="s">
@@ -34909,7 +35239,10 @@
       <c r="BH6" s="4">
         <v>53.0</v>
       </c>
-      <c r="BI6" s="4"/>
+      <c r="BI6" s="4">
+        <v>55.0</v>
+      </c>
+      <c r="BJ6" s="4"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="1" t="s">
@@ -35092,7 +35425,10 @@
       <c r="BH7" s="4">
         <v>1335.0</v>
       </c>
-      <c r="BI7" s="4"/>
+      <c r="BI7" s="4">
+        <v>1335.0</v>
+      </c>
+      <c r="BJ7" s="4"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="1" t="s">
@@ -35275,7 +35611,10 @@
       <c r="BH8" s="4">
         <v>121.0</v>
       </c>
-      <c r="BI8" s="4"/>
+      <c r="BI8" s="4">
+        <v>121.0</v>
+      </c>
+      <c r="BJ8" s="4"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="1" t="s">
@@ -35458,7 +35797,10 @@
       <c r="BH9" s="4">
         <v>1111.0</v>
       </c>
-      <c r="BI9" s="4"/>
+      <c r="BI9" s="4">
+        <v>1168.0</v>
+      </c>
+      <c r="BJ9" s="4"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="1" t="s">
@@ -35641,7 +35983,10 @@
       <c r="BH10" s="4">
         <v>6525.0</v>
       </c>
-      <c r="BI10" s="4"/>
+      <c r="BI10" s="4">
+        <v>7221.0</v>
+      </c>
+      <c r="BJ10" s="4"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="1" t="s">
@@ -35824,7 +36169,10 @@
       <c r="BH11" s="4">
         <v>1840.0</v>
       </c>
-      <c r="BI11" s="4"/>
+      <c r="BI11" s="4">
+        <v>1899.0</v>
+      </c>
+      <c r="BJ11" s="4"/>
     </row>
     <row r="12" ht="14.25" customHeight="1"/>
     <row r="13" ht="14.25" customHeight="1"/>
@@ -36841,7 +37189,7 @@
     <col customWidth="1" min="7" max="15" width="7.13"/>
     <col customWidth="1" min="16" max="36" width="8.0"/>
     <col customWidth="1" min="37" max="43" width="7.63"/>
-    <col customWidth="1" min="44" max="61" width="9.88"/>
+    <col customWidth="1" min="44" max="62" width="9.88"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -37025,9 +37373,12 @@
       <c r="BH1" s="2">
         <v>43975.0</v>
       </c>
-      <c r="BI1" s="2">
+      <c r="BI1" s="3">
+        <v>43976.0</v>
+      </c>
+      <c r="BJ1" s="2">
         <f>today()</f>
-        <v>43976</v>
+        <v>43977</v>
       </c>
     </row>
     <row r="2" ht="14.25" hidden="1" customHeight="1">
@@ -37188,6 +37539,7 @@
       <c r="BG2" s="4"/>
       <c r="BH2" s="4"/>
       <c r="BI2" s="4"/>
+      <c r="BJ2" s="4"/>
     </row>
     <row r="3" ht="14.25" hidden="1" customHeight="1">
       <c r="A3" s="14" t="s">
@@ -37430,6 +37782,7 @@
         <v>974</v>
       </c>
       <c r="BI3" s="14"/>
+      <c r="BJ3" s="14"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="1" t="s">
@@ -37670,7 +38023,11 @@
         <f>(Recoveries!BH3-Recoveries!BG3)-(Deaths!BH3-Deaths!BG3)</f>
         <v>1</v>
       </c>
-      <c r="BI4" s="4"/>
+      <c r="BI4" s="1">
+        <f>(Recoveries!BI3-Recoveries!BH3)-(Deaths!BI3-Deaths!BH3)</f>
+        <v>0</v>
+      </c>
+      <c r="BJ4" s="4"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="1" t="s">
@@ -37911,7 +38268,11 @@
         <f>(Recoveries!BH4-Recoveries!BG4)-(Deaths!BH4-Deaths!BG4)</f>
         <v>0</v>
       </c>
-      <c r="BI5" s="4"/>
+      <c r="BI5" s="1">
+        <f>(Recoveries!BI4-Recoveries!BH4)-(Deaths!BI4-Deaths!BH4)</f>
+        <v>0</v>
+      </c>
+      <c r="BJ5" s="4"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="1" t="s">
@@ -38152,7 +38513,11 @@
         <f>(Recoveries!BH5-Recoveries!BG5)-(Deaths!BH5-Deaths!BG5)</f>
         <v>0</v>
       </c>
-      <c r="BI6" s="4"/>
+      <c r="BI6" s="1">
+        <f>(Recoveries!BI5-Recoveries!BH5)-(Deaths!BI5-Deaths!BH5)</f>
+        <v>3</v>
+      </c>
+      <c r="BJ6" s="4"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="1" t="s">
@@ -38393,7 +38758,11 @@
         <f>(Recoveries!BH6-Recoveries!BG6)-(Deaths!BH6-Deaths!BG6)</f>
         <v>2</v>
       </c>
-      <c r="BI7" s="4"/>
+      <c r="BI7" s="1">
+        <f>(Recoveries!BI6-Recoveries!BH6)-(Deaths!BI6-Deaths!BH6)</f>
+        <v>2</v>
+      </c>
+      <c r="BJ7" s="4"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="1" t="s">
@@ -38634,7 +39003,11 @@
         <f>(Recoveries!BH7-Recoveries!BG7)-(Deaths!BH7-Deaths!BG7)</f>
         <v>298</v>
       </c>
-      <c r="BI8" s="4"/>
+      <c r="BI8" s="1">
+        <f>(Recoveries!BI7-Recoveries!BH7)-(Deaths!BI7-Deaths!BH7)</f>
+        <v>-2</v>
+      </c>
+      <c r="BJ8" s="4"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="1" t="s">
@@ -38875,7 +39248,11 @@
         <f>(Recoveries!BH8-Recoveries!BG8)-(Deaths!BH8-Deaths!BG8)</f>
         <v>0</v>
       </c>
-      <c r="BI9" s="4"/>
+      <c r="BI9" s="1">
+        <f>(Recoveries!BI8-Recoveries!BH8)-(Deaths!BI8-Deaths!BH8)</f>
+        <v>0</v>
+      </c>
+      <c r="BJ9" s="4"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="1" t="s">
@@ -39116,7 +39493,11 @@
         <f>(Recoveries!BH9-Recoveries!BG9)-(Deaths!BH9-Deaths!BG9)</f>
         <v>230</v>
       </c>
-      <c r="BI10" s="4"/>
+      <c r="BI10" s="1">
+        <f>(Recoveries!BI9-Recoveries!BH9)-(Deaths!BI9-Deaths!BH9)</f>
+        <v>57</v>
+      </c>
+      <c r="BJ10" s="4"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="1" t="s">
@@ -39357,7 +39738,11 @@
         <f>(Recoveries!BH10-Recoveries!BG10)-(Deaths!BH10-Deaths!BG10)</f>
         <v>379</v>
       </c>
-      <c r="BI11" s="4"/>
+      <c r="BI11" s="1">
+        <f>(Recoveries!BI10-Recoveries!BH10)-(Deaths!BI10-Deaths!BH10)</f>
+        <v>647</v>
+      </c>
+      <c r="BJ11" s="4"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="1" t="s">
@@ -39598,7 +39983,11 @@
         <f>(Recoveries!BH11-Recoveries!BG11)-(Deaths!BH11-Deaths!BG11)</f>
         <v>64</v>
       </c>
-      <c r="BI12" s="4"/>
+      <c r="BI12" s="1">
+        <f>(Recoveries!BI11-Recoveries!BH11)-(Deaths!BI11-Deaths!BH11)</f>
+        <v>58</v>
+      </c>
+      <c r="BJ12" s="4"/>
     </row>
     <row r="13" ht="14.25" customHeight="1"/>
     <row r="14" ht="14.25" customHeight="1"/>
@@ -40614,7 +41003,7 @@
     <col customWidth="1" min="2" max="6" width="8.38"/>
     <col customWidth="1" min="7" max="15" width="7.13"/>
     <col customWidth="1" min="16" max="36" width="8.0"/>
-    <col customWidth="1" min="37" max="61" width="7.63"/>
+    <col customWidth="1" min="37" max="62" width="7.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -40792,15 +41181,18 @@
       <c r="BF1" s="2">
         <v>43973.0</v>
       </c>
-      <c r="BG1" s="3">
+      <c r="BG1" s="2">
         <v>43974.0</v>
       </c>
-      <c r="BH1" s="3">
+      <c r="BH1" s="2">
         <v>43975.0</v>
       </c>
-      <c r="BI1" s="2">
+      <c r="BI1" s="3">
+        <v>43976.0</v>
+      </c>
+      <c r="BJ1" s="2">
         <f>today()</f>
-        <v>43976</v>
+        <v>43977</v>
       </c>
     </row>
     <row r="2" ht="14.25" hidden="1" customHeight="1">
@@ -41004,8 +41396,9 @@
       <c r="BF2" s="1"/>
       <c r="BG2" s="1"/>
       <c r="BH2" s="1"/>
-      <c r="BI2" s="1">
-        <f>Confirmed!BI2-Deaths!AX2-Recoveries!AX2</f>
+      <c r="BI2" s="1"/>
+      <c r="BJ2" s="1">
+        <f>Confirmed!BJ2-Deaths!AX2-Recoveries!AX2</f>
         <v>0</v>
       </c>
     </row>
@@ -41014,7 +41407,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="15">
-        <f t="shared" ref="B3:BI3" si="1">sum(B4:B12)</f>
+        <f t="shared" ref="B3:BJ3" si="1">sum(B4:B12)</f>
         <v>848</v>
       </c>
       <c r="C3" s="15">
@@ -41250,6 +41643,10 @@
         <v>11054</v>
       </c>
       <c r="BI3" s="15">
+        <f t="shared" si="1"/>
+        <v>11217</v>
+      </c>
+      <c r="BJ3" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -41494,7 +41891,11 @@
         <f>Confirmed!BH3-Deaths!BH3-Recoveries!BH3</f>
         <v>11</v>
       </c>
-      <c r="BI4" s="1"/>
+      <c r="BI4" s="1">
+        <f>Confirmed!BI3-Deaths!BI3-Recoveries!BI3</f>
+        <v>16</v>
+      </c>
+      <c r="BJ4" s="1"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="1" t="s">
@@ -41736,7 +42137,11 @@
         <f>Confirmed!BH4-Deaths!BH4-Recoveries!BH4</f>
         <v>64</v>
       </c>
-      <c r="BI5" s="1"/>
+      <c r="BI5" s="1">
+        <f>Confirmed!BI4-Deaths!BI4-Recoveries!BI4</f>
+        <v>79</v>
+      </c>
+      <c r="BJ5" s="1"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="1" t="s">
@@ -41978,7 +42383,11 @@
         <f>Confirmed!BH5-Deaths!BH5-Recoveries!BH5</f>
         <v>43</v>
       </c>
-      <c r="BI6" s="1"/>
+      <c r="BI6" s="1">
+        <f>Confirmed!BI5-Deaths!BI5-Recoveries!BI5</f>
+        <v>41</v>
+      </c>
+      <c r="BJ6" s="1"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="1" t="s">
@@ -42220,7 +42629,11 @@
         <f>Confirmed!BH6-Deaths!BH6-Recoveries!BH6</f>
         <v>72</v>
       </c>
-      <c r="BI7" s="1"/>
+      <c r="BI7" s="1">
+        <f>Confirmed!BI6-Deaths!BI6-Recoveries!BI6</f>
+        <v>74</v>
+      </c>
+      <c r="BJ7" s="1"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="1" t="s">
@@ -42462,7 +42875,11 @@
         <f>Confirmed!BH7-Deaths!BH7-Recoveries!BH7</f>
         <v>1296</v>
       </c>
-      <c r="BI8" s="1"/>
+      <c r="BI8" s="1">
+        <f>Confirmed!BI7-Deaths!BI7-Recoveries!BI7</f>
+        <v>1352</v>
+      </c>
+      <c r="BJ8" s="1"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="1" t="s">
@@ -42704,7 +43121,11 @@
         <f>Confirmed!BH8-Deaths!BH8-Recoveries!BH8</f>
         <v>75</v>
       </c>
-      <c r="BI9" s="1"/>
+      <c r="BI9" s="1">
+        <f>Confirmed!BI8-Deaths!BI8-Recoveries!BI8</f>
+        <v>81</v>
+      </c>
+      <c r="BJ9" s="1"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="1" t="s">
@@ -42946,7 +43367,11 @@
         <f>Confirmed!BH9-Deaths!BH9-Recoveries!BH9</f>
         <v>655</v>
       </c>
-      <c r="BI10" s="1"/>
+      <c r="BI10" s="1">
+        <f>Confirmed!BI9-Deaths!BI9-Recoveries!BI9</f>
+        <v>665</v>
+      </c>
+      <c r="BJ10" s="1"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="1" t="s">
@@ -43188,7 +43613,11 @@
         <f>Confirmed!BH10-Deaths!BH10-Recoveries!BH10</f>
         <v>7934</v>
       </c>
-      <c r="BI11" s="1"/>
+      <c r="BI11" s="1">
+        <f>Confirmed!BI10-Deaths!BI10-Recoveries!BI10</f>
+        <v>7845</v>
+      </c>
+      <c r="BJ11" s="1"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="1" t="s">
@@ -43430,7 +43859,11 @@
         <f>Confirmed!BH11-Deaths!BH11-Recoveries!BH11</f>
         <v>904</v>
       </c>
-      <c r="BI12" s="1"/>
+      <c r="BI12" s="1">
+        <f>Confirmed!BI11-Deaths!BI11-Recoveries!BI11</f>
+        <v>1064</v>
+      </c>
+      <c r="BJ12" s="1"/>
     </row>
     <row r="13" ht="14.25" customHeight="1"/>
     <row r="14" ht="14.25" customHeight="1"/>
@@ -44891,7 +45324,7 @@
       <c r="AV2" s="1"/>
       <c r="AW2" s="1"/>
       <c r="AX2" s="1">
-        <f>Confirmed!BI2-Deaths!AX2-Recoveries!AX2</f>
+        <f>Confirmed!BJ2-Deaths!AX2-Recoveries!AX2</f>
         <v>0</v>
       </c>
       <c r="AY2" s="1"/>

</xml_diff>

<commit_message>
updated definitions of infection rate to positivity rate.
</commit_message>
<xml_diff>
--- a/Data/Covid2019/SA_data_archive/Province_database.xlsx
+++ b/Data/Covid2019/SA_data_archive/Province_database.xlsx
@@ -15,7 +15,7 @@
     <sheet state="visible" name="Closed" sheetId="10" r:id="rId13"/>
     <sheet state="visible" name="Recovery Rate" sheetId="11" r:id="rId14"/>
     <sheet state="visible" name="Death Rate" sheetId="12" r:id="rId15"/>
-    <sheet state="visible" name="Infection Rate" sheetId="13" r:id="rId16"/>
+    <sheet state="visible" name="Positivity Rate" sheetId="13" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -818,11 +818,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1066188317"/>
-        <c:axId val="1276226511"/>
+        <c:axId val="623804385"/>
+        <c:axId val="766335223"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1066188317"/>
+        <c:axId val="623804385"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -850,6 +850,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:spPr/>
@@ -867,10 +868,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1276226511"/>
+        <c:crossAx val="766335223"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1276226511"/>
+        <c:axId val="766335223"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -939,7 +940,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1066188317"/>
+        <c:crossAx val="623804385"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1200,11 +1201,11 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="1406877495"/>
-        <c:axId val="1267460300"/>
+        <c:axId val="983174185"/>
+        <c:axId val="1351377379"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1406877495"/>
+        <c:axId val="983174185"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1232,6 +1233,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:spPr/>
@@ -1249,10 +1251,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1267460300"/>
+        <c:crossAx val="1351377379"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1267460300"/>
+        <c:axId val="1351377379"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1321,7 +1323,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1406877495"/>
+        <c:crossAx val="983174185"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1365,7 +1367,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t>Infection Rate (National is the average based on provincial population - Stats Sa 2019)</a:t>
+              <a:t>Positivity Rate (National is the average based on provincial population - Stats Sa 2019)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1382,7 +1384,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Infection Rate'!$A$2</c:f>
+              <c:f>'Positivity Rate'!$A$2</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -1392,18 +1394,18 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>'Infection Rate'!$B$1:$CB$1</c:f>
+              <c:f>'Positivity Rate'!$B$1:$CB$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Infection Rate'!$B$2:$CB$2</c:f>
+              <c:f>'Positivity Rate'!$B$2:$CB$2</c:f>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="276209895"/>
-        <c:axId val="1901420795"/>
+        <c:axId val="2098011608"/>
+        <c:axId val="162245870"/>
       </c:barChart>
       <c:lineChart>
         <c:ser>
@@ -1411,7 +1413,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Infection Rate'!$A$3</c:f>
+              <c:f>'Positivity Rate'!$A$3</c:f>
             </c:strRef>
           </c:tx>
           <c:marker>
@@ -1419,12 +1421,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Infection Rate'!$B$1:$CB$1</c:f>
+              <c:f>'Positivity Rate'!$B$1:$CB$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Infection Rate'!$B$3:$CB$3</c:f>
+              <c:f>'Positivity Rate'!$B$3:$CB$3</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1434,7 +1436,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Infection Rate'!$A$4</c:f>
+              <c:f>'Positivity Rate'!$A$4</c:f>
             </c:strRef>
           </c:tx>
           <c:marker>
@@ -1442,12 +1444,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Infection Rate'!$B$1:$CB$1</c:f>
+              <c:f>'Positivity Rate'!$B$1:$CB$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Infection Rate'!$B$4:$CB$4</c:f>
+              <c:f>'Positivity Rate'!$B$4:$CB$4</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1457,7 +1459,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Infection Rate'!$A$5</c:f>
+              <c:f>'Positivity Rate'!$A$5</c:f>
             </c:strRef>
           </c:tx>
           <c:marker>
@@ -1465,12 +1467,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Infection Rate'!$B$1:$CB$1</c:f>
+              <c:f>'Positivity Rate'!$B$1:$CB$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Infection Rate'!$B$5:$CB$5</c:f>
+              <c:f>'Positivity Rate'!$B$5:$CB$5</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1480,7 +1482,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Infection Rate'!$A$6</c:f>
+              <c:f>'Positivity Rate'!$A$6</c:f>
             </c:strRef>
           </c:tx>
           <c:marker>
@@ -1488,12 +1490,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Infection Rate'!$B$1:$CB$1</c:f>
+              <c:f>'Positivity Rate'!$B$1:$CB$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Infection Rate'!$B$6:$CB$6</c:f>
+              <c:f>'Positivity Rate'!$B$6:$CB$6</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1503,7 +1505,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Infection Rate'!$A$7</c:f>
+              <c:f>'Positivity Rate'!$A$7</c:f>
             </c:strRef>
           </c:tx>
           <c:marker>
@@ -1511,12 +1513,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Infection Rate'!$B$1:$CB$1</c:f>
+              <c:f>'Positivity Rate'!$B$1:$CB$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Infection Rate'!$B$7:$CB$7</c:f>
+              <c:f>'Positivity Rate'!$B$7:$CB$7</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1526,7 +1528,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Infection Rate'!$A$8</c:f>
+              <c:f>'Positivity Rate'!$A$8</c:f>
             </c:strRef>
           </c:tx>
           <c:marker>
@@ -1534,12 +1536,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Infection Rate'!$B$1:$CB$1</c:f>
+              <c:f>'Positivity Rate'!$B$1:$CB$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Infection Rate'!$B$8:$CB$8</c:f>
+              <c:f>'Positivity Rate'!$B$8:$CB$8</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1549,7 +1551,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Infection Rate'!$A$9</c:f>
+              <c:f>'Positivity Rate'!$A$9</c:f>
             </c:strRef>
           </c:tx>
           <c:marker>
@@ -1557,12 +1559,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Infection Rate'!$B$1:$CB$1</c:f>
+              <c:f>'Positivity Rate'!$B$1:$CB$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Infection Rate'!$B$9:$CB$9</c:f>
+              <c:f>'Positivity Rate'!$B$9:$CB$9</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1572,7 +1574,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Infection Rate'!$A$10</c:f>
+              <c:f>'Positivity Rate'!$A$10</c:f>
             </c:strRef>
           </c:tx>
           <c:marker>
@@ -1580,12 +1582,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Infection Rate'!$B$1:$CB$1</c:f>
+              <c:f>'Positivity Rate'!$B$1:$CB$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Infection Rate'!$B$10:$CB$10</c:f>
+              <c:f>'Positivity Rate'!$B$10:$CB$10</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1595,7 +1597,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Infection Rate'!$A$11</c:f>
+              <c:f>'Positivity Rate'!$A$11</c:f>
             </c:strRef>
           </c:tx>
           <c:marker>
@@ -1603,21 +1605,21 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Infection Rate'!$B$1:$CB$1</c:f>
+              <c:f>'Positivity Rate'!$B$1:$CB$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Infection Rate'!$B$11:$CB$11</c:f>
+              <c:f>'Positivity Rate'!$B$11:$CB$11</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="276209895"/>
-        <c:axId val="1901420795"/>
+        <c:axId val="2098011608"/>
+        <c:axId val="162245870"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="276209895"/>
+        <c:axId val="2098011608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1645,6 +1647,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:spPr/>
@@ -1662,10 +1665,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1901420795"/>
+        <c:crossAx val="162245870"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1901420795"/>
+        <c:axId val="162245870"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1734,7 +1737,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276209895"/>
+        <c:crossAx val="2098011608"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2032,11 +2035,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="776312066"/>
-        <c:axId val="229110155"/>
+        <c:axId val="2009817716"/>
+        <c:axId val="1677602718"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="776312066"/>
+        <c:axId val="2009817716"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2064,6 +2067,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:spPr/>
@@ -2081,10 +2085,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229110155"/>
+        <c:crossAx val="1677602718"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="229110155"/>
+        <c:axId val="1677602718"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2153,7 +2157,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="776312066"/>
+        <c:crossAx val="2009817716"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2470,11 +2474,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="886010224"/>
-        <c:axId val="534555831"/>
+        <c:axId val="1558855073"/>
+        <c:axId val="825106918"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="886010224"/>
+        <c:axId val="1558855073"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2502,6 +2506,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:spPr/>
@@ -2519,10 +2524,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="534555831"/>
+        <c:crossAx val="825106918"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="534555831"/>
+        <c:axId val="825106918"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2591,7 +2596,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="886010224"/>
+        <c:crossAx val="1558855073"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2672,8 +2677,8 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1498251758"/>
-        <c:axId val="382784017"/>
+        <c:axId val="549202746"/>
+        <c:axId val="1926553242"/>
       </c:barChart>
       <c:lineChart>
         <c:ser>
@@ -2883,11 +2888,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1498251758"/>
-        <c:axId val="382784017"/>
+        <c:axId val="549202746"/>
+        <c:axId val="1926553242"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1498251758"/>
+        <c:axId val="549202746"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2915,6 +2920,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:spPr/>
@@ -2932,10 +2938,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="382784017"/>
+        <c:crossAx val="1926553242"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="382784017"/>
+        <c:axId val="1926553242"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3004,7 +3010,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1498251758"/>
+        <c:crossAx val="549202746"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3085,8 +3091,8 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="2010240791"/>
-        <c:axId val="1985609309"/>
+        <c:axId val="983099281"/>
+        <c:axId val="1034919517"/>
       </c:barChart>
       <c:lineChart>
         <c:ser>
@@ -3296,11 +3302,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2010240791"/>
-        <c:axId val="1985609309"/>
+        <c:axId val="983099281"/>
+        <c:axId val="1034919517"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2010240791"/>
+        <c:axId val="983099281"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3328,6 +3334,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:spPr/>
@@ -3345,10 +3352,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1985609309"/>
+        <c:crossAx val="1034919517"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1985609309"/>
+        <c:axId val="1034919517"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3417,7 +3424,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2010240791"/>
+        <c:crossAx val="983099281"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3506,8 +3513,8 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1676428533"/>
-        <c:axId val="1503626248"/>
+        <c:axId val="1733491944"/>
+        <c:axId val="525109247"/>
       </c:barChart>
       <c:lineChart>
         <c:ser>
@@ -3717,11 +3724,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1676428533"/>
-        <c:axId val="1503626248"/>
+        <c:axId val="1733491944"/>
+        <c:axId val="525109247"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1676428533"/>
+        <c:axId val="1733491944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3749,6 +3756,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:spPr/>
@@ -3766,10 +3774,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1503626248"/>
+        <c:crossAx val="525109247"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1503626248"/>
+        <c:axId val="525109247"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3838,7 +3846,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1676428533"/>
+        <c:crossAx val="1733491944"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3907,6 +3915,7 @@
             </a:solidFill>
           </c:spPr>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -3961,6 +3970,7 @@
             </a:solidFill>
           </c:spPr>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -3988,11 +3998,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1685292552"/>
-        <c:axId val="951809983"/>
+        <c:axId val="1007624151"/>
+        <c:axId val="310143606"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1685292552"/>
+        <c:axId val="1007624151"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4020,6 +4030,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:spPr/>
@@ -4037,10 +4048,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="951809983"/>
+        <c:crossAx val="310143606"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="951809983"/>
+        <c:axId val="310143606"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4109,7 +4120,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1685292552"/>
+        <c:crossAx val="1007624151"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4178,6 +4189,7 @@
             </a:solidFill>
           </c:spPr>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -4219,6 +4231,7 @@
             </a:solidFill>
           </c:spPr>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -4260,6 +4273,7 @@
             </a:solidFill>
           </c:spPr>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -4301,6 +4315,7 @@
             </a:solidFill>
           </c:spPr>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -4328,11 +4343,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1122316642"/>
-        <c:axId val="1174292035"/>
+        <c:axId val="1898074433"/>
+        <c:axId val="1685616125"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1122316642"/>
+        <c:axId val="1898074433"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4360,6 +4375,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:spPr/>
@@ -4377,10 +4393,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1174292035"/>
+        <c:crossAx val="1685616125"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1174292035"/>
+        <c:axId val="1685616125"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4449,7 +4465,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1122316642"/>
+        <c:crossAx val="1898074433"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4710,11 +4726,11 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="866222389"/>
-        <c:axId val="1174278739"/>
+        <c:axId val="1129433965"/>
+        <c:axId val="2016187129"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="866222389"/>
+        <c:axId val="1129433965"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4742,6 +4758,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:spPr/>
@@ -4759,10 +4776,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1174278739"/>
+        <c:crossAx val="2016187129"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1174278739"/>
+        <c:axId val="2016187129"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4831,7 +4848,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="866222389"/>
+        <c:crossAx val="1129433965"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -5125,7 +5142,7 @@
     <xdr:ext cx="4229100" cy="5829300"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 7" title="Chart"/>
+        <xdr:cNvPr id="6" name="Chart 6" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5155,7 +5172,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 6" title="Chart"/>
+        <xdr:cNvPr id="7" name="Chart 7" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5662,7 +5679,7 @@
       </c>
       <c r="CB1" s="2">
         <f>today()</f>
-        <v>43995</v>
+        <v>43998</v>
       </c>
     </row>
     <row r="2" ht="14.25" hidden="1" customHeight="1">
@@ -13249,7 +13266,7 @@
       </c>
       <c r="CB1" s="2">
         <f>today()</f>
-        <v>43995</v>
+        <v>43998</v>
       </c>
     </row>
     <row r="2" ht="14.25" hidden="1" customHeight="1">
@@ -17607,7 +17624,7 @@
       </c>
       <c r="CB1" s="2">
         <f>today()</f>
-        <v>43995</v>
+        <v>43998</v>
       </c>
     </row>
     <row r="2" ht="14.25" hidden="1" customHeight="1">
@@ -21955,7 +21972,7 @@
       </c>
       <c r="CB1" s="2">
         <f>today()</f>
-        <v>43995</v>
+        <v>43998</v>
       </c>
     </row>
     <row r="2" ht="14.25" hidden="1" customHeight="1">
@@ -26303,7 +26320,7 @@
       </c>
       <c r="CB1" s="2">
         <f>today()</f>
-        <v>43995</v>
+        <v>43998</v>
       </c>
     </row>
     <row r="2" ht="14.25" hidden="1" customHeight="1">
@@ -31033,7 +31050,7 @@
       </c>
       <c r="CB1" s="2">
         <f>today()</f>
-        <v>43995</v>
+        <v>43998</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
@@ -36120,7 +36137,7 @@
       </c>
       <c r="CB1" s="2">
         <f>TODAY()</f>
-        <v>43995</v>
+        <v>43998</v>
       </c>
     </row>
     <row r="2" ht="14.25" hidden="1" customHeight="1">
@@ -40542,7 +40559,7 @@
       </c>
       <c r="CB1" s="2">
         <f>today()</f>
-        <v>43995</v>
+        <v>43998</v>
       </c>
     </row>
     <row r="2" ht="14.25" hidden="1" customHeight="1">
@@ -44153,7 +44170,7 @@
       </c>
       <c r="CB1" s="2">
         <f>today()</f>
-        <v>43995</v>
+        <v>43998</v>
       </c>
     </row>
     <row r="2" ht="14.25" hidden="1" customHeight="1">
@@ -47764,7 +47781,7 @@
       </c>
       <c r="CB1" s="2">
         <f>today()</f>
-        <v>43995</v>
+        <v>43998</v>
       </c>
     </row>
     <row r="2" ht="14.25" hidden="1" customHeight="1">
@@ -52221,7 +52238,7 @@
       </c>
       <c r="CB1" s="2">
         <f>today()</f>
-        <v>43995</v>
+        <v>43998</v>
       </c>
     </row>
     <row r="2" ht="14.25" hidden="1" customHeight="1">

</xml_diff>